<commit_message>
plots and metrics fixes
</commit_message>
<xml_diff>
--- a/training/results/results_test.xlsx
+++ b/training/results/results_test.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y22"/>
+  <dimension ref="A1:BM22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,55 +474,95 @@
       </c>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>round 0.5</t>
-        </is>
-      </c>
+      <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
       <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>best_single_threshold_0.05_0.95</t>
-        </is>
-      </c>
+      <c r="H1" s="1" t="n"/>
       <c r="I1" s="1" t="n"/>
-      <c r="J1" s="1" t="n"/>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>best_multiple_thresholds_0.05_0.95</t>
-        </is>
-      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>round 0.5</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="n"/>
       <c r="L1" s="1" t="n"/>
       <c r="M1" s="1" t="n"/>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>best_graph_thresholds_0.05_0.95</t>
-        </is>
-      </c>
+      <c r="N1" s="1" t="n"/>
       <c r="O1" s="1" t="n"/>
       <c r="P1" s="1" t="n"/>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>best_single_threshold_0.25_0.75</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="n"/>
+      <c r="Q1" s="1" t="n"/>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>best_single_threshold_0.05_0.95</t>
+        </is>
+      </c>
       <c r="S1" s="1" t="n"/>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>best_multiple_thresholds_0.25_0.75</t>
-        </is>
-      </c>
+      <c r="T1" s="1" t="n"/>
       <c r="U1" s="1" t="n"/>
       <c r="V1" s="1" t="n"/>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>best_graph_thresholds_0.25_0.75</t>
-        </is>
-      </c>
+      <c r="W1" s="1" t="n"/>
       <c r="X1" s="1" t="n"/>
       <c r="Y1" s="1" t="n"/>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>best_multiple_thresholds_0.05_0.95</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="n"/>
+      <c r="AB1" s="1" t="n"/>
+      <c r="AC1" s="1" t="n"/>
+      <c r="AD1" s="1" t="n"/>
+      <c r="AE1" s="1" t="n"/>
+      <c r="AF1" s="1" t="n"/>
+      <c r="AG1" s="1" t="n"/>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>best_graph_thresholds_0.05_0.95</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="n"/>
+      <c r="AJ1" s="1" t="n"/>
+      <c r="AK1" s="1" t="n"/>
+      <c r="AL1" s="1" t="n"/>
+      <c r="AM1" s="1" t="n"/>
+      <c r="AN1" s="1" t="n"/>
+      <c r="AO1" s="1" t="n"/>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>best_single_threshold_0.25_0.75</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="n"/>
+      <c r="AR1" s="1" t="n"/>
+      <c r="AS1" s="1" t="n"/>
+      <c r="AT1" s="1" t="n"/>
+      <c r="AU1" s="1" t="n"/>
+      <c r="AV1" s="1" t="n"/>
+      <c r="AW1" s="1" t="n"/>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>best_multiple_thresholds_0.25_0.75</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="n"/>
+      <c r="AZ1" s="1" t="n"/>
+      <c r="BA1" s="1" t="n"/>
+      <c r="BB1" s="1" t="n"/>
+      <c r="BC1" s="1" t="n"/>
+      <c r="BD1" s="1" t="n"/>
+      <c r="BE1" s="1" t="n"/>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>best_graph_thresholds_0.25_0.75</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="n"/>
+      <c r="BH1" s="1" t="n"/>
+      <c r="BI1" s="1" t="n"/>
+      <c r="BJ1" s="1" t="n"/>
+      <c r="BK1" s="1" t="n"/>
+      <c r="BL1" s="1" t="n"/>
+      <c r="BM1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -537,117 +577,317 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="D2" s="1" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
         <is>
           <t>rmse</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="N2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="O2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="H2" s="1" t="inlineStr">
+      <c r="Q2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
+        </is>
+      </c>
+      <c r="R2" s="1" t="inlineStr">
         <is>
           <t>rmse</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="S2" s="1" t="inlineStr">
+        <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="T2" s="1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="U2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="V2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="W2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="X2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="Y2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
+        </is>
+      </c>
+      <c r="Z2" s="1" t="inlineStr">
         <is>
           <t>rmse</t>
         </is>
       </c>
-      <c r="L2" s="1" t="inlineStr">
+      <c r="AA2" s="1" t="inlineStr">
+        <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AB2" s="1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="M2" s="1" t="inlineStr">
+      <c r="AC2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AD2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AE2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="AF2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="N2" s="1" t="inlineStr">
+      <c r="AG2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
+        </is>
+      </c>
+      <c r="AH2" s="1" t="inlineStr">
         <is>
           <t>rmse</t>
         </is>
       </c>
-      <c r="O2" s="1" t="inlineStr">
+      <c r="AI2" s="1" t="inlineStr">
+        <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AJ2" s="1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="P2" s="1" t="inlineStr">
+      <c r="AK2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AL2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AM2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="AN2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="Q2" s="1" t="inlineStr">
+      <c r="AO2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
+        </is>
+      </c>
+      <c r="AP2" s="1" t="inlineStr">
         <is>
           <t>rmse</t>
         </is>
       </c>
-      <c r="R2" s="1" t="inlineStr">
+      <c r="AQ2" s="1" t="inlineStr">
+        <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AR2" s="1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="S2" s="1" t="inlineStr">
+      <c r="AS2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AT2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AU2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="AV2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="T2" s="1" t="inlineStr">
+      <c r="AW2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
+        </is>
+      </c>
+      <c r="AX2" s="1" t="inlineStr">
         <is>
           <t>rmse</t>
         </is>
       </c>
-      <c r="U2" s="1" t="inlineStr">
+      <c r="AY2" s="1" t="inlineStr">
+        <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AZ2" s="1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="V2" s="1" t="inlineStr">
+      <c r="BA2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="BB2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="BC2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="BD2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="W2" s="1" t="inlineStr">
+      <c r="BE2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
+        </is>
+      </c>
+      <c r="BF2" s="1" t="inlineStr">
         <is>
           <t>rmse</t>
         </is>
       </c>
-      <c r="X2" s="1" t="inlineStr">
+      <c r="BG2" s="1" t="inlineStr">
+        <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="BH2" s="1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="Y2" s="1" t="inlineStr">
+      <c r="BI2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="BJ2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="BK2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="BL2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
+        </is>
+      </c>
+      <c r="BM2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
         </is>
       </c>
     </row>
@@ -661,71 +901,189 @@
         <v>0.6091792271036202</v>
       </c>
       <c r="C4" t="n">
+        <v>0.6180943735427414</v>
+      </c>
+      <c r="D4" t="n">
         <v>0.4525010110345065</v>
       </c>
-      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
+        <v>0.4229372878062176</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.382040654605194</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9589937897963997</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="n">
         <v>0.6398964413257052</v>
       </c>
-      <c r="F4" t="n">
+      <c r="K4" t="n">
+        <v>0.6897246274071355</v>
+      </c>
+      <c r="L4" t="n">
         <v>0.3668639053254438</v>
       </c>
-      <c r="G4" t="n">
+      <c r="M4" t="n">
+        <v>0.4112758128214844</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.4757200616519119</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.9324204072006917</v>
+      </c>
+      <c r="P4" t="n">
         <v>0.6520710059171597</v>
       </c>
-      <c r="H4" t="n">
+      <c r="Q4" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="R4" t="n">
         <v>0.6305815855975138</v>
       </c>
-      <c r="I4" t="n">
+      <c r="S4" t="n">
+        <v>0.6980139893804611</v>
+      </c>
+      <c r="T4" t="n">
         <v>0.3526627218934911</v>
       </c>
-      <c r="J4" t="n">
+      <c r="U4" t="n">
+        <v>0.4218919690940813</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.4872235293708265</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.9350522757644839</v>
+      </c>
+      <c r="X4" t="n">
         <v>0.6674556213017752</v>
       </c>
-      <c r="K4" t="n">
+      <c r="Y4" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="Z4" t="n">
         <v>0.6211270534826568</v>
       </c>
-      <c r="L4" t="n">
+      <c r="AA4" t="n">
+        <v>0.6846156109421431</v>
+      </c>
+      <c r="AB4" t="n">
         <v>0.3455621301775148</v>
       </c>
-      <c r="M4" t="n">
+      <c r="AC4" t="n">
+        <v>0.4034110711589981</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.4686985347456838</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0.9374891911013286</v>
+      </c>
+      <c r="AF4" t="n">
         <v>0.672189349112426</v>
       </c>
-      <c r="N4" t="n">
+      <c r="AG4" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="AH4" t="n">
         <v>0.6285043968726759</v>
       </c>
-      <c r="O4" t="n">
+      <c r="AI4" t="n">
+        <v>0.6555004004061831</v>
+      </c>
+      <c r="AJ4" t="n">
         <v>0.3459519297887649</v>
       </c>
-      <c r="P4" t="n">
+      <c r="AK4" t="n">
+        <v>0.3655255744097044</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>0.4296807749326664</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0.9368131436207845</v>
+      </c>
+      <c r="AN4" t="n">
         <v>0.676923076923077</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="AO4" t="n">
+        <v>0.9798816568047337</v>
+      </c>
+      <c r="AP4" t="n">
         <v>0.6305815855975138</v>
       </c>
-      <c r="R4" t="n">
+      <c r="AQ4" t="n">
+        <v>0.6980139893804611</v>
+      </c>
+      <c r="AR4" t="n">
         <v>0.3526627218934911</v>
       </c>
-      <c r="S4" t="n">
+      <c r="AS4" t="n">
+        <v>0.4218919690940813</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>0.4872235293708265</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>0.9350522757644839</v>
+      </c>
+      <c r="AV4" t="n">
         <v>0.6674556213017752</v>
       </c>
-      <c r="T4" t="n">
+      <c r="AW4" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="AX4" t="n">
         <v>0.6249260311258431</v>
       </c>
-      <c r="U4" t="n">
+      <c r="AY4" t="n">
+        <v>0.7074948935350311</v>
+      </c>
+      <c r="AZ4" t="n">
         <v>0.3408284023668639</v>
       </c>
-      <c r="V4" t="n">
+      <c r="BA4" t="n">
+        <v>0.4071799281383982</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>0.5005490243781451</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>0.937269082619291</v>
+      </c>
+      <c r="BD4" t="n">
         <v>0.6804733727810651</v>
       </c>
-      <c r="W4" t="n">
+      <c r="BE4" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="BF4" t="n">
         <v>0.6180615061698925</v>
       </c>
-      <c r="X4" t="n">
+      <c r="BG4" t="n">
+        <v>0.6549281273710738</v>
+      </c>
+      <c r="BH4" t="n">
         <v>0.3400347700254513</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="BI4" t="n">
+        <v>0.3664701543441086</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>0.4289308520217814</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>0.93805832874774</v>
+      </c>
+      <c r="BL4" t="n">
         <v>0.6792899408284023</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>0.9834319526627219</v>
       </c>
     </row>
     <row r="5">
@@ -738,71 +1096,189 @@
         <v>0.6066834765467946</v>
       </c>
       <c r="C5" t="n">
+        <v>0.6152599750840554</v>
+      </c>
+      <c r="D5" t="n">
         <v>0.4506175590769879</v>
       </c>
-      <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
+        <v>0.4221831108424272</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.3785448369404324</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.9593962738778398</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="n">
         <v>0.633390426161197</v>
       </c>
-      <c r="F5" t="n">
+      <c r="K5" t="n">
+        <v>0.6873351266204395</v>
+      </c>
+      <c r="L5" t="n">
         <v>0.3538461538461539</v>
       </c>
-      <c r="G5" t="n">
+      <c r="M5" t="n">
+        <v>0.406594023108082</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.4724295762863355</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.9349233550821476</v>
+      </c>
+      <c r="P5" t="n">
         <v>0.6662721893491125</v>
       </c>
-      <c r="H5" t="n">
+      <c r="Q5" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="R5" t="n">
         <v>0.633390426161197</v>
       </c>
-      <c r="I5" t="n">
+      <c r="S5" t="n">
+        <v>0.6873351266204395</v>
+      </c>
+      <c r="T5" t="n">
         <v>0.3538461538461539</v>
       </c>
-      <c r="J5" t="n">
+      <c r="U5" t="n">
+        <v>0.406594023108082</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.4724295762863355</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.9349233550821476</v>
+      </c>
+      <c r="X5" t="n">
         <v>0.6662721893491125</v>
       </c>
-      <c r="K5" t="n">
+      <c r="Y5" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="Z5" t="n">
         <v>0.6296425209132654</v>
       </c>
-      <c r="L5" t="n">
+      <c r="AA5" t="n">
+        <v>0.6820468087494997</v>
+      </c>
+      <c r="AB5" t="n">
         <v>0.3467455621301775</v>
       </c>
-      <c r="M5" t="n">
+      <c r="AC5" t="n">
+        <v>0.4310293147806636</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0.4651878493253767</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0.9356905903623929</v>
+      </c>
+      <c r="AF5" t="n">
         <v>0.6745562130177515</v>
       </c>
-      <c r="N5" t="n">
+      <c r="AG5" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="AH5" t="n">
         <v>0.609428793653878</v>
       </c>
-      <c r="O5" t="n">
+      <c r="AI5" t="n">
+        <v>0.6378425507108177</v>
+      </c>
+      <c r="AJ5" t="n">
         <v>0.3245061253572235</v>
       </c>
-      <c r="P5" t="n">
+      <c r="AK5" t="n">
+        <v>0.3441856572589514</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>0.4068431194972821</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>0.9393003694678091</v>
+      </c>
+      <c r="AN5" t="n">
         <v>0.6970414201183432</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="AO5" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="AP5" t="n">
         <v>0.633390426161197</v>
       </c>
-      <c r="R5" t="n">
+      <c r="AQ5" t="n">
+        <v>0.6873351266204395</v>
+      </c>
+      <c r="AR5" t="n">
         <v>0.3538461538461539</v>
       </c>
-      <c r="S5" t="n">
+      <c r="AS5" t="n">
+        <v>0.406594023108082</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0.4724295762863355</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.9349233550821476</v>
+      </c>
+      <c r="AV5" t="n">
         <v>0.6662721893491125</v>
       </c>
-      <c r="T5" t="n">
+      <c r="AW5" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="AX5" t="n">
         <v>0.6124932073044426</v>
       </c>
-      <c r="U5" t="n">
+      <c r="AY5" t="n">
+        <v>0.7074082302333098</v>
+      </c>
+      <c r="AZ5" t="n">
         <v>0.3325443786982248</v>
       </c>
-      <c r="V5" t="n">
+      <c r="BA5" t="n">
+        <v>0.4051866051659079</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>0.5004264042018234</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>0.9362943164845531</v>
+      </c>
+      <c r="BD5" t="n">
         <v>0.6863905325443787</v>
       </c>
-      <c r="W5" t="n">
+      <c r="BE5" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="BF5" t="n">
         <v>0.607483819232328</v>
       </c>
-      <c r="X5" t="n">
+      <c r="BG5" t="n">
+        <v>0.6378968439854098</v>
+      </c>
+      <c r="BH5" t="n">
         <v>0.3292398531678744</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="BI5" t="n">
+        <v>0.3463418778499546</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>0.4069123835665462</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>0.9393695464193067</v>
+      </c>
+      <c r="BL5" t="n">
         <v>0.6887573964497041</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>0.9846153846153847</v>
       </c>
     </row>
     <row r="6">
@@ -815,71 +1291,189 @@
         <v>0.6085150377211097</v>
       </c>
       <c r="C6" t="n">
+        <v>0.6204683456581611</v>
+      </c>
+      <c r="D6" t="n">
         <v>0.4502765917298872</v>
       </c>
-      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
+        <v>0.4199647361246967</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.3849809679637752</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.9591981762440059</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="n">
         <v>0.6324555320336759</v>
       </c>
-      <c r="F6" t="n">
+      <c r="K6" t="n">
+        <v>0.6835764481668571</v>
+      </c>
+      <c r="L6" t="n">
         <v>0.3502958579881657</v>
       </c>
-      <c r="G6" t="n">
+      <c r="M6" t="n">
+        <v>0.3960064247014668</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.467276760488416</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.9345554594764562</v>
+      </c>
+      <c r="P6" t="n">
         <v>0.6710059171597633</v>
       </c>
-      <c r="H6" t="n">
+      <c r="Q6" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="R6" t="n">
         <v>0.6324555320336759</v>
       </c>
-      <c r="I6" t="n">
+      <c r="S6" t="n">
+        <v>0.6835764481668571</v>
+      </c>
+      <c r="T6" t="n">
         <v>0.3502958579881657</v>
       </c>
-      <c r="J6" t="n">
+      <c r="U6" t="n">
+        <v>0.3960064247014668</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.467276760488416</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.9345554594764562</v>
+      </c>
+      <c r="X6" t="n">
         <v>0.6710059171597633</v>
       </c>
-      <c r="K6" t="n">
+      <c r="Y6" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="Z6" t="n">
         <v>0.6590292304801199</v>
       </c>
-      <c r="L6" t="n">
+      <c r="AA6" t="n">
+        <v>0.6994182038983934</v>
+      </c>
+      <c r="AB6" t="n">
         <v>0.3775147928994083</v>
       </c>
-      <c r="M6" t="n">
+      <c r="AC6" t="n">
+        <v>0.4158129855424297</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0.4891858239444546</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0.9273987894033487</v>
+      </c>
+      <c r="AF6" t="n">
         <v>0.6473372781065089</v>
       </c>
-      <c r="N6" t="n">
+      <c r="AG6" t="n">
+        <v>0.978698224852071</v>
+      </c>
+      <c r="AH6" t="n">
         <v>0.6250427483072962</v>
       </c>
-      <c r="O6" t="n">
+      <c r="AI6" t="n">
+        <v>0.6355583406062126</v>
+      </c>
+      <c r="AJ6" t="n">
         <v>0.3341675035415116</v>
       </c>
-      <c r="P6" t="n">
+      <c r="AK6" t="n">
+        <v>0.3359340598600982</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0.4039344043141225</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.9370080968477321</v>
+      </c>
+      <c r="AN6" t="n">
         <v>0.6923076923076923</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="AO6" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="AP6" t="n">
         <v>0.6324555320336759</v>
       </c>
-      <c r="R6" t="n">
+      <c r="AQ6" t="n">
+        <v>0.6835764481668571</v>
+      </c>
+      <c r="AR6" t="n">
         <v>0.3502958579881657</v>
       </c>
-      <c r="S6" t="n">
+      <c r="AS6" t="n">
+        <v>0.3960064247014668</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.467276760488416</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.9345554594764562</v>
+      </c>
+      <c r="AV6" t="n">
         <v>0.6710059171597633</v>
       </c>
-      <c r="T6" t="n">
+      <c r="AW6" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="AX6" t="n">
         <v>0.6305815855975138</v>
       </c>
-      <c r="U6" t="n">
+      <c r="AY6" t="n">
+        <v>0.703959013536917</v>
+      </c>
+      <c r="AZ6" t="n">
         <v>0.3479289940828402</v>
       </c>
-      <c r="V6" t="n">
+      <c r="BA6" t="n">
+        <v>0.4014632144076808</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>0.4955582927398693</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>0.9367030893797658</v>
+      </c>
+      <c r="BD6" t="n">
         <v>0.6733727810650888</v>
       </c>
-      <c r="W6" t="n">
+      <c r="BE6" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="BF6" t="n">
         <v>0.6231465103057326</v>
       </c>
-      <c r="X6" t="n">
+      <c r="BG6" t="n">
+        <v>0.636966432138438</v>
+      </c>
+      <c r="BH6" t="n">
         <v>0.3389012313521625</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="BI6" t="n">
+        <v>0.3398128477388861</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>0.4057262356711713</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>0.9367502554830595</v>
+      </c>
+      <c r="BL6" t="n">
         <v>0.6840236686390533</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>0.9798816568047337</v>
       </c>
     </row>
     <row r="7">
@@ -892,71 +1486,189 @@
         <v>0.6274585880517152</v>
       </c>
       <c r="C7" t="n">
+        <v>0.6547800997752682</v>
+      </c>
+      <c r="D7" t="n">
         <v>0.4616095074713775</v>
       </c>
-      <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
+        <v>0.43442282076456</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.4287369790617102</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.9546922411760081</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="n">
         <v>0.6545245349594661</v>
       </c>
-      <c r="F7" t="n">
+      <c r="K7" t="n">
+        <v>0.6794828877072008</v>
+      </c>
+      <c r="L7" t="n">
         <v>0.3692307692307693</v>
       </c>
-      <c r="G7" t="n">
+      <c r="M7" t="n">
+        <v>0.3898846160265609</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.4616969946869164</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.9308670701988837</v>
+      </c>
+      <c r="P7" t="n">
         <v>0.6544378698224852</v>
       </c>
-      <c r="H7" t="n">
+      <c r="Q7" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="R7" t="n">
         <v>0.6472518143988502</v>
       </c>
-      <c r="I7" t="n">
+      <c r="S7" t="n">
+        <v>0.6794949702119487</v>
+      </c>
+      <c r="T7" t="n">
         <v>0.3597633136094674</v>
       </c>
-      <c r="J7" t="n">
+      <c r="U7" t="n">
+        <v>0.3899010358829816</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.4617134145433371</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.9316531719204465</v>
+      </c>
+      <c r="X7" t="n">
         <v>0.663905325443787</v>
       </c>
-      <c r="K7" t="n">
+      <c r="Y7" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="Z7" t="n">
         <v>0.673241738062802</v>
       </c>
-      <c r="L7" t="n">
+      <c r="AA7" t="n">
+        <v>0.682605959165969</v>
+      </c>
+      <c r="AB7" t="n">
         <v>0.3940828402366864</v>
       </c>
-      <c r="M7" t="n">
+      <c r="AC7" t="n">
+        <v>0.394382384603763</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0.4659508954888926</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0.9271818253281975</v>
+      </c>
+      <c r="AF7" t="n">
         <v>0.6295857988165681</v>
       </c>
-      <c r="N7" t="n">
+      <c r="AG7" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="AH7" t="n">
         <v>0.6567231436183164</v>
       </c>
-      <c r="O7" t="n">
+      <c r="AI7" t="n">
+        <v>0.6754153366733711</v>
+      </c>
+      <c r="AJ7" t="n">
         <v>0.3487090867469425</v>
       </c>
-      <c r="P7" t="n">
+      <c r="AK7" t="n">
+        <v>0.3798087261690064</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>0.4561858770136031</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>0.9306658281581637</v>
+      </c>
+      <c r="AN7" t="n">
         <v>0.6887573964497041</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="AO7" t="n">
+        <v>0.9680473372781065</v>
+      </c>
+      <c r="AP7" t="n">
         <v>0.6472518143988502</v>
       </c>
-      <c r="R7" t="n">
+      <c r="AQ7" t="n">
+        <v>0.6794949702119487</v>
+      </c>
+      <c r="AR7" t="n">
         <v>0.3597633136094674</v>
       </c>
-      <c r="S7" t="n">
+      <c r="AS7" t="n">
+        <v>0.3899010358829816</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0.4617134145433371</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0.9316531719204465</v>
+      </c>
+      <c r="AV7" t="n">
         <v>0.663905325443787</v>
       </c>
-      <c r="T7" t="n">
+      <c r="AW7" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="AX7" t="n">
         <v>0.6617173282340483</v>
       </c>
-      <c r="U7" t="n">
+      <c r="AY7" t="n">
+        <v>0.6852614943599901</v>
+      </c>
+      <c r="AZ7" t="n">
         <v>0.3692307692307693</v>
       </c>
-      <c r="V7" t="n">
+      <c r="BA7" t="n">
+        <v>0.3954047731352842</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>0.4695833156524867</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>0.9306280952755287</v>
+      </c>
+      <c r="BD7" t="n">
         <v>0.659171597633136</v>
       </c>
-      <c r="W7" t="n">
+      <c r="BE7" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="BF7" t="n">
         <v>0.6485633352186657</v>
       </c>
-      <c r="X7" t="n">
+      <c r="BG7" t="n">
+        <v>0.6404772425069131</v>
+      </c>
+      <c r="BH7" t="n">
         <v>0.3522593826049307</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="BI7" t="n">
+        <v>0.3380078603681406</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>0.4102110981692591</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>0.9307538715509787</v>
+      </c>
+      <c r="BL7" t="n">
         <v>0.6781065088757396</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>0.9751479289940829</v>
       </c>
     </row>
     <row r="8">
@@ -969,71 +1681,189 @@
         <v>0.6231961753542494</v>
       </c>
       <c r="C8" t="n">
+        <v>0.6475440226724331</v>
+      </c>
+      <c r="D8" t="n">
         <v>0.4581329389437645</v>
       </c>
-      <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
+        <v>0.4257441705116161</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.4193132612987965</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.9554028771323009</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="n">
         <v>0.642664571514013</v>
       </c>
-      <c r="F8" t="n">
+      <c r="K8" t="n">
+        <v>0.6795956494698689</v>
+      </c>
+      <c r="L8" t="n">
         <v>0.3609467455621302</v>
       </c>
-      <c r="G8" t="n">
+      <c r="M8" t="n">
+        <v>0.3921248246397566</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.461850246778373</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.9328763461991981</v>
+      </c>
+      <c r="P8" t="n">
         <v>0.6615384615384615</v>
       </c>
-      <c r="H8" t="n">
+      <c r="Q8" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="R8" t="n">
         <v>0.6463369703876924</v>
       </c>
-      <c r="I8" t="n">
+      <c r="S8" t="n">
+        <v>0.6829842074389531</v>
+      </c>
+      <c r="T8" t="n">
         <v>0.3538461538461539</v>
       </c>
-      <c r="J8" t="n">
+      <c r="U8" t="n">
+        <v>0.3924502144476882</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.4664674276110148</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.9328511909441082</v>
+      </c>
+      <c r="X8" t="n">
         <v>0.672189349112426</v>
       </c>
-      <c r="K8" t="n">
+      <c r="Y8" t="n">
+        <v>0.978698224852071</v>
+      </c>
+      <c r="Z8" t="n">
         <v>0.6670610273439631</v>
       </c>
-      <c r="L8" t="n">
+      <c r="AA8" t="n">
+        <v>0.695246229593111</v>
+      </c>
+      <c r="AB8" t="n">
         <v>0.3763313609467456</v>
       </c>
-      <c r="M8" t="n">
+      <c r="AC8" t="n">
+        <v>0.4089360801353088</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>0.4833673197634368</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>0.9262164924141184</v>
+      </c>
+      <c r="AF8" t="n">
         <v>0.6520710059171597</v>
       </c>
-      <c r="N8" t="n">
+      <c r="AG8" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="AH8" t="n">
         <v>0.6562714851961153</v>
       </c>
-      <c r="O8" t="n">
+      <c r="AI8" t="n">
+        <v>0.6480965502188107</v>
+      </c>
+      <c r="AJ8" t="n">
         <v>0.343812504187075</v>
       </c>
-      <c r="P8" t="n">
+      <c r="AK8" t="n">
+        <v>0.3367678583912433</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>0.4200291384055234</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>0.933036710950397</v>
+      </c>
+      <c r="AN8" t="n">
         <v>0.6946745562130178</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="AO8" t="n">
+        <v>0.9680473372781065</v>
+      </c>
+      <c r="AP8" t="n">
         <v>0.6463369703876924</v>
       </c>
-      <c r="R8" t="n">
+      <c r="AQ8" t="n">
+        <v>0.6829842074389531</v>
+      </c>
+      <c r="AR8" t="n">
         <v>0.3538461538461539</v>
       </c>
-      <c r="S8" t="n">
+      <c r="AS8" t="n">
+        <v>0.3924502144476882</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>0.4664674276110148</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>0.9328511909441082</v>
+      </c>
+      <c r="AV8" t="n">
         <v>0.672189349112426</v>
       </c>
-      <c r="T8" t="n">
+      <c r="AW8" t="n">
+        <v>0.978698224852071</v>
+      </c>
+      <c r="AX8" t="n">
         <v>0.6590292304801199</v>
       </c>
-      <c r="U8" t="n">
+      <c r="AY8" t="n">
+        <v>0.7277652269540663</v>
+      </c>
+      <c r="AZ8" t="n">
         <v>0.3538461538461539</v>
       </c>
-      <c r="V8" t="n">
+      <c r="BA8" t="n">
+        <v>0.4162216636935658</v>
+      </c>
+      <c r="BB8" t="n">
+        <v>0.5296422255635036</v>
+      </c>
+      <c r="BC8" t="n">
+        <v>0.9312884207216414</v>
+      </c>
+      <c r="BD8" t="n">
         <v>0.6792899408284023</v>
       </c>
-      <c r="W8" t="n">
+      <c r="BE8" t="n">
+        <v>0.9727810650887574</v>
+      </c>
+      <c r="BF8" t="n">
         <v>0.6471923537518717</v>
       </c>
-      <c r="X8" t="n">
+      <c r="BG8" t="n">
+        <v>0.6458698813988788</v>
+      </c>
+      <c r="BH8" t="n">
         <v>0.3485462319977259</v>
       </c>
-      <c r="Y8" t="n">
+      <c r="BI8" t="n">
+        <v>0.3387561889013129</v>
+      </c>
+      <c r="BJ8" t="n">
+        <v>0.4171479036982017</v>
+      </c>
+      <c r="BK8" t="n">
+        <v>0.9332316641773446</v>
+      </c>
+      <c r="BL8" t="n">
         <v>0.6816568047337278</v>
+      </c>
+      <c r="BM8" t="n">
+        <v>0.9763313609467456</v>
       </c>
     </row>
     <row r="9">
@@ -1046,71 +1876,189 @@
         <v>0.6238736643249453</v>
       </c>
       <c r="C9" t="n">
+        <v>0.6505401601531055</v>
+      </c>
+      <c r="D9" t="n">
         <v>0.458583312345496</v>
       </c>
-      <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
+        <v>0.4279289107842686</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.4232024999720281</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.9560443361370962</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="n">
         <v>0.6454208296431702</v>
       </c>
-      <c r="F9" t="n">
+      <c r="K9" t="n">
+        <v>0.6797228352575057</v>
+      </c>
+      <c r="L9" t="n">
         <v>0.3621301775147929</v>
       </c>
-      <c r="G9" t="n">
+      <c r="M9" t="n">
+        <v>0.3909801875752323</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.4620231327705022</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.9337190472447134</v>
+      </c>
+      <c r="P9" t="n">
         <v>0.6615384615384615</v>
       </c>
-      <c r="H9" t="n">
+      <c r="Q9" t="n">
+        <v>0.9798816568047337</v>
+      </c>
+      <c r="R9" t="n">
         <v>0.6435846357954428</v>
       </c>
-      <c r="I9" t="n">
+      <c r="S9" t="n">
+        <v>0.7105600837480252</v>
+      </c>
+      <c r="T9" t="n">
         <v>0.3526627218934911</v>
       </c>
-      <c r="J9" t="n">
+      <c r="U9" t="n">
+        <v>0.4026623456713827</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.5048956326160006</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.9340146214920211</v>
+      </c>
+      <c r="X9" t="n">
         <v>0.6745562130177515</v>
       </c>
-      <c r="K9" t="n">
+      <c r="Y9" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="Z9" t="n">
         <v>0.6527139518645054</v>
       </c>
-      <c r="L9" t="n">
+      <c r="AA9" t="n">
+        <v>0.6792998659002999</v>
+      </c>
+      <c r="AB9" t="n">
         <v>0.3692307692307693</v>
       </c>
-      <c r="M9" t="n">
+      <c r="AC9" t="n">
+        <v>0.3933556394225973</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>0.4614483078121654</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>0.931058879018945</v>
+      </c>
+      <c r="AF9" t="n">
         <v>0.6544378698224852</v>
       </c>
-      <c r="N9" t="n">
+      <c r="AG9" t="n">
+        <v>0.9798816568047337</v>
+      </c>
+      <c r="AH9" t="n">
         <v>0.648934875833757</v>
       </c>
-      <c r="O9" t="n">
+      <c r="AI9" t="n">
+        <v>0.6441732619680518</v>
+      </c>
+      <c r="AJ9" t="n">
         <v>0.3438419550396201</v>
       </c>
-      <c r="P9" t="n">
+      <c r="AK9" t="n">
+        <v>0.3399296196576965</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>0.4149591914345602</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>0.9337190472447134</v>
+      </c>
+      <c r="AN9" t="n">
         <v>0.693491124260355</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="AO9" t="n">
+        <v>0.9668639053254438</v>
+      </c>
+      <c r="AP9" t="n">
         <v>0.6435846357954428</v>
       </c>
-      <c r="R9" t="n">
+      <c r="AQ9" t="n">
+        <v>0.7105600837480252</v>
+      </c>
+      <c r="AR9" t="n">
         <v>0.3526627218934911</v>
       </c>
-      <c r="S9" t="n">
+      <c r="AS9" t="n">
+        <v>0.4026623456713827</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0.5048956326160006</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.9340146214920211</v>
+      </c>
+      <c r="AV9" t="n">
         <v>0.6745562130177515</v>
       </c>
-      <c r="T9" t="n">
+      <c r="AW9" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="AX9" t="n">
         <v>0.6249260311258431</v>
       </c>
-      <c r="U9" t="n">
+      <c r="AY9" t="n">
+        <v>0.6764817692204672</v>
+      </c>
+      <c r="AZ9" t="n">
         <v>0.3431952662721893</v>
       </c>
-      <c r="V9" t="n">
+      <c r="BA9" t="n">
+        <v>0.3892934662968631</v>
+      </c>
+      <c r="BB9" t="n">
+        <v>0.4576275840876534</v>
+      </c>
+      <c r="BC9" t="n">
+        <v>0.9359767313890417</v>
+      </c>
+      <c r="BD9" t="n">
         <v>0.6781065088757396</v>
       </c>
-      <c r="W9" t="n">
+      <c r="BE9" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="BF9" t="n">
         <v>0.6397516342665694</v>
       </c>
-      <c r="X9" t="n">
+      <c r="BG9" t="n">
+        <v>0.6419329846076135</v>
+      </c>
+      <c r="BH9" t="n">
         <v>0.348575682850271</v>
       </c>
-      <c r="Y9" t="n">
+      <c r="BI9" t="n">
+        <v>0.3419179501677661</v>
+      </c>
+      <c r="BJ9" t="n">
+        <v>0.4120779567272385</v>
+      </c>
+      <c r="BK9" t="n">
+        <v>0.9339140004716611</v>
+      </c>
+      <c r="BL9" t="n">
         <v>0.6804733727810651</v>
+      </c>
+      <c r="BM9" t="n">
+        <v>0.9751479289940829</v>
       </c>
     </row>
     <row r="10">
@@ -1123,71 +2071,189 @@
         <v>0.4942965567185033</v>
       </c>
       <c r="C10" t="n">
+        <v>0.6067127751946909</v>
+      </c>
+      <c r="D10" t="n">
         <v>0.3472105258651251</v>
       </c>
-      <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
+        <v>0.3934425383849193</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.3681003915844435</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.9770363965097083</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="n">
         <v>0.5125640384294671</v>
       </c>
-      <c r="F10" t="n">
+      <c r="K10" t="n">
+        <v>0.5962414758560869</v>
+      </c>
+      <c r="L10" t="n">
         <v>0.2177514792899408</v>
       </c>
-      <c r="G10" t="n">
+      <c r="M10" t="n">
+        <v>0.2689844154452598</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.3555038975310447</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.9568241490448864</v>
+      </c>
+      <c r="P10" t="n">
         <v>0.8011834319526627</v>
       </c>
-      <c r="H10" t="n">
+      <c r="Q10" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="R10" t="n">
         <v>0.5125640384294671</v>
       </c>
-      <c r="I10" t="n">
+      <c r="S10" t="n">
+        <v>0.5962414758560869</v>
+      </c>
+      <c r="T10" t="n">
         <v>0.2177514792899408</v>
       </c>
-      <c r="J10" t="n">
+      <c r="U10" t="n">
+        <v>0.2689844154452598</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.3555038975310447</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.9568241490448864</v>
+      </c>
+      <c r="X10" t="n">
         <v>0.8011834319526627</v>
       </c>
-      <c r="K10" t="n">
+      <c r="Y10" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="Z10" t="n">
         <v>0.5428393465962261</v>
       </c>
-      <c r="L10" t="n">
+      <c r="AA10" t="n">
+        <v>0.6115371438006899</v>
+      </c>
+      <c r="AB10" t="n">
         <v>0.2473372781065089</v>
       </c>
-      <c r="M10" t="n">
+      <c r="AC10" t="n">
+        <v>0.2843526061000089</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>0.3739776782479056</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>0.9512365380080182</v>
+      </c>
+      <c r="AF10" t="n">
         <v>0.7727810650887574</v>
       </c>
-      <c r="N10" t="n">
+      <c r="AG10" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="AH10" t="n">
         <v>0.4857484021051881</v>
       </c>
-      <c r="O10" t="n">
+      <c r="AI10" t="n">
+        <v>0.5971617203860753</v>
+      </c>
+      <c r="AJ10" t="n">
         <v>0.1915325847455647</v>
       </c>
-      <c r="P10" t="n">
+      <c r="AK10" t="n">
+        <v>0.2708091713879109</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>0.3566021202944571</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>0.9583963524880119</v>
+      </c>
+      <c r="AN10" t="n">
         <v>0.8307692307692308</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="AO10" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="AP10" t="n">
         <v>0.5125640384294671</v>
       </c>
-      <c r="R10" t="n">
+      <c r="AQ10" t="n">
+        <v>0.5962414758560869</v>
+      </c>
+      <c r="AR10" t="n">
         <v>0.2177514792899408</v>
       </c>
-      <c r="S10" t="n">
+      <c r="AS10" t="n">
+        <v>0.2689844154452598</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>0.3555038975310447</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>0.9568241490448864</v>
+      </c>
+      <c r="AV10" t="n">
         <v>0.8011834319526627</v>
       </c>
-      <c r="T10" t="n">
+      <c r="AW10" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="AX10" t="n">
         <v>0.5008867875722987</v>
       </c>
-      <c r="U10" t="n">
+      <c r="AY10" t="n">
+        <v>0.5961744187172013</v>
+      </c>
+      <c r="AZ10" t="n">
         <v>0.2035502958579882</v>
       </c>
-      <c r="V10" t="n">
+      <c r="BA10" t="n">
+        <v>0.2657988653848962</v>
+      </c>
+      <c r="BB10" t="n">
+        <v>0.3554239375327929</v>
+      </c>
+      <c r="BC10" t="n">
+        <v>0.95619212326075</v>
+      </c>
+      <c r="BD10" t="n">
         <v>0.8165680473372781</v>
       </c>
-      <c r="W10" t="n">
+      <c r="BE10" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="BF10" t="n">
         <v>0.4953977853897263</v>
       </c>
-      <c r="X10" t="n">
+      <c r="BG10" t="n">
+        <v>0.5980278563594071</v>
+      </c>
+      <c r="BH10" t="n">
         <v>0.2010000403668665</v>
       </c>
-      <c r="Y10" t="n">
+      <c r="BI10" t="n">
+        <v>0.2718443680752815</v>
+      </c>
+      <c r="BJ10" t="n">
+        <v>0.3576373169818277</v>
+      </c>
+      <c r="BK10" t="n">
+        <v>0.9580661897649556</v>
+      </c>
+      <c r="BL10" t="n">
         <v>0.821301775147929</v>
+      </c>
+      <c r="BM10" t="n">
+        <v>0.9846153846153847</v>
       </c>
     </row>
     <row r="11">
@@ -1200,71 +2266,189 @@
         <v>0.5862203024542455</v>
       </c>
       <c r="C11" t="n">
+        <v>0.7747276358948593</v>
+      </c>
+      <c r="D11" t="n">
         <v>0.4112175851766155</v>
       </c>
-      <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
+        <v>0.4805414953307796</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.6002029098192376</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.9590692555616697</v>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="n">
         <v>0.633390426161197</v>
       </c>
-      <c r="F11" t="n">
+      <c r="K11" t="n">
+        <v>0.8205539802432845</v>
+      </c>
+      <c r="L11" t="n">
         <v>0.3443786982248521</v>
       </c>
-      <c r="G11" t="n">
+      <c r="M11" t="n">
+        <v>0.4407138349732355</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.6733088344930965</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.9309991352881063</v>
+      </c>
+      <c r="P11" t="n">
         <v>0.6828402366863905</v>
       </c>
-      <c r="H11" t="n">
+      <c r="Q11" t="n">
+        <v>0.9739644970414201</v>
+      </c>
+      <c r="R11" t="n">
         <v>0.7016464154456233</v>
       </c>
-      <c r="I11" t="n">
+      <c r="S11" t="n">
+        <v>0.7893841050423023</v>
+      </c>
+      <c r="T11" t="n">
         <v>0.4260355029585799</v>
       </c>
-      <c r="J11" t="n">
+      <c r="U11" t="n">
+        <v>0.4631208089866726</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.6231272652934365</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.9282383460419779</v>
+      </c>
+      <c r="X11" t="n">
         <v>0.6059171597633136</v>
       </c>
-      <c r="K11" t="n">
+      <c r="Y11" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="Z11" t="n">
         <v>0.6445033866354896</v>
       </c>
-      <c r="L11" t="n">
+      <c r="AA11" t="n">
+        <v>0.8542069145347269</v>
+      </c>
+      <c r="AB11" t="n">
         <v>0.3325443786982248</v>
       </c>
-      <c r="M11" t="n">
+      <c r="AC11" t="n">
+        <v>0.4730153999104796</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>0.7296694528389381</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0.9315682729345177</v>
+      </c>
+      <c r="AF11" t="n">
         <v>0.7065088757396449</v>
       </c>
-      <c r="N11" t="n">
+      <c r="AG11" t="n">
+        <v>0.9633136094674556</v>
+      </c>
+      <c r="AH11" t="n">
         <v>0.7016464154456233</v>
       </c>
-      <c r="O11" t="n">
+      <c r="AI11" t="n">
+        <v>0.7893841050423023</v>
+      </c>
+      <c r="AJ11" t="n">
         <v>0.4260355029585799</v>
       </c>
-      <c r="P11" t="n">
+      <c r="AK11" t="n">
+        <v>0.4631208089866726</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>0.6231272652934365</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>0.9282383460419779</v>
+      </c>
+      <c r="AN11" t="n">
         <v>0.6059171597633136</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="AO11" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="AP11" t="n">
         <v>0.651806774286611</v>
       </c>
-      <c r="R11" t="n">
+      <c r="AQ11" t="n">
+        <v>0.7667822591076271</v>
+      </c>
+      <c r="AR11" t="n">
         <v>0.3704142011834319</v>
       </c>
-      <c r="S11" t="n">
+      <c r="AS11" t="n">
+        <v>0.4070150695911505</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>0.5879550328821962</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>0.9307884600267274</v>
+      </c>
+      <c r="AV11" t="n">
         <v>0.6556213017751479</v>
       </c>
-      <c r="T11" t="n">
+      <c r="AW11" t="n">
+        <v>0.9751479289940829</v>
+      </c>
+      <c r="AX11" t="n">
         <v>0.6287020535908477</v>
       </c>
-      <c r="U11" t="n">
+      <c r="AY11" t="n">
+        <v>0.8361010748521609</v>
+      </c>
+      <c r="AZ11" t="n">
         <v>0.3266272189349113</v>
       </c>
-      <c r="V11" t="n">
+      <c r="BA11" t="n">
+        <v>0.4555597269929796</v>
+      </c>
+      <c r="BB11" t="n">
+        <v>0.6990650073689387</v>
+      </c>
+      <c r="BC11" t="n">
+        <v>0.9343542174357362</v>
+      </c>
+      <c r="BD11" t="n">
         <v>0.7053254437869823</v>
       </c>
-      <c r="W11" t="n">
+      <c r="BE11" t="n">
+        <v>0.9704142011834319</v>
+      </c>
+      <c r="BF11" t="n">
         <v>0.651806774286611</v>
       </c>
-      <c r="X11" t="n">
+      <c r="BG11" t="n">
+        <v>0.7667822591076271</v>
+      </c>
+      <c r="BH11" t="n">
         <v>0.3704142011834319</v>
       </c>
-      <c r="Y11" t="n">
+      <c r="BI11" t="n">
+        <v>0.4070150695911505</v>
+      </c>
+      <c r="BJ11" t="n">
+        <v>0.5879550328821962</v>
+      </c>
+      <c r="BK11" t="n">
+        <v>0.9307884600267274</v>
+      </c>
+      <c r="BL11" t="n">
         <v>0.6556213017751479</v>
+      </c>
+      <c r="BM11" t="n">
+        <v>0.9751479289940829</v>
       </c>
     </row>
     <row r="12">
@@ -1277,71 +2461,189 @@
         <v>0.4467402618283487</v>
       </c>
       <c r="C12" t="n">
+        <v>0.5668173650973868</v>
+      </c>
+      <c r="D12" t="n">
         <v>0.263498224852071</v>
       </c>
-      <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
+        <v>0.3424043125107377</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.3212819253759442</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.9799952833896706</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="n">
         <v>0.4925480182640652</v>
       </c>
-      <c r="F12" t="n">
+      <c r="K12" t="n">
+        <v>0.6284945221690352</v>
+      </c>
+      <c r="L12" t="n">
         <v>0.1905325443786982</v>
       </c>
-      <c r="G12" t="n">
+      <c r="M12" t="n">
+        <v>0.2942171276302885</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.395005364396484</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.9600031444068863</v>
+      </c>
+      <c r="P12" t="n">
         <v>0.829585798816568</v>
       </c>
-      <c r="H12" t="n">
+      <c r="Q12" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="R12" t="n">
         <v>0.4937478934117296</v>
       </c>
-      <c r="I12" t="n">
+      <c r="S12" t="n">
+        <v>0.6431215278839518</v>
+      </c>
+      <c r="T12" t="n">
         <v>0.1893491124260355</v>
       </c>
-      <c r="J12" t="n">
+      <c r="U12" t="n">
+        <v>0.3094873878932521</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.4136052996277887</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.9612954956371355</v>
+      </c>
+      <c r="X12" t="n">
         <v>0.8319526627218935</v>
       </c>
-      <c r="K12" t="n">
+      <c r="Y12" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="Z12" t="n">
         <v>0.5137171648327384</v>
       </c>
-      <c r="L12" t="n">
+      <c r="AA12" t="n">
+        <v>0.6315384603567777</v>
+      </c>
+      <c r="AB12" t="n">
         <v>0.2047337278106509</v>
       </c>
-      <c r="M12" t="n">
+      <c r="AC12" t="n">
+        <v>0.2959656336218747</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0.3988408269098094</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0.9579655687445956</v>
+      </c>
+      <c r="AF12" t="n">
         <v>0.8189349112426035</v>
       </c>
-      <c r="N12" t="n">
+      <c r="AG12" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="AH12" t="n">
         <v>0.4877189995122264</v>
       </c>
-      <c r="O12" t="n">
+      <c r="AI12" t="n">
+        <v>0.6465303491816524</v>
+      </c>
+      <c r="AJ12" t="n">
         <v>0.1905325443786982</v>
       </c>
-      <c r="P12" t="n">
+      <c r="AK12" t="n">
+        <v>0.3232003508647483</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>0.4180014924129494</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>0.9625060922883422</v>
+      </c>
+      <c r="AN12" t="n">
         <v>0.8284023668639053</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="AO12" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="AP12" t="n">
         <v>0.4937478934117296</v>
       </c>
-      <c r="R12" t="n">
+      <c r="AQ12" t="n">
+        <v>0.6431215278839518</v>
+      </c>
+      <c r="AR12" t="n">
         <v>0.1893491124260355</v>
       </c>
-      <c r="S12" t="n">
+      <c r="AS12" t="n">
+        <v>0.3094873878932521</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0.4136052996277887</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.9612954956371355</v>
+      </c>
+      <c r="AV12" t="n">
         <v>0.8319526627218935</v>
       </c>
-      <c r="T12" t="n">
+      <c r="AW12" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="AX12" t="n">
         <v>0.5148677086363542</v>
       </c>
-      <c r="U12" t="n">
+      <c r="AY12" t="n">
+        <v>0.6406375715079251</v>
+      </c>
+      <c r="AZ12" t="n">
         <v>0.2035502958579882</v>
       </c>
-      <c r="V12" t="n">
+      <c r="BA12" t="n">
+        <v>0.3040630438700719</v>
+      </c>
+      <c r="BB12" t="n">
+        <v>0.4104164980275718</v>
+      </c>
+      <c r="BC12" t="n">
+        <v>0.9581165002751356</v>
+      </c>
+      <c r="BD12" t="n">
         <v>0.821301775147929</v>
       </c>
-      <c r="W12" t="n">
+      <c r="BE12" t="n">
+        <v>0.9798816568047337</v>
+      </c>
+      <c r="BF12" t="n">
         <v>0.4877189995122264</v>
       </c>
-      <c r="X12" t="n">
+      <c r="BG12" t="n">
+        <v>0.6465303491816524</v>
+      </c>
+      <c r="BH12" t="n">
         <v>0.1905325443786982</v>
       </c>
-      <c r="Y12" t="n">
+      <c r="BI12" t="n">
+        <v>0.3232003508647483</v>
+      </c>
+      <c r="BJ12" t="n">
+        <v>0.4180014924129494</v>
+      </c>
+      <c r="BK12" t="n">
+        <v>0.9625060922883422</v>
+      </c>
+      <c r="BL12" t="n">
         <v>0.8284023668639053</v>
+      </c>
+      <c r="BM12" t="n">
+        <v>0.9846153846153847</v>
       </c>
     </row>
     <row r="13">
@@ -1351,74 +2653,192 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4554190548258276</v>
+        <v>0.4623824243811015</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2745606345879602</v>
-      </c>
-      <c r="D13" t="inlineStr"/>
+        <v>0.6340636203826128</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.2835653659182524</v>
+      </c>
       <c r="E13" t="n">
-        <v>0.4791511231506904</v>
+        <v>0.3916669329988137</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1798816568047337</v>
+        <v>0.402036674692706</v>
       </c>
       <c r="G13" t="n">
-        <v>0.8390532544378698</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.6837072628704299</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.4035502958579882</v>
-      </c>
+        <v>0.9774891911013285</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="n">
-        <v>0.6177514792899408</v>
+        <v>0.506759048984634</v>
       </c>
       <c r="K13" t="n">
-        <v>0.5547001962252291</v>
+        <v>0.6832498933534507</v>
       </c>
       <c r="L13" t="n">
-        <v>0.2461538461538462</v>
+        <v>0.2047337278106509</v>
       </c>
       <c r="M13" t="n">
-        <v>0.778698224852071</v>
+        <v>0.3676863681113329</v>
       </c>
       <c r="N13" t="n">
-        <v>0.6839639214624242</v>
+        <v>0.4668304167675018</v>
       </c>
       <c r="O13" t="n">
-        <v>0.4059822971712957</v>
+        <v>0.9576448392421979</v>
       </c>
       <c r="P13" t="n">
-        <v>0.6177514792899408</v>
+        <v>0.8153846153846154</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.5373615137407071</v>
+        <v>0.9846153846153847</v>
       </c>
       <c r="R13" t="n">
-        <v>0.2414201183431953</v>
+        <v>0.6897388237372275</v>
       </c>
       <c r="S13" t="n">
-        <v>0.7751479289940828</v>
+        <v>0.8069421254921904</v>
       </c>
       <c r="T13" t="n">
-        <v>0.5032439148860347</v>
+        <v>0.4165680473372781</v>
       </c>
       <c r="U13" t="n">
-        <v>0.1988165680473373</v>
+        <v>0.498881278649509</v>
       </c>
       <c r="V13" t="n">
-        <v>0.8224852071005917</v>
+        <v>0.6511555938938538</v>
       </c>
       <c r="W13" t="n">
-        <v>0.5376880331662462</v>
+        <v>0.9405864318842858</v>
       </c>
       <c r="X13" t="n">
-        <v>0.2438521196565028</v>
+        <v>0.6047337278106509</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.7751479289940828</v>
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.5704768066996664</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>0.7045740871608913</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0.2662721893491125</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>0.3875769576655045</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>0.4964246442986033</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0.9460231113906139</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>0.757396449704142</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>0.6901479538241796</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>0.8071588678204578</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>0.4196669759671213</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>0.5006239891110495</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>0.6515054379012032</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>0.9406147315462621</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>0.6047337278106509</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>0.54934064834945</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>0.6865582680204986</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>0.2544378698224852</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>0.3755228840810114</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>0.4713622553873067</v>
+      </c>
+      <c r="AU13" t="n">
+        <v>0.951972329219401</v>
+      </c>
+      <c r="AV13" t="n">
+        <v>0.7633136094674556</v>
+      </c>
+      <c r="AW13" t="n">
+        <v>0.98698224852071</v>
+      </c>
+      <c r="AX13" t="n">
+        <v>0.5228506297835824</v>
+      </c>
+      <c r="AY13" t="n">
+        <v>0.7018357277289305</v>
+      </c>
+      <c r="AZ13" t="n">
+        <v>0.221301775147929</v>
+      </c>
+      <c r="BA13" t="n">
+        <v>0.393812658605438</v>
+      </c>
+      <c r="BB13" t="n">
+        <v>0.4925733887167976</v>
+      </c>
+      <c r="BC13" t="n">
+        <v>0.9541985692948668</v>
+      </c>
+      <c r="BD13" t="n">
+        <v>0.7988165680473372</v>
+      </c>
+      <c r="BE13" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="BF13" t="n">
+        <v>0.5498542544404671</v>
+      </c>
+      <c r="BG13" t="n">
+        <v>0.686813001765878</v>
+      </c>
+      <c r="BH13" t="n">
+        <v>0.2575367984523284</v>
+      </c>
+      <c r="BI13" t="n">
+        <v>0.377265594542552</v>
+      </c>
+      <c r="BJ13" t="n">
+        <v>0.471712099394656</v>
+      </c>
+      <c r="BK13" t="n">
+        <v>0.9520540837984435</v>
+      </c>
+      <c r="BL13" t="n">
+        <v>0.7633136094674556</v>
+      </c>
+      <c r="BM13" t="n">
+        <v>0.9857988165680474</v>
       </c>
     </row>
     <row r="14">
@@ -1431,71 +2851,189 @@
         <v>0.6499886207470034</v>
       </c>
       <c r="C14" t="n">
+        <v>0.6852985072099496</v>
+      </c>
+      <c r="D14" t="n">
         <v>0.3467455621301775</v>
       </c>
-      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
+        <v>0.3861356324277022</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.4696340439841853</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.9304614417105573</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="n">
         <v>0.6499886207470034</v>
       </c>
-      <c r="F14" t="n">
-        <v>0.3467455621301775</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.6887573964497041</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.6499886207470034</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.3467455621301775</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.6887573964497041</v>
-      </c>
       <c r="K14" t="n">
-        <v>0.6499886207470034</v>
+        <v>0.6852985072099496</v>
       </c>
       <c r="L14" t="n">
         <v>0.3467455621301775</v>
       </c>
       <c r="M14" t="n">
-        <v>0.6887573964497041</v>
+        <v>0.3861356324277022</v>
       </c>
       <c r="N14" t="n">
-        <v>0.6499886207470034</v>
+        <v>0.4696340439841853</v>
       </c>
       <c r="O14" t="n">
-        <v>0.3467455621301775</v>
+        <v>0.9304614417105573</v>
       </c>
       <c r="P14" t="n">
         <v>0.6887573964497041</v>
       </c>
       <c r="Q14" t="n">
+        <v>0.9668639053254438</v>
+      </c>
+      <c r="R14" t="n">
         <v>0.6499886207470034</v>
       </c>
-      <c r="R14" t="n">
+      <c r="S14" t="n">
+        <v>0.6852985072099496</v>
+      </c>
+      <c r="T14" t="n">
         <v>0.3467455621301775</v>
       </c>
-      <c r="S14" t="n">
+      <c r="U14" t="n">
+        <v>0.3861356324277022</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0.4696340439841853</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0.9304614417105573</v>
+      </c>
+      <c r="X14" t="n">
         <v>0.6887573964497041</v>
       </c>
-      <c r="T14" t="n">
+      <c r="Y14" t="n">
+        <v>0.9668639053254438</v>
+      </c>
+      <c r="Z14" t="n">
         <v>0.6499886207470034</v>
       </c>
-      <c r="U14" t="n">
+      <c r="AA14" t="n">
+        <v>0.6852985072099496</v>
+      </c>
+      <c r="AB14" t="n">
         <v>0.3467455621301775</v>
       </c>
-      <c r="V14" t="n">
+      <c r="AC14" t="n">
+        <v>0.3861356324277022</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>0.4696340439841853</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>0.9304614417105573</v>
+      </c>
+      <c r="AF14" t="n">
         <v>0.6887573964497041</v>
       </c>
-      <c r="W14" t="n">
+      <c r="AG14" t="n">
+        <v>0.9668639053254438</v>
+      </c>
+      <c r="AH14" t="n">
         <v>0.6499886207470034</v>
       </c>
-      <c r="X14" t="n">
+      <c r="AI14" t="n">
+        <v>0.6852985072099496</v>
+      </c>
+      <c r="AJ14" t="n">
         <v>0.3467455621301775</v>
       </c>
-      <c r="Y14" t="n">
+      <c r="AK14" t="n">
+        <v>0.3861356324277022</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>0.4696340439841853</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>0.9304614417105573</v>
+      </c>
+      <c r="AN14" t="n">
         <v>0.6887573964497041</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>0.9668639053254438</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>0.6499886207470034</v>
+      </c>
+      <c r="AQ14" t="n">
+        <v>0.6852985072099496</v>
+      </c>
+      <c r="AR14" t="n">
+        <v>0.3467455621301775</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>0.3861356324277022</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>0.4696340439841853</v>
+      </c>
+      <c r="AU14" t="n">
+        <v>0.9304614417105573</v>
+      </c>
+      <c r="AV14" t="n">
+        <v>0.6887573964497041</v>
+      </c>
+      <c r="AW14" t="n">
+        <v>0.9668639053254438</v>
+      </c>
+      <c r="AX14" t="n">
+        <v>0.6499886207470034</v>
+      </c>
+      <c r="AY14" t="n">
+        <v>0.6852985072099496</v>
+      </c>
+      <c r="AZ14" t="n">
+        <v>0.3467455621301775</v>
+      </c>
+      <c r="BA14" t="n">
+        <v>0.3861356324277022</v>
+      </c>
+      <c r="BB14" t="n">
+        <v>0.4696340439841853</v>
+      </c>
+      <c r="BC14" t="n">
+        <v>0.9304614417105573</v>
+      </c>
+      <c r="BD14" t="n">
+        <v>0.6887573964497041</v>
+      </c>
+      <c r="BE14" t="n">
+        <v>0.9668639053254438</v>
+      </c>
+      <c r="BF14" t="n">
+        <v>0.6499886207470034</v>
+      </c>
+      <c r="BG14" t="n">
+        <v>0.6852985072099496</v>
+      </c>
+      <c r="BH14" t="n">
+        <v>0.3467455621301775</v>
+      </c>
+      <c r="BI14" t="n">
+        <v>0.3861356324277022</v>
+      </c>
+      <c r="BJ14" t="n">
+        <v>0.4696340439841853</v>
+      </c>
+      <c r="BK14" t="n">
+        <v>0.9304614417105573</v>
+      </c>
+      <c r="BL14" t="n">
+        <v>0.6887573964497041</v>
+      </c>
+      <c r="BM14" t="n">
+        <v>0.9668639053254438</v>
       </c>
     </row>
     <row r="15">
@@ -1508,71 +3046,189 @@
         <v>0.6066690508655493</v>
       </c>
       <c r="C15" t="n">
+        <v>0.6576778610115588</v>
+      </c>
+      <c r="D15" t="n">
         <v>0.3112426035502959</v>
       </c>
-      <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
+        <v>0.3610679494145611</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.4325401688647393</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.9394764562534392</v>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="n">
         <v>0.6066690508655493</v>
       </c>
-      <c r="F15" t="n">
-        <v>0.3112426035502959</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.7159763313609467</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.6066690508655493</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0.3112426035502959</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0.7159763313609467</v>
-      </c>
       <c r="K15" t="n">
-        <v>0.6066690508655493</v>
+        <v>0.6576778610115588</v>
       </c>
       <c r="L15" t="n">
         <v>0.3112426035502959</v>
       </c>
       <c r="M15" t="n">
-        <v>0.7159763313609467</v>
+        <v>0.3610679494145611</v>
       </c>
       <c r="N15" t="n">
-        <v>0.6066690508655493</v>
+        <v>0.4325401688647393</v>
       </c>
       <c r="O15" t="n">
-        <v>0.3112426035502959</v>
+        <v>0.9394764562534392</v>
       </c>
       <c r="P15" t="n">
         <v>0.7159763313609467</v>
       </c>
       <c r="Q15" t="n">
+        <v>0.9739644970414201</v>
+      </c>
+      <c r="R15" t="n">
         <v>0.6066690508655493</v>
       </c>
-      <c r="R15" t="n">
+      <c r="S15" t="n">
+        <v>0.6576778610115588</v>
+      </c>
+      <c r="T15" t="n">
         <v>0.3112426035502959</v>
       </c>
-      <c r="S15" t="n">
+      <c r="U15" t="n">
+        <v>0.3610679494145611</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0.4325401688647393</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0.9394764562534392</v>
+      </c>
+      <c r="X15" t="n">
         <v>0.7159763313609467</v>
       </c>
-      <c r="T15" t="n">
+      <c r="Y15" t="n">
+        <v>0.9739644970414201</v>
+      </c>
+      <c r="Z15" t="n">
         <v>0.6066690508655493</v>
       </c>
-      <c r="U15" t="n">
+      <c r="AA15" t="n">
+        <v>0.6576778610115588</v>
+      </c>
+      <c r="AB15" t="n">
         <v>0.3112426035502959</v>
       </c>
-      <c r="V15" t="n">
+      <c r="AC15" t="n">
+        <v>0.3610679494145611</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>0.4325401688647393</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>0.9394764562534392</v>
+      </c>
+      <c r="AF15" t="n">
         <v>0.7159763313609467</v>
       </c>
-      <c r="W15" t="n">
+      <c r="AG15" t="n">
+        <v>0.9739644970414201</v>
+      </c>
+      <c r="AH15" t="n">
         <v>0.6066690508655493</v>
       </c>
-      <c r="X15" t="n">
+      <c r="AI15" t="n">
+        <v>0.6576778610115588</v>
+      </c>
+      <c r="AJ15" t="n">
         <v>0.3112426035502959</v>
       </c>
-      <c r="Y15" t="n">
+      <c r="AK15" t="n">
+        <v>0.3610679494145611</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>0.4325401688647393</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>0.9394764562534392</v>
+      </c>
+      <c r="AN15" t="n">
         <v>0.7159763313609467</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>0.9739644970414201</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>0.6066690508655493</v>
+      </c>
+      <c r="AQ15" t="n">
+        <v>0.6576778610115588</v>
+      </c>
+      <c r="AR15" t="n">
+        <v>0.3112426035502959</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>0.3610679494145611</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>0.4325401688647393</v>
+      </c>
+      <c r="AU15" t="n">
+        <v>0.9394764562534392</v>
+      </c>
+      <c r="AV15" t="n">
+        <v>0.7159763313609467</v>
+      </c>
+      <c r="AW15" t="n">
+        <v>0.9739644970414201</v>
+      </c>
+      <c r="AX15" t="n">
+        <v>0.6066690508655493</v>
+      </c>
+      <c r="AY15" t="n">
+        <v>0.6576778610115588</v>
+      </c>
+      <c r="AZ15" t="n">
+        <v>0.3112426035502959</v>
+      </c>
+      <c r="BA15" t="n">
+        <v>0.3610679494145611</v>
+      </c>
+      <c r="BB15" t="n">
+        <v>0.4325401688647393</v>
+      </c>
+      <c r="BC15" t="n">
+        <v>0.9394764562534392</v>
+      </c>
+      <c r="BD15" t="n">
+        <v>0.7159763313609467</v>
+      </c>
+      <c r="BE15" t="n">
+        <v>0.9739644970414201</v>
+      </c>
+      <c r="BF15" t="n">
+        <v>0.6066690508655493</v>
+      </c>
+      <c r="BG15" t="n">
+        <v>0.6576778610115588</v>
+      </c>
+      <c r="BH15" t="n">
+        <v>0.3112426035502959</v>
+      </c>
+      <c r="BI15" t="n">
+        <v>0.3610679494145611</v>
+      </c>
+      <c r="BJ15" t="n">
+        <v>0.4325401688647393</v>
+      </c>
+      <c r="BK15" t="n">
+        <v>0.9394764562534392</v>
+      </c>
+      <c r="BL15" t="n">
+        <v>0.7159763313609467</v>
+      </c>
+      <c r="BM15" t="n">
+        <v>0.9739644970414201</v>
       </c>
     </row>
     <row r="16">
@@ -1585,71 +3241,189 @@
         <v>0.6017725297110137</v>
       </c>
       <c r="C16" t="n">
+        <v>0.6883138174732198</v>
+      </c>
+      <c r="D16" t="n">
         <v>0.2035502958579882</v>
       </c>
-      <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
+        <v>0.3474697619873517</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.473775911324557</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.956943636506564</v>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="n">
         <v>0.6017725297110137</v>
       </c>
-      <c r="F16" t="n">
-        <v>0.2035502958579882</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.8319526627218935</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.6017725297110137</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0.2035502958579882</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0.8319526627218935</v>
-      </c>
       <c r="K16" t="n">
-        <v>0.6017725297110137</v>
+        <v>0.6883138174732198</v>
       </c>
       <c r="L16" t="n">
         <v>0.2035502958579882</v>
       </c>
       <c r="M16" t="n">
-        <v>0.8319526627218935</v>
+        <v>0.3474697619873517</v>
       </c>
       <c r="N16" t="n">
-        <v>0.6017725297110137</v>
+        <v>0.473775911324557</v>
       </c>
       <c r="O16" t="n">
-        <v>0.2035502958579882</v>
+        <v>0.956943636506564</v>
       </c>
       <c r="P16" t="n">
         <v>0.8319526627218935</v>
       </c>
       <c r="Q16" t="n">
+        <v>0.9751479289940829</v>
+      </c>
+      <c r="R16" t="n">
         <v>0.6017725297110137</v>
       </c>
-      <c r="R16" t="n">
+      <c r="S16" t="n">
+        <v>0.6883138174732198</v>
+      </c>
+      <c r="T16" t="n">
         <v>0.2035502958579882</v>
       </c>
-      <c r="S16" t="n">
+      <c r="U16" t="n">
+        <v>0.3474697619873517</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0.473775911324557</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0.956943636506564</v>
+      </c>
+      <c r="X16" t="n">
         <v>0.8319526627218935</v>
       </c>
-      <c r="T16" t="n">
+      <c r="Y16" t="n">
+        <v>0.9751479289940829</v>
+      </c>
+      <c r="Z16" t="n">
         <v>0.6017725297110137</v>
       </c>
-      <c r="U16" t="n">
+      <c r="AA16" t="n">
+        <v>0.6883138174732198</v>
+      </c>
+      <c r="AB16" t="n">
         <v>0.2035502958579882</v>
       </c>
-      <c r="V16" t="n">
+      <c r="AC16" t="n">
+        <v>0.3474697619873517</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>0.473775911324557</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>0.956943636506564</v>
+      </c>
+      <c r="AF16" t="n">
         <v>0.8319526627218935</v>
       </c>
-      <c r="W16" t="n">
+      <c r="AG16" t="n">
+        <v>0.9751479289940829</v>
+      </c>
+      <c r="AH16" t="n">
         <v>0.6017725297110137</v>
       </c>
-      <c r="X16" t="n">
+      <c r="AI16" t="n">
+        <v>0.6883138174732198</v>
+      </c>
+      <c r="AJ16" t="n">
         <v>0.2035502958579882</v>
       </c>
-      <c r="Y16" t="n">
+      <c r="AK16" t="n">
+        <v>0.3474697619873517</v>
+      </c>
+      <c r="AL16" t="n">
+        <v>0.473775911324557</v>
+      </c>
+      <c r="AM16" t="n">
+        <v>0.956943636506564</v>
+      </c>
+      <c r="AN16" t="n">
         <v>0.8319526627218935</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>0.9751479289940829</v>
+      </c>
+      <c r="AP16" t="n">
+        <v>0.6017725297110137</v>
+      </c>
+      <c r="AQ16" t="n">
+        <v>0.6883138174732198</v>
+      </c>
+      <c r="AR16" t="n">
+        <v>0.2035502958579882</v>
+      </c>
+      <c r="AS16" t="n">
+        <v>0.3474697619873517</v>
+      </c>
+      <c r="AT16" t="n">
+        <v>0.473775911324557</v>
+      </c>
+      <c r="AU16" t="n">
+        <v>0.956943636506564</v>
+      </c>
+      <c r="AV16" t="n">
+        <v>0.8319526627218935</v>
+      </c>
+      <c r="AW16" t="n">
+        <v>0.9751479289940829</v>
+      </c>
+      <c r="AX16" t="n">
+        <v>0.6017725297110137</v>
+      </c>
+      <c r="AY16" t="n">
+        <v>0.6883138174732198</v>
+      </c>
+      <c r="AZ16" t="n">
+        <v>0.2035502958579882</v>
+      </c>
+      <c r="BA16" t="n">
+        <v>0.3474697619873517</v>
+      </c>
+      <c r="BB16" t="n">
+        <v>0.473775911324557</v>
+      </c>
+      <c r="BC16" t="n">
+        <v>0.956943636506564</v>
+      </c>
+      <c r="BD16" t="n">
+        <v>0.8319526627218935</v>
+      </c>
+      <c r="BE16" t="n">
+        <v>0.9751479289940829</v>
+      </c>
+      <c r="BF16" t="n">
+        <v>0.6017725297110137</v>
+      </c>
+      <c r="BG16" t="n">
+        <v>0.6883138174732198</v>
+      </c>
+      <c r="BH16" t="n">
+        <v>0.2035502958579882</v>
+      </c>
+      <c r="BI16" t="n">
+        <v>0.3474697619873517</v>
+      </c>
+      <c r="BJ16" t="n">
+        <v>0.473775911324557</v>
+      </c>
+      <c r="BK16" t="n">
+        <v>0.956943636506564</v>
+      </c>
+      <c r="BL16" t="n">
+        <v>0.8319526627218935</v>
+      </c>
+      <c r="BM16" t="n">
+        <v>0.9751479289940829</v>
       </c>
     </row>
     <row r="17">
@@ -1662,71 +3436,189 @@
         <v>0.5938541250959626</v>
       </c>
       <c r="C17" t="n">
+        <v>0.661357302381815</v>
+      </c>
+      <c r="D17" t="n">
         <v>0.2958579881656805</v>
       </c>
-      <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
+        <v>0.3663589015892664</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.4373934814137515</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.9435893404606556</v>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="n">
         <v>0.5938541250959626</v>
       </c>
-      <c r="F17" t="n">
-        <v>0.2958579881656805</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.7301775147928994</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.5938541250959626</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.2958579881656805</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0.7301775147928994</v>
-      </c>
       <c r="K17" t="n">
-        <v>0.5938541250959626</v>
+        <v>0.661357302381815</v>
       </c>
       <c r="L17" t="n">
         <v>0.2958579881656805</v>
       </c>
       <c r="M17" t="n">
-        <v>0.7301775147928994</v>
+        <v>0.3663589015892664</v>
       </c>
       <c r="N17" t="n">
-        <v>0.5938541250959626</v>
+        <v>0.4373934814137515</v>
       </c>
       <c r="O17" t="n">
-        <v>0.2958579881656805</v>
+        <v>0.9435893404606556</v>
       </c>
       <c r="P17" t="n">
         <v>0.7301775147928994</v>
       </c>
       <c r="Q17" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="R17" t="n">
         <v>0.5938541250959626</v>
       </c>
-      <c r="R17" t="n">
+      <c r="S17" t="n">
+        <v>0.661357302381815</v>
+      </c>
+      <c r="T17" t="n">
         <v>0.2958579881656805</v>
       </c>
-      <c r="S17" t="n">
+      <c r="U17" t="n">
+        <v>0.3663589015892664</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.4373934814137515</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0.9435893404606556</v>
+      </c>
+      <c r="X17" t="n">
         <v>0.7301775147928994</v>
       </c>
-      <c r="T17" t="n">
+      <c r="Y17" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="Z17" t="n">
         <v>0.5938541250959626</v>
       </c>
-      <c r="U17" t="n">
+      <c r="AA17" t="n">
+        <v>0.661357302381815</v>
+      </c>
+      <c r="AB17" t="n">
         <v>0.2958579881656805</v>
       </c>
-      <c r="V17" t="n">
+      <c r="AC17" t="n">
+        <v>0.3663589015892664</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>0.4373934814137515</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>0.9435893404606556</v>
+      </c>
+      <c r="AF17" t="n">
         <v>0.7301775147928994</v>
       </c>
-      <c r="W17" t="n">
+      <c r="AG17" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="AH17" t="n">
         <v>0.5938541250959626</v>
       </c>
-      <c r="X17" t="n">
+      <c r="AI17" t="n">
+        <v>0.661357302381815</v>
+      </c>
+      <c r="AJ17" t="n">
         <v>0.2958579881656805</v>
       </c>
-      <c r="Y17" t="n">
+      <c r="AK17" t="n">
+        <v>0.3663589015892664</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>0.4373934814137515</v>
+      </c>
+      <c r="AM17" t="n">
+        <v>0.9435893404606556</v>
+      </c>
+      <c r="AN17" t="n">
         <v>0.7301775147928994</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="AP17" t="n">
+        <v>0.5938541250959626</v>
+      </c>
+      <c r="AQ17" t="n">
+        <v>0.661357302381815</v>
+      </c>
+      <c r="AR17" t="n">
+        <v>0.2958579881656805</v>
+      </c>
+      <c r="AS17" t="n">
+        <v>0.3663589015892664</v>
+      </c>
+      <c r="AT17" t="n">
+        <v>0.4373934814137515</v>
+      </c>
+      <c r="AU17" t="n">
+        <v>0.9435893404606556</v>
+      </c>
+      <c r="AV17" t="n">
+        <v>0.7301775147928994</v>
+      </c>
+      <c r="AW17" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="AX17" t="n">
+        <v>0.5938541250959626</v>
+      </c>
+      <c r="AY17" t="n">
+        <v>0.661357302381815</v>
+      </c>
+      <c r="AZ17" t="n">
+        <v>0.2958579881656805</v>
+      </c>
+      <c r="BA17" t="n">
+        <v>0.3663589015892664</v>
+      </c>
+      <c r="BB17" t="n">
+        <v>0.4373934814137515</v>
+      </c>
+      <c r="BC17" t="n">
+        <v>0.9435893404606556</v>
+      </c>
+      <c r="BD17" t="n">
+        <v>0.7301775147928994</v>
+      </c>
+      <c r="BE17" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="BF17" t="n">
+        <v>0.5938541250959626</v>
+      </c>
+      <c r="BG17" t="n">
+        <v>0.661357302381815</v>
+      </c>
+      <c r="BH17" t="n">
+        <v>0.2958579881656805</v>
+      </c>
+      <c r="BI17" t="n">
+        <v>0.3663589015892664</v>
+      </c>
+      <c r="BJ17" t="n">
+        <v>0.4373934814137515</v>
+      </c>
+      <c r="BK17" t="n">
+        <v>0.9435893404606556</v>
+      </c>
+      <c r="BL17" t="n">
+        <v>0.7301775147928994</v>
+      </c>
+      <c r="BM17" t="n">
+        <v>0.9763313609467456</v>
       </c>
     </row>
     <row r="18">
@@ -1739,71 +3631,189 @@
         <v>0.6095880848048908</v>
       </c>
       <c r="C18" t="n">
+        <v>0.6608846749711658</v>
+      </c>
+      <c r="D18" t="n">
         <v>0.3005917159763314</v>
       </c>
-      <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
+        <v>0.3648799752862116</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.4367685536117434</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.9400267274585331</v>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="n">
         <v>0.6095880848048908</v>
       </c>
-      <c r="F18" t="n">
-        <v>0.3005917159763314</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.7325443786982249</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.6095880848048908</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0.3005917159763314</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.7325443786982249</v>
-      </c>
       <c r="K18" t="n">
-        <v>0.6095880848048908</v>
+        <v>0.6608846749711658</v>
       </c>
       <c r="L18" t="n">
         <v>0.3005917159763314</v>
       </c>
       <c r="M18" t="n">
-        <v>0.7325443786982249</v>
+        <v>0.3648799752862116</v>
       </c>
       <c r="N18" t="n">
-        <v>0.6095880848048908</v>
+        <v>0.4367685536117434</v>
       </c>
       <c r="O18" t="n">
-        <v>0.3005917159763314</v>
+        <v>0.9400267274585331</v>
       </c>
       <c r="P18" t="n">
         <v>0.7325443786982249</v>
       </c>
       <c r="Q18" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="R18" t="n">
         <v>0.6095880848048908</v>
       </c>
-      <c r="R18" t="n">
+      <c r="S18" t="n">
+        <v>0.6608846749711658</v>
+      </c>
+      <c r="T18" t="n">
         <v>0.3005917159763314</v>
       </c>
-      <c r="S18" t="n">
+      <c r="U18" t="n">
+        <v>0.3648799752862116</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0.4367685536117434</v>
+      </c>
+      <c r="W18" t="n">
+        <v>0.9400267274585331</v>
+      </c>
+      <c r="X18" t="n">
         <v>0.7325443786982249</v>
       </c>
-      <c r="T18" t="n">
+      <c r="Y18" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="Z18" t="n">
         <v>0.6095880848048908</v>
       </c>
-      <c r="U18" t="n">
+      <c r="AA18" t="n">
+        <v>0.6608846749711658</v>
+      </c>
+      <c r="AB18" t="n">
         <v>0.3005917159763314</v>
       </c>
-      <c r="V18" t="n">
+      <c r="AC18" t="n">
+        <v>0.3648799752862116</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>0.4367685536117434</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>0.9400267274585331</v>
+      </c>
+      <c r="AF18" t="n">
         <v>0.7325443786982249</v>
       </c>
-      <c r="W18" t="n">
+      <c r="AG18" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="AH18" t="n">
         <v>0.6095880848048908</v>
       </c>
-      <c r="X18" t="n">
+      <c r="AI18" t="n">
+        <v>0.6608846749711658</v>
+      </c>
+      <c r="AJ18" t="n">
         <v>0.3005917159763314</v>
       </c>
-      <c r="Y18" t="n">
+      <c r="AK18" t="n">
+        <v>0.3648799752862116</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>0.4367685536117434</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>0.9400267274585331</v>
+      </c>
+      <c r="AN18" t="n">
         <v>0.7325443786982249</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="AP18" t="n">
+        <v>0.6095880848048908</v>
+      </c>
+      <c r="AQ18" t="n">
+        <v>0.6608846749711658</v>
+      </c>
+      <c r="AR18" t="n">
+        <v>0.3005917159763314</v>
+      </c>
+      <c r="AS18" t="n">
+        <v>0.3648799752862116</v>
+      </c>
+      <c r="AT18" t="n">
+        <v>0.4367685536117434</v>
+      </c>
+      <c r="AU18" t="n">
+        <v>0.9400267274585331</v>
+      </c>
+      <c r="AV18" t="n">
+        <v>0.7325443786982249</v>
+      </c>
+      <c r="AW18" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="AX18" t="n">
+        <v>0.6095880848048908</v>
+      </c>
+      <c r="AY18" t="n">
+        <v>0.6608846749711658</v>
+      </c>
+      <c r="AZ18" t="n">
+        <v>0.3005917159763314</v>
+      </c>
+      <c r="BA18" t="n">
+        <v>0.3648799752862116</v>
+      </c>
+      <c r="BB18" t="n">
+        <v>0.4367685536117434</v>
+      </c>
+      <c r="BC18" t="n">
+        <v>0.9400267274585331</v>
+      </c>
+      <c r="BD18" t="n">
+        <v>0.7325443786982249</v>
+      </c>
+      <c r="BE18" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="BF18" t="n">
+        <v>0.6095880848048908</v>
+      </c>
+      <c r="BG18" t="n">
+        <v>0.6608846749711658</v>
+      </c>
+      <c r="BH18" t="n">
+        <v>0.3005917159763314</v>
+      </c>
+      <c r="BI18" t="n">
+        <v>0.3648799752862116</v>
+      </c>
+      <c r="BJ18" t="n">
+        <v>0.4367685536117434</v>
+      </c>
+      <c r="BK18" t="n">
+        <v>0.9400267274585331</v>
+      </c>
+      <c r="BL18" t="n">
+        <v>0.7325443786982249</v>
+      </c>
+      <c r="BM18" t="n">
+        <v>0.9692307692307692</v>
       </c>
     </row>
     <row r="19">
@@ -1816,71 +3826,189 @@
         <v>0.6027550161279918</v>
       </c>
       <c r="C19" t="n">
+        <v>0.6919515956109662</v>
+      </c>
+      <c r="D19" t="n">
         <v>0.2</v>
       </c>
-      <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
+        <v>0.3505817859045826</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.4787970106685621</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.9571040012577627</v>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="n">
         <v>0.6027550161279918</v>
       </c>
-      <c r="F19" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.8378698224852071</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.6027550161279918</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0.8378698224852071</v>
-      </c>
       <c r="K19" t="n">
-        <v>0.6027550161279918</v>
+        <v>0.6919515956109662</v>
       </c>
       <c r="L19" t="n">
         <v>0.2</v>
       </c>
       <c r="M19" t="n">
-        <v>0.8378698224852071</v>
+        <v>0.3505817859045826</v>
       </c>
       <c r="N19" t="n">
-        <v>0.6027550161279918</v>
+        <v>0.4787970106685621</v>
       </c>
       <c r="O19" t="n">
-        <v>0.2</v>
+        <v>0.9571040012577627</v>
       </c>
       <c r="P19" t="n">
         <v>0.8378698224852071</v>
       </c>
       <c r="Q19" t="n">
+        <v>0.9727810650887574</v>
+      </c>
+      <c r="R19" t="n">
         <v>0.6027550161279918</v>
       </c>
-      <c r="R19" t="n">
+      <c r="S19" t="n">
+        <v>0.6919515956109662</v>
+      </c>
+      <c r="T19" t="n">
         <v>0.2</v>
       </c>
-      <c r="S19" t="n">
+      <c r="U19" t="n">
+        <v>0.3505817859045826</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0.4787970106685621</v>
+      </c>
+      <c r="W19" t="n">
+        <v>0.9571040012577627</v>
+      </c>
+      <c r="X19" t="n">
         <v>0.8378698224852071</v>
       </c>
-      <c r="T19" t="n">
+      <c r="Y19" t="n">
+        <v>0.9727810650887574</v>
+      </c>
+      <c r="Z19" t="n">
         <v>0.6027550161279918</v>
       </c>
-      <c r="U19" t="n">
+      <c r="AA19" t="n">
+        <v>0.6919515956109662</v>
+      </c>
+      <c r="AB19" t="n">
         <v>0.2</v>
       </c>
-      <c r="V19" t="n">
+      <c r="AC19" t="n">
+        <v>0.3505817859045826</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>0.4787970106685621</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>0.9571040012577627</v>
+      </c>
+      <c r="AF19" t="n">
         <v>0.8378698224852071</v>
       </c>
-      <c r="W19" t="n">
+      <c r="AG19" t="n">
+        <v>0.9727810650887574</v>
+      </c>
+      <c r="AH19" t="n">
         <v>0.6027550161279918</v>
       </c>
-      <c r="X19" t="n">
+      <c r="AI19" t="n">
+        <v>0.6919515956109662</v>
+      </c>
+      <c r="AJ19" t="n">
         <v>0.2</v>
       </c>
-      <c r="Y19" t="n">
+      <c r="AK19" t="n">
+        <v>0.3505817859045826</v>
+      </c>
+      <c r="AL19" t="n">
+        <v>0.4787970106685621</v>
+      </c>
+      <c r="AM19" t="n">
+        <v>0.9571040012577627</v>
+      </c>
+      <c r="AN19" t="n">
         <v>0.8378698224852071</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>0.9727810650887574</v>
+      </c>
+      <c r="AP19" t="n">
+        <v>0.6027550161279918</v>
+      </c>
+      <c r="AQ19" t="n">
+        <v>0.6919515956109662</v>
+      </c>
+      <c r="AR19" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AS19" t="n">
+        <v>0.3505817859045826</v>
+      </c>
+      <c r="AT19" t="n">
+        <v>0.4787970106685621</v>
+      </c>
+      <c r="AU19" t="n">
+        <v>0.9571040012577627</v>
+      </c>
+      <c r="AV19" t="n">
+        <v>0.8378698224852071</v>
+      </c>
+      <c r="AW19" t="n">
+        <v>0.9727810650887574</v>
+      </c>
+      <c r="AX19" t="n">
+        <v>0.6027550161279918</v>
+      </c>
+      <c r="AY19" t="n">
+        <v>0.6919515956109662</v>
+      </c>
+      <c r="AZ19" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BA19" t="n">
+        <v>0.3505817859045826</v>
+      </c>
+      <c r="BB19" t="n">
+        <v>0.4787970106685621</v>
+      </c>
+      <c r="BC19" t="n">
+        <v>0.9571040012577627</v>
+      </c>
+      <c r="BD19" t="n">
+        <v>0.8378698224852071</v>
+      </c>
+      <c r="BE19" t="n">
+        <v>0.9727810650887574</v>
+      </c>
+      <c r="BF19" t="n">
+        <v>0.6027550161279918</v>
+      </c>
+      <c r="BG19" t="n">
+        <v>0.6919515956109662</v>
+      </c>
+      <c r="BH19" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BI19" t="n">
+        <v>0.3505817859045826</v>
+      </c>
+      <c r="BJ19" t="n">
+        <v>0.4787970106685621</v>
+      </c>
+      <c r="BK19" t="n">
+        <v>0.9571040012577627</v>
+      </c>
+      <c r="BL19" t="n">
+        <v>0.8378698224852071</v>
+      </c>
+      <c r="BM19" t="n">
+        <v>0.9727810650887574</v>
       </c>
     </row>
     <row r="20">
@@ -1893,71 +4021,189 @@
         <v>0.5317553841367666</v>
       </c>
       <c r="C20" t="n">
+        <v>0.6138490378095712</v>
+      </c>
+      <c r="D20" t="n">
         <v>0.3882510321476291</v>
       </c>
-      <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
+        <v>0.4121357438145184</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.3768106412197364</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.9684710321515604</v>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="n">
         <v>0.565266863719195</v>
       </c>
-      <c r="F20" t="n">
+      <c r="K20" t="n">
+        <v>0.6786384329859394</v>
+      </c>
+      <c r="L20" t="n">
         <v>0.2840236686390533</v>
       </c>
-      <c r="G20" t="n">
+      <c r="M20" t="n">
+        <v>0.3737183070107226</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.4605501227256114</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.9476236144957157</v>
+      </c>
+      <c r="P20" t="n">
         <v>0.7325443786982249</v>
       </c>
-      <c r="H20" t="n">
+      <c r="Q20" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="R20" t="n">
         <v>0.565266863719195</v>
       </c>
-      <c r="I20" t="n">
+      <c r="S20" t="n">
+        <v>0.6786384329859394</v>
+      </c>
+      <c r="T20" t="n">
         <v>0.2840236686390533</v>
       </c>
-      <c r="J20" t="n">
+      <c r="U20" t="n">
+        <v>0.3737183070107226</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0.4605501227256114</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0.9476236144957157</v>
+      </c>
+      <c r="X20" t="n">
         <v>0.7325443786982249</v>
       </c>
-      <c r="K20" t="n">
+      <c r="Y20" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="Z20" t="n">
         <v>0.5704768066996664</v>
       </c>
-      <c r="L20" t="n">
+      <c r="AA20" t="n">
+        <v>0.685260114959152</v>
+      </c>
+      <c r="AB20" t="n">
         <v>0.285207100591716</v>
       </c>
-      <c r="M20" t="n">
+      <c r="AC20" t="n">
+        <v>0.380279334372393</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>0.4695814251538302</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>0.9411807247857873</v>
+      </c>
+      <c r="AF20" t="n">
         <v>0.7337278106508875</v>
       </c>
-      <c r="N20" t="n">
+      <c r="AG20" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="AH20" t="n">
         <v>0.5589508346026139</v>
       </c>
-      <c r="O20" t="n">
+      <c r="AI20" t="n">
+        <v>0.6835609480856952</v>
+      </c>
+      <c r="AJ20" t="n">
         <v>0.272189349112426</v>
       </c>
-      <c r="P20" t="n">
+      <c r="AK20" t="n">
+        <v>0.3784105788023592</v>
+      </c>
+      <c r="AL20" t="n">
+        <v>0.4672555697478145</v>
+      </c>
+      <c r="AM20" t="n">
+        <v>0.9435264523229306</v>
+      </c>
+      <c r="AN20" t="n">
         <v>0.7467455621301775</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="AO20" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="AP20" t="n">
         <v>0.565266863719195</v>
       </c>
-      <c r="R20" t="n">
+      <c r="AQ20" t="n">
+        <v>0.6786384329859394</v>
+      </c>
+      <c r="AR20" t="n">
         <v>0.2840236686390533</v>
       </c>
-      <c r="S20" t="n">
+      <c r="AS20" t="n">
+        <v>0.3737183070107226</v>
+      </c>
+      <c r="AT20" t="n">
+        <v>0.4605501227256114</v>
+      </c>
+      <c r="AU20" t="n">
+        <v>0.9476236144957157</v>
+      </c>
+      <c r="AV20" t="n">
         <v>0.7325443786982249</v>
       </c>
-      <c r="T20" t="n">
+      <c r="AW20" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="AX20" t="n">
         <v>0.5600084530215783</v>
       </c>
-      <c r="U20" t="n">
+      <c r="AY20" t="n">
+        <v>0.6712728627684483</v>
+      </c>
+      <c r="AZ20" t="n">
         <v>0.2733727810650888</v>
       </c>
-      <c r="V20" t="n">
+      <c r="BA20" t="n">
+        <v>0.3617622653438928</v>
+      </c>
+      <c r="BB20" t="n">
+        <v>0.4506072562893481</v>
+      </c>
+      <c r="BC20" t="n">
+        <v>0.9463752849618741</v>
+      </c>
+      <c r="BD20" t="n">
         <v>0.7455621301775148</v>
       </c>
-      <c r="W20" t="n">
+      <c r="BE20" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="BF20" t="n">
         <v>0.5642191021813</v>
       </c>
-      <c r="X20" t="n">
+      <c r="BG20" t="n">
+        <v>0.6839050472811407</v>
+      </c>
+      <c r="BH20" t="n">
         <v>0.2781065088757396</v>
       </c>
-      <c r="Y20" t="n">
+      <c r="BI20" t="n">
+        <v>0.378881122751164</v>
+      </c>
+      <c r="BJ20" t="n">
+        <v>0.4677261136966193</v>
+      </c>
+      <c r="BK20" t="n">
+        <v>0.9432088672274193</v>
+      </c>
+      <c r="BL20" t="n">
         <v>0.7408284023668639</v>
+      </c>
+      <c r="BM20" t="n">
+        <v>0.9822485207100592</v>
       </c>
     </row>
     <row r="21">
@@ -1967,74 +4213,192 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.5417482111279694</v>
+        <v>0.5621177201983111</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2414201183431953</v>
-      </c>
-      <c r="D21" t="inlineStr"/>
+        <v>0.6535159627964467</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.2662721893491125</v>
+      </c>
       <c r="E21" t="n">
-        <v>0.5417482111279694</v>
+        <v>0.3586532500000599</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2414201183431953</v>
+        <v>0.4270831136297668</v>
       </c>
       <c r="G21" t="n">
-        <v>0.7834319526627219</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.5417482111279694</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0.2414201183431953</v>
-      </c>
+        <v>0.9489379765741687</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="n">
-        <v>0.7834319526627219</v>
+        <v>0.5621177201983111</v>
       </c>
       <c r="K21" t="n">
-        <v>0.5417482111279694</v>
+        <v>0.6535159627964467</v>
       </c>
       <c r="L21" t="n">
-        <v>0.2414201183431953</v>
+        <v>0.2662721893491125</v>
       </c>
       <c r="M21" t="n">
-        <v>0.7834319526627219</v>
+        <v>0.3586532500000599</v>
       </c>
       <c r="N21" t="n">
-        <v>0.5417482111279694</v>
+        <v>0.4270831136297668</v>
       </c>
       <c r="O21" t="n">
-        <v>0.2414201183431953</v>
+        <v>0.9489379765741687</v>
       </c>
       <c r="P21" t="n">
-        <v>0.7834319526627219</v>
+        <v>0.757396449704142</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.5417482111279694</v>
+        <v>0.9775147928994082</v>
       </c>
       <c r="R21" t="n">
-        <v>0.2414201183431953</v>
+        <v>0.5621177201983111</v>
       </c>
       <c r="S21" t="n">
-        <v>0.7834319526627219</v>
+        <v>0.6535159627964467</v>
       </c>
       <c r="T21" t="n">
-        <v>0.5417482111279694</v>
+        <v>0.2662721893491125</v>
       </c>
       <c r="U21" t="n">
-        <v>0.2414201183431953</v>
+        <v>0.3586532500000599</v>
       </c>
       <c r="V21" t="n">
-        <v>0.7834319526627219</v>
+        <v>0.4270831136297668</v>
       </c>
       <c r="W21" t="n">
-        <v>0.5417482111279694</v>
+        <v>0.9489379765741687</v>
       </c>
       <c r="X21" t="n">
-        <v>0.2414201183431953</v>
+        <v>0.757396449704142</v>
       </c>
       <c r="Y21" t="n">
-        <v>0.7834319526627219</v>
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0.5621177201983111</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>0.6535159627964467</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>0.2662721893491125</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>0.3586532500000599</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>0.4270831136297668</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>0.9489379765741687</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>0.757396449704142</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>0.5621177201983111</v>
+      </c>
+      <c r="AI21" t="n">
+        <v>0.6535159627964467</v>
+      </c>
+      <c r="AJ21" t="n">
+        <v>0.2662721893491125</v>
+      </c>
+      <c r="AK21" t="n">
+        <v>0.3586532500000599</v>
+      </c>
+      <c r="AL21" t="n">
+        <v>0.4270831136297668</v>
+      </c>
+      <c r="AM21" t="n">
+        <v>0.9489379765741687</v>
+      </c>
+      <c r="AN21" t="n">
+        <v>0.757396449704142</v>
+      </c>
+      <c r="AO21" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="AP21" t="n">
+        <v>0.5621177201983111</v>
+      </c>
+      <c r="AQ21" t="n">
+        <v>0.6535159627964467</v>
+      </c>
+      <c r="AR21" t="n">
+        <v>0.2662721893491125</v>
+      </c>
+      <c r="AS21" t="n">
+        <v>0.3586532500000599</v>
+      </c>
+      <c r="AT21" t="n">
+        <v>0.4270831136297668</v>
+      </c>
+      <c r="AU21" t="n">
+        <v>0.9489379765741687</v>
+      </c>
+      <c r="AV21" t="n">
+        <v>0.757396449704142</v>
+      </c>
+      <c r="AW21" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="AX21" t="n">
+        <v>0.5621177201983111</v>
+      </c>
+      <c r="AY21" t="n">
+        <v>0.6535159627964467</v>
+      </c>
+      <c r="AZ21" t="n">
+        <v>0.2662721893491125</v>
+      </c>
+      <c r="BA21" t="n">
+        <v>0.3586532500000599</v>
+      </c>
+      <c r="BB21" t="n">
+        <v>0.4270831136297668</v>
+      </c>
+      <c r="BC21" t="n">
+        <v>0.9489379765741687</v>
+      </c>
+      <c r="BD21" t="n">
+        <v>0.757396449704142</v>
+      </c>
+      <c r="BE21" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="BF21" t="n">
+        <v>0.5621177201983111</v>
+      </c>
+      <c r="BG21" t="n">
+        <v>0.6535159627964467</v>
+      </c>
+      <c r="BH21" t="n">
+        <v>0.2662721893491125</v>
+      </c>
+      <c r="BI21" t="n">
+        <v>0.3586532500000599</v>
+      </c>
+      <c r="BJ21" t="n">
+        <v>0.4270831136297668</v>
+      </c>
+      <c r="BK21" t="n">
+        <v>0.9489379765741687</v>
+      </c>
+      <c r="BL21" t="n">
+        <v>0.757396449704142</v>
+      </c>
+      <c r="BM21" t="n">
+        <v>0.9775147928994082</v>
       </c>
     </row>
     <row r="22">
@@ -2044,86 +4408,204 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.5307134864818566</v>
+        <v>0.6305815855975138</v>
       </c>
       <c r="C22" t="n">
-        <v>0.2248520710059172</v>
-      </c>
-      <c r="D22" t="inlineStr"/>
+        <v>0.6276893301377549</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.3431952662721893</v>
+      </c>
       <c r="E22" t="n">
-        <v>0.5318272620751878</v>
+        <v>0.3576477345855125</v>
       </c>
       <c r="F22" t="n">
-        <v>0.2260355029585799</v>
+        <v>0.3939938951687834</v>
       </c>
       <c r="G22" t="n">
-        <v>0.7988165680473372</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0.5318272620751878</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0.2260355029585799</v>
-      </c>
+        <v>0.9381432277336688</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="n">
-        <v>0.7988165680473372</v>
+        <v>0.6305815855975138</v>
       </c>
       <c r="K22" t="n">
-        <v>0.5318272620751878</v>
+        <v>0.6276893301377549</v>
       </c>
       <c r="L22" t="n">
-        <v>0.2260355029585799</v>
+        <v>0.3431952662721893</v>
       </c>
       <c r="M22" t="n">
-        <v>0.7988165680473372</v>
+        <v>0.3576477345855125</v>
       </c>
       <c r="N22" t="n">
-        <v>0.5318272620751878</v>
+        <v>0.3939938951687834</v>
       </c>
       <c r="O22" t="n">
-        <v>0.2260355029585799</v>
+        <v>0.9381432277336688</v>
       </c>
       <c r="P22" t="n">
-        <v>0.7988165680473372</v>
+        <v>0.6816568047337278</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.5318272620751878</v>
+        <v>0.9775147928994082</v>
       </c>
       <c r="R22" t="n">
-        <v>0.2260355029585799</v>
+        <v>0.6305815855975138</v>
       </c>
       <c r="S22" t="n">
-        <v>0.7988165680473372</v>
+        <v>0.6276893301377549</v>
       </c>
       <c r="T22" t="n">
-        <v>0.5318272620751878</v>
+        <v>0.3431952662721893</v>
       </c>
       <c r="U22" t="n">
-        <v>0.2260355029585799</v>
+        <v>0.3576477345855125</v>
       </c>
       <c r="V22" t="n">
-        <v>0.7988165680473372</v>
+        <v>0.3939938951687834</v>
       </c>
       <c r="W22" t="n">
-        <v>0.5318272620751878</v>
+        <v>0.9381432277336688</v>
       </c>
       <c r="X22" t="n">
-        <v>0.2260355029585799</v>
+        <v>0.6816568047337278</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.7988165680473372</v>
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>0.6305815855975138</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>0.6276893301377549</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>0.3431952662721893</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>0.3576477345855125</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>0.3939938951687834</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>0.9381432277336688</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>0.6816568047337278</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>0.6305815855975138</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>0.6276893301377549</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>0.3431952662721893</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>0.3576477345855125</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>0.3939938951687834</v>
+      </c>
+      <c r="AM22" t="n">
+        <v>0.9381432277336688</v>
+      </c>
+      <c r="AN22" t="n">
+        <v>0.6816568047337278</v>
+      </c>
+      <c r="AO22" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="AP22" t="n">
+        <v>0.6305815855975138</v>
+      </c>
+      <c r="AQ22" t="n">
+        <v>0.6276893301377549</v>
+      </c>
+      <c r="AR22" t="n">
+        <v>0.3431952662721893</v>
+      </c>
+      <c r="AS22" t="n">
+        <v>0.3576477345855125</v>
+      </c>
+      <c r="AT22" t="n">
+        <v>0.3939938951687834</v>
+      </c>
+      <c r="AU22" t="n">
+        <v>0.9381432277336688</v>
+      </c>
+      <c r="AV22" t="n">
+        <v>0.6816568047337278</v>
+      </c>
+      <c r="AW22" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="AX22" t="n">
+        <v>0.6305815855975138</v>
+      </c>
+      <c r="AY22" t="n">
+        <v>0.6276893301377549</v>
+      </c>
+      <c r="AZ22" t="n">
+        <v>0.3431952662721893</v>
+      </c>
+      <c r="BA22" t="n">
+        <v>0.3576477345855125</v>
+      </c>
+      <c r="BB22" t="n">
+        <v>0.3939938951687834</v>
+      </c>
+      <c r="BC22" t="n">
+        <v>0.9381432277336688</v>
+      </c>
+      <c r="BD22" t="n">
+        <v>0.6816568047337278</v>
+      </c>
+      <c r="BE22" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="BF22" t="n">
+        <v>0.6305815855975138</v>
+      </c>
+      <c r="BG22" t="n">
+        <v>0.6276893301377549</v>
+      </c>
+      <c r="BH22" t="n">
+        <v>0.3431952662721893</v>
+      </c>
+      <c r="BI22" t="n">
+        <v>0.3576477345855125</v>
+      </c>
+      <c r="BJ22" t="n">
+        <v>0.3939938951687834</v>
+      </c>
+      <c r="BK22" t="n">
+        <v>0.9381432277336688</v>
+      </c>
+      <c r="BL22" t="n">
+        <v>0.6816568047337278</v>
+      </c>
+      <c r="BM22" t="n">
+        <v>0.9775147928994082</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="AP1:AW1"/>
+    <mergeCell ref="R1:Y1"/>
+    <mergeCell ref="Z1:AG1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="AX1:BE1"/>
+    <mergeCell ref="AH1:AO1"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="BF1:BM1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
plots and metrics fixes (#13)
</commit_message>
<xml_diff>
--- a/training/results/results_test.xlsx
+++ b/training/results/results_test.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y22"/>
+  <dimension ref="A1:BM22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,55 +474,95 @@
       </c>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>round 0.5</t>
-        </is>
-      </c>
+      <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
       <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>best_single_threshold_0.05_0.95</t>
-        </is>
-      </c>
+      <c r="H1" s="1" t="n"/>
       <c r="I1" s="1" t="n"/>
-      <c r="J1" s="1" t="n"/>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>best_multiple_thresholds_0.05_0.95</t>
-        </is>
-      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>round 0.5</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="n"/>
       <c r="L1" s="1" t="n"/>
       <c r="M1" s="1" t="n"/>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>best_graph_thresholds_0.05_0.95</t>
-        </is>
-      </c>
+      <c r="N1" s="1" t="n"/>
       <c r="O1" s="1" t="n"/>
       <c r="P1" s="1" t="n"/>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>best_single_threshold_0.25_0.75</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="n"/>
+      <c r="Q1" s="1" t="n"/>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>best_single_threshold_0.05_0.95</t>
+        </is>
+      </c>
       <c r="S1" s="1" t="n"/>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>best_multiple_thresholds_0.25_0.75</t>
-        </is>
-      </c>
+      <c r="T1" s="1" t="n"/>
       <c r="U1" s="1" t="n"/>
       <c r="V1" s="1" t="n"/>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>best_graph_thresholds_0.25_0.75</t>
-        </is>
-      </c>
+      <c r="W1" s="1" t="n"/>
       <c r="X1" s="1" t="n"/>
       <c r="Y1" s="1" t="n"/>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>best_multiple_thresholds_0.05_0.95</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="n"/>
+      <c r="AB1" s="1" t="n"/>
+      <c r="AC1" s="1" t="n"/>
+      <c r="AD1" s="1" t="n"/>
+      <c r="AE1" s="1" t="n"/>
+      <c r="AF1" s="1" t="n"/>
+      <c r="AG1" s="1" t="n"/>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>best_graph_thresholds_0.05_0.95</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="n"/>
+      <c r="AJ1" s="1" t="n"/>
+      <c r="AK1" s="1" t="n"/>
+      <c r="AL1" s="1" t="n"/>
+      <c r="AM1" s="1" t="n"/>
+      <c r="AN1" s="1" t="n"/>
+      <c r="AO1" s="1" t="n"/>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>best_single_threshold_0.25_0.75</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="n"/>
+      <c r="AR1" s="1" t="n"/>
+      <c r="AS1" s="1" t="n"/>
+      <c r="AT1" s="1" t="n"/>
+      <c r="AU1" s="1" t="n"/>
+      <c r="AV1" s="1" t="n"/>
+      <c r="AW1" s="1" t="n"/>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>best_multiple_thresholds_0.25_0.75</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="n"/>
+      <c r="AZ1" s="1" t="n"/>
+      <c r="BA1" s="1" t="n"/>
+      <c r="BB1" s="1" t="n"/>
+      <c r="BC1" s="1" t="n"/>
+      <c r="BD1" s="1" t="n"/>
+      <c r="BE1" s="1" t="n"/>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>best_graph_thresholds_0.25_0.75</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="n"/>
+      <c r="BH1" s="1" t="n"/>
+      <c r="BI1" s="1" t="n"/>
+      <c r="BJ1" s="1" t="n"/>
+      <c r="BK1" s="1" t="n"/>
+      <c r="BL1" s="1" t="n"/>
+      <c r="BM1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -537,117 +577,317 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="D2" s="1" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
         <is>
           <t>rmse</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="N2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="O2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="H2" s="1" t="inlineStr">
+      <c r="Q2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
+        </is>
+      </c>
+      <c r="R2" s="1" t="inlineStr">
         <is>
           <t>rmse</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="S2" s="1" t="inlineStr">
+        <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="T2" s="1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="U2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="V2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="W2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="X2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="Y2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
+        </is>
+      </c>
+      <c r="Z2" s="1" t="inlineStr">
         <is>
           <t>rmse</t>
         </is>
       </c>
-      <c r="L2" s="1" t="inlineStr">
+      <c r="AA2" s="1" t="inlineStr">
+        <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AB2" s="1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="M2" s="1" t="inlineStr">
+      <c r="AC2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AD2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AE2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="AF2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="N2" s="1" t="inlineStr">
+      <c r="AG2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
+        </is>
+      </c>
+      <c r="AH2" s="1" t="inlineStr">
         <is>
           <t>rmse</t>
         </is>
       </c>
-      <c r="O2" s="1" t="inlineStr">
+      <c r="AI2" s="1" t="inlineStr">
+        <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AJ2" s="1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="P2" s="1" t="inlineStr">
+      <c r="AK2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AL2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AM2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="AN2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="Q2" s="1" t="inlineStr">
+      <c r="AO2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
+        </is>
+      </c>
+      <c r="AP2" s="1" t="inlineStr">
         <is>
           <t>rmse</t>
         </is>
       </c>
-      <c r="R2" s="1" t="inlineStr">
+      <c r="AQ2" s="1" t="inlineStr">
+        <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AR2" s="1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="S2" s="1" t="inlineStr">
+      <c r="AS2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AT2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AU2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="AV2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="T2" s="1" t="inlineStr">
+      <c r="AW2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
+        </is>
+      </c>
+      <c r="AX2" s="1" t="inlineStr">
         <is>
           <t>rmse</t>
         </is>
       </c>
-      <c r="U2" s="1" t="inlineStr">
+      <c r="AY2" s="1" t="inlineStr">
+        <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="AZ2" s="1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="V2" s="1" t="inlineStr">
+      <c r="BA2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="BB2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="BC2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="BD2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="W2" s="1" t="inlineStr">
+      <c r="BE2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
+        </is>
+      </c>
+      <c r="BF2" s="1" t="inlineStr">
         <is>
           <t>rmse</t>
         </is>
       </c>
-      <c r="X2" s="1" t="inlineStr">
+      <c r="BG2" s="1" t="inlineStr">
+        <is>
+          <t>rmse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="BH2" s="1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="Y2" s="1" t="inlineStr">
+      <c r="BI2" s="1" t="inlineStr">
+        <is>
+          <t>mae_macroaveraged</t>
+        </is>
+      </c>
+      <c r="BJ2" s="1" t="inlineStr">
+        <is>
+          <t>mse_macroaveraged</t>
+        </is>
+      </c>
+      <c r="BK2" s="1" t="inlineStr">
+        <is>
+          <t>somers_d</t>
+        </is>
+      </c>
+      <c r="BL2" s="1" t="inlineStr">
         <is>
           <t>accuracy</t>
+        </is>
+      </c>
+      <c r="BM2" s="1" t="inlineStr">
+        <is>
+          <t>accuracy1</t>
         </is>
       </c>
     </row>
@@ -661,71 +901,189 @@
         <v>0.6091792271036202</v>
       </c>
       <c r="C4" t="n">
+        <v>0.6180943735427414</v>
+      </c>
+      <c r="D4" t="n">
         <v>0.4525010110345065</v>
       </c>
-      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
+        <v>0.4229372878062176</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.382040654605194</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9589937897963997</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="n">
         <v>0.6398964413257052</v>
       </c>
-      <c r="F4" t="n">
+      <c r="K4" t="n">
+        <v>0.6897246274071355</v>
+      </c>
+      <c r="L4" t="n">
         <v>0.3668639053254438</v>
       </c>
-      <c r="G4" t="n">
+      <c r="M4" t="n">
+        <v>0.4112758128214844</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.4757200616519119</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.9324204072006917</v>
+      </c>
+      <c r="P4" t="n">
         <v>0.6520710059171597</v>
       </c>
-      <c r="H4" t="n">
+      <c r="Q4" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="R4" t="n">
         <v>0.6305815855975138</v>
       </c>
-      <c r="I4" t="n">
+      <c r="S4" t="n">
+        <v>0.6980139893804611</v>
+      </c>
+      <c r="T4" t="n">
         <v>0.3526627218934911</v>
       </c>
-      <c r="J4" t="n">
+      <c r="U4" t="n">
+        <v>0.4218919690940813</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.4872235293708265</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.9350522757644839</v>
+      </c>
+      <c r="X4" t="n">
         <v>0.6674556213017752</v>
       </c>
-      <c r="K4" t="n">
+      <c r="Y4" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="Z4" t="n">
         <v>0.6211270534826568</v>
       </c>
-      <c r="L4" t="n">
+      <c r="AA4" t="n">
+        <v>0.6846156109421431</v>
+      </c>
+      <c r="AB4" t="n">
         <v>0.3455621301775148</v>
       </c>
-      <c r="M4" t="n">
+      <c r="AC4" t="n">
+        <v>0.4034110711589981</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.4686985347456838</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0.9374891911013286</v>
+      </c>
+      <c r="AF4" t="n">
         <v>0.672189349112426</v>
       </c>
-      <c r="N4" t="n">
+      <c r="AG4" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="AH4" t="n">
         <v>0.6285043968726759</v>
       </c>
-      <c r="O4" t="n">
+      <c r="AI4" t="n">
+        <v>0.6555004004061831</v>
+      </c>
+      <c r="AJ4" t="n">
         <v>0.3459519297887649</v>
       </c>
-      <c r="P4" t="n">
+      <c r="AK4" t="n">
+        <v>0.3655255744097044</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>0.4296807749326664</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0.9368131436207845</v>
+      </c>
+      <c r="AN4" t="n">
         <v>0.676923076923077</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="AO4" t="n">
+        <v>0.9798816568047337</v>
+      </c>
+      <c r="AP4" t="n">
         <v>0.6305815855975138</v>
       </c>
-      <c r="R4" t="n">
+      <c r="AQ4" t="n">
+        <v>0.6980139893804611</v>
+      </c>
+      <c r="AR4" t="n">
         <v>0.3526627218934911</v>
       </c>
-      <c r="S4" t="n">
+      <c r="AS4" t="n">
+        <v>0.4218919690940813</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>0.4872235293708265</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>0.9350522757644839</v>
+      </c>
+      <c r="AV4" t="n">
         <v>0.6674556213017752</v>
       </c>
-      <c r="T4" t="n">
+      <c r="AW4" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="AX4" t="n">
         <v>0.6249260311258431</v>
       </c>
-      <c r="U4" t="n">
+      <c r="AY4" t="n">
+        <v>0.7074948935350311</v>
+      </c>
+      <c r="AZ4" t="n">
         <v>0.3408284023668639</v>
       </c>
-      <c r="V4" t="n">
+      <c r="BA4" t="n">
+        <v>0.4071799281383982</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>0.5005490243781451</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>0.937269082619291</v>
+      </c>
+      <c r="BD4" t="n">
         <v>0.6804733727810651</v>
       </c>
-      <c r="W4" t="n">
+      <c r="BE4" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="BF4" t="n">
         <v>0.6180615061698925</v>
       </c>
-      <c r="X4" t="n">
+      <c r="BG4" t="n">
+        <v>0.6549281273710738</v>
+      </c>
+      <c r="BH4" t="n">
         <v>0.3400347700254513</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="BI4" t="n">
+        <v>0.3664701543441086</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>0.4289308520217814</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>0.93805832874774</v>
+      </c>
+      <c r="BL4" t="n">
         <v>0.6792899408284023</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>0.9834319526627219</v>
       </c>
     </row>
     <row r="5">
@@ -738,71 +1096,189 @@
         <v>0.6066834765467946</v>
       </c>
       <c r="C5" t="n">
+        <v>0.6152599750840554</v>
+      </c>
+      <c r="D5" t="n">
         <v>0.4506175590769879</v>
       </c>
-      <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
+        <v>0.4221831108424272</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.3785448369404324</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.9593962738778398</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="n">
         <v>0.633390426161197</v>
       </c>
-      <c r="F5" t="n">
+      <c r="K5" t="n">
+        <v>0.6873351266204395</v>
+      </c>
+      <c r="L5" t="n">
         <v>0.3538461538461539</v>
       </c>
-      <c r="G5" t="n">
+      <c r="M5" t="n">
+        <v>0.406594023108082</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.4724295762863355</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.9349233550821476</v>
+      </c>
+      <c r="P5" t="n">
         <v>0.6662721893491125</v>
       </c>
-      <c r="H5" t="n">
+      <c r="Q5" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="R5" t="n">
         <v>0.633390426161197</v>
       </c>
-      <c r="I5" t="n">
+      <c r="S5" t="n">
+        <v>0.6873351266204395</v>
+      </c>
+      <c r="T5" t="n">
         <v>0.3538461538461539</v>
       </c>
-      <c r="J5" t="n">
+      <c r="U5" t="n">
+        <v>0.406594023108082</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.4724295762863355</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.9349233550821476</v>
+      </c>
+      <c r="X5" t="n">
         <v>0.6662721893491125</v>
       </c>
-      <c r="K5" t="n">
+      <c r="Y5" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="Z5" t="n">
         <v>0.6296425209132654</v>
       </c>
-      <c r="L5" t="n">
+      <c r="AA5" t="n">
+        <v>0.6820468087494997</v>
+      </c>
+      <c r="AB5" t="n">
         <v>0.3467455621301775</v>
       </c>
-      <c r="M5" t="n">
+      <c r="AC5" t="n">
+        <v>0.4310293147806636</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0.4651878493253767</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0.9356905903623929</v>
+      </c>
+      <c r="AF5" t="n">
         <v>0.6745562130177515</v>
       </c>
-      <c r="N5" t="n">
+      <c r="AG5" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="AH5" t="n">
         <v>0.609428793653878</v>
       </c>
-      <c r="O5" t="n">
+      <c r="AI5" t="n">
+        <v>0.6378425507108177</v>
+      </c>
+      <c r="AJ5" t="n">
         <v>0.3245061253572235</v>
       </c>
-      <c r="P5" t="n">
+      <c r="AK5" t="n">
+        <v>0.3441856572589514</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>0.4068431194972821</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>0.9393003694678091</v>
+      </c>
+      <c r="AN5" t="n">
         <v>0.6970414201183432</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="AO5" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="AP5" t="n">
         <v>0.633390426161197</v>
       </c>
-      <c r="R5" t="n">
+      <c r="AQ5" t="n">
+        <v>0.6873351266204395</v>
+      </c>
+      <c r="AR5" t="n">
         <v>0.3538461538461539</v>
       </c>
-      <c r="S5" t="n">
+      <c r="AS5" t="n">
+        <v>0.406594023108082</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0.4724295762863355</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.9349233550821476</v>
+      </c>
+      <c r="AV5" t="n">
         <v>0.6662721893491125</v>
       </c>
-      <c r="T5" t="n">
+      <c r="AW5" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="AX5" t="n">
         <v>0.6124932073044426</v>
       </c>
-      <c r="U5" t="n">
+      <c r="AY5" t="n">
+        <v>0.7074082302333098</v>
+      </c>
+      <c r="AZ5" t="n">
         <v>0.3325443786982248</v>
       </c>
-      <c r="V5" t="n">
+      <c r="BA5" t="n">
+        <v>0.4051866051659079</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>0.5004264042018234</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>0.9362943164845531</v>
+      </c>
+      <c r="BD5" t="n">
         <v>0.6863905325443787</v>
       </c>
-      <c r="W5" t="n">
+      <c r="BE5" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="BF5" t="n">
         <v>0.607483819232328</v>
       </c>
-      <c r="X5" t="n">
+      <c r="BG5" t="n">
+        <v>0.6378968439854098</v>
+      </c>
+      <c r="BH5" t="n">
         <v>0.3292398531678744</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="BI5" t="n">
+        <v>0.3463418778499546</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>0.4069123835665462</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>0.9393695464193067</v>
+      </c>
+      <c r="BL5" t="n">
         <v>0.6887573964497041</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>0.9846153846153847</v>
       </c>
     </row>
     <row r="6">
@@ -815,71 +1291,189 @@
         <v>0.6085150377211097</v>
       </c>
       <c r="C6" t="n">
+        <v>0.6204683456581611</v>
+      </c>
+      <c r="D6" t="n">
         <v>0.4502765917298872</v>
       </c>
-      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
+        <v>0.4199647361246967</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.3849809679637752</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.9591981762440059</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="n">
         <v>0.6324555320336759</v>
       </c>
-      <c r="F6" t="n">
+      <c r="K6" t="n">
+        <v>0.6835764481668571</v>
+      </c>
+      <c r="L6" t="n">
         <v>0.3502958579881657</v>
       </c>
-      <c r="G6" t="n">
+      <c r="M6" t="n">
+        <v>0.3960064247014668</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.467276760488416</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.9345554594764562</v>
+      </c>
+      <c r="P6" t="n">
         <v>0.6710059171597633</v>
       </c>
-      <c r="H6" t="n">
+      <c r="Q6" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="R6" t="n">
         <v>0.6324555320336759</v>
       </c>
-      <c r="I6" t="n">
+      <c r="S6" t="n">
+        <v>0.6835764481668571</v>
+      </c>
+      <c r="T6" t="n">
         <v>0.3502958579881657</v>
       </c>
-      <c r="J6" t="n">
+      <c r="U6" t="n">
+        <v>0.3960064247014668</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.467276760488416</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.9345554594764562</v>
+      </c>
+      <c r="X6" t="n">
         <v>0.6710059171597633</v>
       </c>
-      <c r="K6" t="n">
+      <c r="Y6" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="Z6" t="n">
         <v>0.6590292304801199</v>
       </c>
-      <c r="L6" t="n">
+      <c r="AA6" t="n">
+        <v>0.6994182038983934</v>
+      </c>
+      <c r="AB6" t="n">
         <v>0.3775147928994083</v>
       </c>
-      <c r="M6" t="n">
+      <c r="AC6" t="n">
+        <v>0.4158129855424297</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0.4891858239444546</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0.9273987894033487</v>
+      </c>
+      <c r="AF6" t="n">
         <v>0.6473372781065089</v>
       </c>
-      <c r="N6" t="n">
+      <c r="AG6" t="n">
+        <v>0.978698224852071</v>
+      </c>
+      <c r="AH6" t="n">
         <v>0.6250427483072962</v>
       </c>
-      <c r="O6" t="n">
+      <c r="AI6" t="n">
+        <v>0.6355583406062126</v>
+      </c>
+      <c r="AJ6" t="n">
         <v>0.3341675035415116</v>
       </c>
-      <c r="P6" t="n">
+      <c r="AK6" t="n">
+        <v>0.3359340598600982</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0.4039344043141225</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.9370080968477321</v>
+      </c>
+      <c r="AN6" t="n">
         <v>0.6923076923076923</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="AO6" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="AP6" t="n">
         <v>0.6324555320336759</v>
       </c>
-      <c r="R6" t="n">
+      <c r="AQ6" t="n">
+        <v>0.6835764481668571</v>
+      </c>
+      <c r="AR6" t="n">
         <v>0.3502958579881657</v>
       </c>
-      <c r="S6" t="n">
+      <c r="AS6" t="n">
+        <v>0.3960064247014668</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.467276760488416</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.9345554594764562</v>
+      </c>
+      <c r="AV6" t="n">
         <v>0.6710059171597633</v>
       </c>
-      <c r="T6" t="n">
+      <c r="AW6" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="AX6" t="n">
         <v>0.6305815855975138</v>
       </c>
-      <c r="U6" t="n">
+      <c r="AY6" t="n">
+        <v>0.703959013536917</v>
+      </c>
+      <c r="AZ6" t="n">
         <v>0.3479289940828402</v>
       </c>
-      <c r="V6" t="n">
+      <c r="BA6" t="n">
+        <v>0.4014632144076808</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>0.4955582927398693</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>0.9367030893797658</v>
+      </c>
+      <c r="BD6" t="n">
         <v>0.6733727810650888</v>
       </c>
-      <c r="W6" t="n">
+      <c r="BE6" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="BF6" t="n">
         <v>0.6231465103057326</v>
       </c>
-      <c r="X6" t="n">
+      <c r="BG6" t="n">
+        <v>0.636966432138438</v>
+      </c>
+      <c r="BH6" t="n">
         <v>0.3389012313521625</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="BI6" t="n">
+        <v>0.3398128477388861</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>0.4057262356711713</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>0.9367502554830595</v>
+      </c>
+      <c r="BL6" t="n">
         <v>0.6840236686390533</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>0.9798816568047337</v>
       </c>
     </row>
     <row r="7">
@@ -892,71 +1486,189 @@
         <v>0.6274585880517152</v>
       </c>
       <c r="C7" t="n">
+        <v>0.6547800997752682</v>
+      </c>
+      <c r="D7" t="n">
         <v>0.4616095074713775</v>
       </c>
-      <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
+        <v>0.43442282076456</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.4287369790617102</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.9546922411760081</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="n">
         <v>0.6545245349594661</v>
       </c>
-      <c r="F7" t="n">
+      <c r="K7" t="n">
+        <v>0.6794828877072008</v>
+      </c>
+      <c r="L7" t="n">
         <v>0.3692307692307693</v>
       </c>
-      <c r="G7" t="n">
+      <c r="M7" t="n">
+        <v>0.3898846160265609</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.4616969946869164</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.9308670701988837</v>
+      </c>
+      <c r="P7" t="n">
         <v>0.6544378698224852</v>
       </c>
-      <c r="H7" t="n">
+      <c r="Q7" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="R7" t="n">
         <v>0.6472518143988502</v>
       </c>
-      <c r="I7" t="n">
+      <c r="S7" t="n">
+        <v>0.6794949702119487</v>
+      </c>
+      <c r="T7" t="n">
         <v>0.3597633136094674</v>
       </c>
-      <c r="J7" t="n">
+      <c r="U7" t="n">
+        <v>0.3899010358829816</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.4617134145433371</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.9316531719204465</v>
+      </c>
+      <c r="X7" t="n">
         <v>0.663905325443787</v>
       </c>
-      <c r="K7" t="n">
+      <c r="Y7" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="Z7" t="n">
         <v>0.673241738062802</v>
       </c>
-      <c r="L7" t="n">
+      <c r="AA7" t="n">
+        <v>0.682605959165969</v>
+      </c>
+      <c r="AB7" t="n">
         <v>0.3940828402366864</v>
       </c>
-      <c r="M7" t="n">
+      <c r="AC7" t="n">
+        <v>0.394382384603763</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0.4659508954888926</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0.9271818253281975</v>
+      </c>
+      <c r="AF7" t="n">
         <v>0.6295857988165681</v>
       </c>
-      <c r="N7" t="n">
+      <c r="AG7" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="AH7" t="n">
         <v>0.6567231436183164</v>
       </c>
-      <c r="O7" t="n">
+      <c r="AI7" t="n">
+        <v>0.6754153366733711</v>
+      </c>
+      <c r="AJ7" t="n">
         <v>0.3487090867469425</v>
       </c>
-      <c r="P7" t="n">
+      <c r="AK7" t="n">
+        <v>0.3798087261690064</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>0.4561858770136031</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>0.9306658281581637</v>
+      </c>
+      <c r="AN7" t="n">
         <v>0.6887573964497041</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="AO7" t="n">
+        <v>0.9680473372781065</v>
+      </c>
+      <c r="AP7" t="n">
         <v>0.6472518143988502</v>
       </c>
-      <c r="R7" t="n">
+      <c r="AQ7" t="n">
+        <v>0.6794949702119487</v>
+      </c>
+      <c r="AR7" t="n">
         <v>0.3597633136094674</v>
       </c>
-      <c r="S7" t="n">
+      <c r="AS7" t="n">
+        <v>0.3899010358829816</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0.4617134145433371</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0.9316531719204465</v>
+      </c>
+      <c r="AV7" t="n">
         <v>0.663905325443787</v>
       </c>
-      <c r="T7" t="n">
+      <c r="AW7" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="AX7" t="n">
         <v>0.6617173282340483</v>
       </c>
-      <c r="U7" t="n">
+      <c r="AY7" t="n">
+        <v>0.6852614943599901</v>
+      </c>
+      <c r="AZ7" t="n">
         <v>0.3692307692307693</v>
       </c>
-      <c r="V7" t="n">
+      <c r="BA7" t="n">
+        <v>0.3954047731352842</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>0.4695833156524867</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>0.9306280952755287</v>
+      </c>
+      <c r="BD7" t="n">
         <v>0.659171597633136</v>
       </c>
-      <c r="W7" t="n">
+      <c r="BE7" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="BF7" t="n">
         <v>0.6485633352186657</v>
       </c>
-      <c r="X7" t="n">
+      <c r="BG7" t="n">
+        <v>0.6404772425069131</v>
+      </c>
+      <c r="BH7" t="n">
         <v>0.3522593826049307</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="BI7" t="n">
+        <v>0.3380078603681406</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>0.4102110981692591</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>0.9307538715509787</v>
+      </c>
+      <c r="BL7" t="n">
         <v>0.6781065088757396</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>0.9751479289940829</v>
       </c>
     </row>
     <row r="8">
@@ -969,71 +1681,189 @@
         <v>0.6231961753542494</v>
       </c>
       <c r="C8" t="n">
+        <v>0.6475440226724331</v>
+      </c>
+      <c r="D8" t="n">
         <v>0.4581329389437645</v>
       </c>
-      <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
+        <v>0.4257441705116161</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.4193132612987965</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.9554028771323009</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="n">
         <v>0.642664571514013</v>
       </c>
-      <c r="F8" t="n">
+      <c r="K8" t="n">
+        <v>0.6795956494698689</v>
+      </c>
+      <c r="L8" t="n">
         <v>0.3609467455621302</v>
       </c>
-      <c r="G8" t="n">
+      <c r="M8" t="n">
+        <v>0.3921248246397566</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.461850246778373</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.9328763461991981</v>
+      </c>
+      <c r="P8" t="n">
         <v>0.6615384615384615</v>
       </c>
-      <c r="H8" t="n">
+      <c r="Q8" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="R8" t="n">
         <v>0.6463369703876924</v>
       </c>
-      <c r="I8" t="n">
+      <c r="S8" t="n">
+        <v>0.6829842074389531</v>
+      </c>
+      <c r="T8" t="n">
         <v>0.3538461538461539</v>
       </c>
-      <c r="J8" t="n">
+      <c r="U8" t="n">
+        <v>0.3924502144476882</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.4664674276110148</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.9328511909441082</v>
+      </c>
+      <c r="X8" t="n">
         <v>0.672189349112426</v>
       </c>
-      <c r="K8" t="n">
+      <c r="Y8" t="n">
+        <v>0.978698224852071</v>
+      </c>
+      <c r="Z8" t="n">
         <v>0.6670610273439631</v>
       </c>
-      <c r="L8" t="n">
+      <c r="AA8" t="n">
+        <v>0.695246229593111</v>
+      </c>
+      <c r="AB8" t="n">
         <v>0.3763313609467456</v>
       </c>
-      <c r="M8" t="n">
+      <c r="AC8" t="n">
+        <v>0.4089360801353088</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>0.4833673197634368</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>0.9262164924141184</v>
+      </c>
+      <c r="AF8" t="n">
         <v>0.6520710059171597</v>
       </c>
-      <c r="N8" t="n">
+      <c r="AG8" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="AH8" t="n">
         <v>0.6562714851961153</v>
       </c>
-      <c r="O8" t="n">
+      <c r="AI8" t="n">
+        <v>0.6480965502188107</v>
+      </c>
+      <c r="AJ8" t="n">
         <v>0.343812504187075</v>
       </c>
-      <c r="P8" t="n">
+      <c r="AK8" t="n">
+        <v>0.3367678583912433</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>0.4200291384055234</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>0.933036710950397</v>
+      </c>
+      <c r="AN8" t="n">
         <v>0.6946745562130178</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="AO8" t="n">
+        <v>0.9680473372781065</v>
+      </c>
+      <c r="AP8" t="n">
         <v>0.6463369703876924</v>
       </c>
-      <c r="R8" t="n">
+      <c r="AQ8" t="n">
+        <v>0.6829842074389531</v>
+      </c>
+      <c r="AR8" t="n">
         <v>0.3538461538461539</v>
       </c>
-      <c r="S8" t="n">
+      <c r="AS8" t="n">
+        <v>0.3924502144476882</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>0.4664674276110148</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>0.9328511909441082</v>
+      </c>
+      <c r="AV8" t="n">
         <v>0.672189349112426</v>
       </c>
-      <c r="T8" t="n">
+      <c r="AW8" t="n">
+        <v>0.978698224852071</v>
+      </c>
+      <c r="AX8" t="n">
         <v>0.6590292304801199</v>
       </c>
-      <c r="U8" t="n">
+      <c r="AY8" t="n">
+        <v>0.7277652269540663</v>
+      </c>
+      <c r="AZ8" t="n">
         <v>0.3538461538461539</v>
       </c>
-      <c r="V8" t="n">
+      <c r="BA8" t="n">
+        <v>0.4162216636935658</v>
+      </c>
+      <c r="BB8" t="n">
+        <v>0.5296422255635036</v>
+      </c>
+      <c r="BC8" t="n">
+        <v>0.9312884207216414</v>
+      </c>
+      <c r="BD8" t="n">
         <v>0.6792899408284023</v>
       </c>
-      <c r="W8" t="n">
+      <c r="BE8" t="n">
+        <v>0.9727810650887574</v>
+      </c>
+      <c r="BF8" t="n">
         <v>0.6471923537518717</v>
       </c>
-      <c r="X8" t="n">
+      <c r="BG8" t="n">
+        <v>0.6458698813988788</v>
+      </c>
+      <c r="BH8" t="n">
         <v>0.3485462319977259</v>
       </c>
-      <c r="Y8" t="n">
+      <c r="BI8" t="n">
+        <v>0.3387561889013129</v>
+      </c>
+      <c r="BJ8" t="n">
+        <v>0.4171479036982017</v>
+      </c>
+      <c r="BK8" t="n">
+        <v>0.9332316641773446</v>
+      </c>
+      <c r="BL8" t="n">
         <v>0.6816568047337278</v>
+      </c>
+      <c r="BM8" t="n">
+        <v>0.9763313609467456</v>
       </c>
     </row>
     <row r="9">
@@ -1046,71 +1876,189 @@
         <v>0.6238736643249453</v>
       </c>
       <c r="C9" t="n">
+        <v>0.6505401601531055</v>
+      </c>
+      <c r="D9" t="n">
         <v>0.458583312345496</v>
       </c>
-      <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
+        <v>0.4279289107842686</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.4232024999720281</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.9560443361370962</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="n">
         <v>0.6454208296431702</v>
       </c>
-      <c r="F9" t="n">
+      <c r="K9" t="n">
+        <v>0.6797228352575057</v>
+      </c>
+      <c r="L9" t="n">
         <v>0.3621301775147929</v>
       </c>
-      <c r="G9" t="n">
+      <c r="M9" t="n">
+        <v>0.3909801875752323</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.4620231327705022</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.9337190472447134</v>
+      </c>
+      <c r="P9" t="n">
         <v>0.6615384615384615</v>
       </c>
-      <c r="H9" t="n">
+      <c r="Q9" t="n">
+        <v>0.9798816568047337</v>
+      </c>
+      <c r="R9" t="n">
         <v>0.6435846357954428</v>
       </c>
-      <c r="I9" t="n">
+      <c r="S9" t="n">
+        <v>0.7105600837480252</v>
+      </c>
+      <c r="T9" t="n">
         <v>0.3526627218934911</v>
       </c>
-      <c r="J9" t="n">
+      <c r="U9" t="n">
+        <v>0.4026623456713827</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.5048956326160006</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.9340146214920211</v>
+      </c>
+      <c r="X9" t="n">
         <v>0.6745562130177515</v>
       </c>
-      <c r="K9" t="n">
+      <c r="Y9" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="Z9" t="n">
         <v>0.6527139518645054</v>
       </c>
-      <c r="L9" t="n">
+      <c r="AA9" t="n">
+        <v>0.6792998659002999</v>
+      </c>
+      <c r="AB9" t="n">
         <v>0.3692307692307693</v>
       </c>
-      <c r="M9" t="n">
+      <c r="AC9" t="n">
+        <v>0.3933556394225973</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>0.4614483078121654</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>0.931058879018945</v>
+      </c>
+      <c r="AF9" t="n">
         <v>0.6544378698224852</v>
       </c>
-      <c r="N9" t="n">
+      <c r="AG9" t="n">
+        <v>0.9798816568047337</v>
+      </c>
+      <c r="AH9" t="n">
         <v>0.648934875833757</v>
       </c>
-      <c r="O9" t="n">
+      <c r="AI9" t="n">
+        <v>0.6441732619680518</v>
+      </c>
+      <c r="AJ9" t="n">
         <v>0.3438419550396201</v>
       </c>
-      <c r="P9" t="n">
+      <c r="AK9" t="n">
+        <v>0.3399296196576965</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>0.4149591914345602</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>0.9337190472447134</v>
+      </c>
+      <c r="AN9" t="n">
         <v>0.693491124260355</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="AO9" t="n">
+        <v>0.9668639053254438</v>
+      </c>
+      <c r="AP9" t="n">
         <v>0.6435846357954428</v>
       </c>
-      <c r="R9" t="n">
+      <c r="AQ9" t="n">
+        <v>0.7105600837480252</v>
+      </c>
+      <c r="AR9" t="n">
         <v>0.3526627218934911</v>
       </c>
-      <c r="S9" t="n">
+      <c r="AS9" t="n">
+        <v>0.4026623456713827</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0.5048956326160006</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.9340146214920211</v>
+      </c>
+      <c r="AV9" t="n">
         <v>0.6745562130177515</v>
       </c>
-      <c r="T9" t="n">
+      <c r="AW9" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="AX9" t="n">
         <v>0.6249260311258431</v>
       </c>
-      <c r="U9" t="n">
+      <c r="AY9" t="n">
+        <v>0.6764817692204672</v>
+      </c>
+      <c r="AZ9" t="n">
         <v>0.3431952662721893</v>
       </c>
-      <c r="V9" t="n">
+      <c r="BA9" t="n">
+        <v>0.3892934662968631</v>
+      </c>
+      <c r="BB9" t="n">
+        <v>0.4576275840876534</v>
+      </c>
+      <c r="BC9" t="n">
+        <v>0.9359767313890417</v>
+      </c>
+      <c r="BD9" t="n">
         <v>0.6781065088757396</v>
       </c>
-      <c r="W9" t="n">
+      <c r="BE9" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="BF9" t="n">
         <v>0.6397516342665694</v>
       </c>
-      <c r="X9" t="n">
+      <c r="BG9" t="n">
+        <v>0.6419329846076135</v>
+      </c>
+      <c r="BH9" t="n">
         <v>0.348575682850271</v>
       </c>
-      <c r="Y9" t="n">
+      <c r="BI9" t="n">
+        <v>0.3419179501677661</v>
+      </c>
+      <c r="BJ9" t="n">
+        <v>0.4120779567272385</v>
+      </c>
+      <c r="BK9" t="n">
+        <v>0.9339140004716611</v>
+      </c>
+      <c r="BL9" t="n">
         <v>0.6804733727810651</v>
+      </c>
+      <c r="BM9" t="n">
+        <v>0.9751479289940829</v>
       </c>
     </row>
     <row r="10">
@@ -1123,71 +2071,189 @@
         <v>0.4942965567185033</v>
       </c>
       <c r="C10" t="n">
+        <v>0.6067127751946909</v>
+      </c>
+      <c r="D10" t="n">
         <v>0.3472105258651251</v>
       </c>
-      <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
+        <v>0.3934425383849193</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.3681003915844435</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.9770363965097083</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="n">
         <v>0.5125640384294671</v>
       </c>
-      <c r="F10" t="n">
+      <c r="K10" t="n">
+        <v>0.5962414758560869</v>
+      </c>
+      <c r="L10" t="n">
         <v>0.2177514792899408</v>
       </c>
-      <c r="G10" t="n">
+      <c r="M10" t="n">
+        <v>0.2689844154452598</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.3555038975310447</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.9568241490448864</v>
+      </c>
+      <c r="P10" t="n">
         <v>0.8011834319526627</v>
       </c>
-      <c r="H10" t="n">
+      <c r="Q10" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="R10" t="n">
         <v>0.5125640384294671</v>
       </c>
-      <c r="I10" t="n">
+      <c r="S10" t="n">
+        <v>0.5962414758560869</v>
+      </c>
+      <c r="T10" t="n">
         <v>0.2177514792899408</v>
       </c>
-      <c r="J10" t="n">
+      <c r="U10" t="n">
+        <v>0.2689844154452598</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.3555038975310447</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.9568241490448864</v>
+      </c>
+      <c r="X10" t="n">
         <v>0.8011834319526627</v>
       </c>
-      <c r="K10" t="n">
+      <c r="Y10" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="Z10" t="n">
         <v>0.5428393465962261</v>
       </c>
-      <c r="L10" t="n">
+      <c r="AA10" t="n">
+        <v>0.6115371438006899</v>
+      </c>
+      <c r="AB10" t="n">
         <v>0.2473372781065089</v>
       </c>
-      <c r="M10" t="n">
+      <c r="AC10" t="n">
+        <v>0.2843526061000089</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>0.3739776782479056</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>0.9512365380080182</v>
+      </c>
+      <c r="AF10" t="n">
         <v>0.7727810650887574</v>
       </c>
-      <c r="N10" t="n">
+      <c r="AG10" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="AH10" t="n">
         <v>0.4857484021051881</v>
       </c>
-      <c r="O10" t="n">
+      <c r="AI10" t="n">
+        <v>0.5971617203860753</v>
+      </c>
+      <c r="AJ10" t="n">
         <v>0.1915325847455647</v>
       </c>
-      <c r="P10" t="n">
+      <c r="AK10" t="n">
+        <v>0.2708091713879109</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>0.3566021202944571</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>0.9583963524880119</v>
+      </c>
+      <c r="AN10" t="n">
         <v>0.8307692307692308</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="AO10" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="AP10" t="n">
         <v>0.5125640384294671</v>
       </c>
-      <c r="R10" t="n">
+      <c r="AQ10" t="n">
+        <v>0.5962414758560869</v>
+      </c>
+      <c r="AR10" t="n">
         <v>0.2177514792899408</v>
       </c>
-      <c r="S10" t="n">
+      <c r="AS10" t="n">
+        <v>0.2689844154452598</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>0.3555038975310447</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>0.9568241490448864</v>
+      </c>
+      <c r="AV10" t="n">
         <v>0.8011834319526627</v>
       </c>
-      <c r="T10" t="n">
+      <c r="AW10" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="AX10" t="n">
         <v>0.5008867875722987</v>
       </c>
-      <c r="U10" t="n">
+      <c r="AY10" t="n">
+        <v>0.5961744187172013</v>
+      </c>
+      <c r="AZ10" t="n">
         <v>0.2035502958579882</v>
       </c>
-      <c r="V10" t="n">
+      <c r="BA10" t="n">
+        <v>0.2657988653848962</v>
+      </c>
+      <c r="BB10" t="n">
+        <v>0.3554239375327929</v>
+      </c>
+      <c r="BC10" t="n">
+        <v>0.95619212326075</v>
+      </c>
+      <c r="BD10" t="n">
         <v>0.8165680473372781</v>
       </c>
-      <c r="W10" t="n">
+      <c r="BE10" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="BF10" t="n">
         <v>0.4953977853897263</v>
       </c>
-      <c r="X10" t="n">
+      <c r="BG10" t="n">
+        <v>0.5980278563594071</v>
+      </c>
+      <c r="BH10" t="n">
         <v>0.2010000403668665</v>
       </c>
-      <c r="Y10" t="n">
+      <c r="BI10" t="n">
+        <v>0.2718443680752815</v>
+      </c>
+      <c r="BJ10" t="n">
+        <v>0.3576373169818277</v>
+      </c>
+      <c r="BK10" t="n">
+        <v>0.9580661897649556</v>
+      </c>
+      <c r="BL10" t="n">
         <v>0.821301775147929</v>
+      </c>
+      <c r="BM10" t="n">
+        <v>0.9846153846153847</v>
       </c>
     </row>
     <row r="11">
@@ -1200,71 +2266,189 @@
         <v>0.5862203024542455</v>
       </c>
       <c r="C11" t="n">
+        <v>0.7747276358948593</v>
+      </c>
+      <c r="D11" t="n">
         <v>0.4112175851766155</v>
       </c>
-      <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
+        <v>0.4805414953307796</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.6002029098192376</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.9590692555616697</v>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="n">
         <v>0.633390426161197</v>
       </c>
-      <c r="F11" t="n">
+      <c r="K11" t="n">
+        <v>0.8205539802432845</v>
+      </c>
+      <c r="L11" t="n">
         <v>0.3443786982248521</v>
       </c>
-      <c r="G11" t="n">
+      <c r="M11" t="n">
+        <v>0.4407138349732355</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.6733088344930965</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.9309991352881063</v>
+      </c>
+      <c r="P11" t="n">
         <v>0.6828402366863905</v>
       </c>
-      <c r="H11" t="n">
+      <c r="Q11" t="n">
+        <v>0.9739644970414201</v>
+      </c>
+      <c r="R11" t="n">
         <v>0.7016464154456233</v>
       </c>
-      <c r="I11" t="n">
+      <c r="S11" t="n">
+        <v>0.7893841050423023</v>
+      </c>
+      <c r="T11" t="n">
         <v>0.4260355029585799</v>
       </c>
-      <c r="J11" t="n">
+      <c r="U11" t="n">
+        <v>0.4631208089866726</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.6231272652934365</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.9282383460419779</v>
+      </c>
+      <c r="X11" t="n">
         <v>0.6059171597633136</v>
       </c>
-      <c r="K11" t="n">
+      <c r="Y11" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="Z11" t="n">
         <v>0.6445033866354896</v>
       </c>
-      <c r="L11" t="n">
+      <c r="AA11" t="n">
+        <v>0.8542069145347269</v>
+      </c>
+      <c r="AB11" t="n">
         <v>0.3325443786982248</v>
       </c>
-      <c r="M11" t="n">
+      <c r="AC11" t="n">
+        <v>0.4730153999104796</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>0.7296694528389381</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0.9315682729345177</v>
+      </c>
+      <c r="AF11" t="n">
         <v>0.7065088757396449</v>
       </c>
-      <c r="N11" t="n">
+      <c r="AG11" t="n">
+        <v>0.9633136094674556</v>
+      </c>
+      <c r="AH11" t="n">
         <v>0.7016464154456233</v>
       </c>
-      <c r="O11" t="n">
+      <c r="AI11" t="n">
+        <v>0.7893841050423023</v>
+      </c>
+      <c r="AJ11" t="n">
         <v>0.4260355029585799</v>
       </c>
-      <c r="P11" t="n">
+      <c r="AK11" t="n">
+        <v>0.4631208089866726</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>0.6231272652934365</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>0.9282383460419779</v>
+      </c>
+      <c r="AN11" t="n">
         <v>0.6059171597633136</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="AO11" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="AP11" t="n">
         <v>0.651806774286611</v>
       </c>
-      <c r="R11" t="n">
+      <c r="AQ11" t="n">
+        <v>0.7667822591076271</v>
+      </c>
+      <c r="AR11" t="n">
         <v>0.3704142011834319</v>
       </c>
-      <c r="S11" t="n">
+      <c r="AS11" t="n">
+        <v>0.4070150695911505</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>0.5879550328821962</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>0.9307884600267274</v>
+      </c>
+      <c r="AV11" t="n">
         <v>0.6556213017751479</v>
       </c>
-      <c r="T11" t="n">
+      <c r="AW11" t="n">
+        <v>0.9751479289940829</v>
+      </c>
+      <c r="AX11" t="n">
         <v>0.6287020535908477</v>
       </c>
-      <c r="U11" t="n">
+      <c r="AY11" t="n">
+        <v>0.8361010748521609</v>
+      </c>
+      <c r="AZ11" t="n">
         <v>0.3266272189349113</v>
       </c>
-      <c r="V11" t="n">
+      <c r="BA11" t="n">
+        <v>0.4555597269929796</v>
+      </c>
+      <c r="BB11" t="n">
+        <v>0.6990650073689387</v>
+      </c>
+      <c r="BC11" t="n">
+        <v>0.9343542174357362</v>
+      </c>
+      <c r="BD11" t="n">
         <v>0.7053254437869823</v>
       </c>
-      <c r="W11" t="n">
+      <c r="BE11" t="n">
+        <v>0.9704142011834319</v>
+      </c>
+      <c r="BF11" t="n">
         <v>0.651806774286611</v>
       </c>
-      <c r="X11" t="n">
+      <c r="BG11" t="n">
+        <v>0.7667822591076271</v>
+      </c>
+      <c r="BH11" t="n">
         <v>0.3704142011834319</v>
       </c>
-      <c r="Y11" t="n">
+      <c r="BI11" t="n">
+        <v>0.4070150695911505</v>
+      </c>
+      <c r="BJ11" t="n">
+        <v>0.5879550328821962</v>
+      </c>
+      <c r="BK11" t="n">
+        <v>0.9307884600267274</v>
+      </c>
+      <c r="BL11" t="n">
         <v>0.6556213017751479</v>
+      </c>
+      <c r="BM11" t="n">
+        <v>0.9751479289940829</v>
       </c>
     </row>
     <row r="12">
@@ -1277,71 +2461,189 @@
         <v>0.4467402618283487</v>
       </c>
       <c r="C12" t="n">
+        <v>0.5668173650973868</v>
+      </c>
+      <c r="D12" t="n">
         <v>0.263498224852071</v>
       </c>
-      <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
+        <v>0.3424043125107377</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.3212819253759442</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.9799952833896706</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="n">
         <v>0.4925480182640652</v>
       </c>
-      <c r="F12" t="n">
+      <c r="K12" t="n">
+        <v>0.6284945221690352</v>
+      </c>
+      <c r="L12" t="n">
         <v>0.1905325443786982</v>
       </c>
-      <c r="G12" t="n">
+      <c r="M12" t="n">
+        <v>0.2942171276302885</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.395005364396484</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.9600031444068863</v>
+      </c>
+      <c r="P12" t="n">
         <v>0.829585798816568</v>
       </c>
-      <c r="H12" t="n">
+      <c r="Q12" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="R12" t="n">
         <v>0.4937478934117296</v>
       </c>
-      <c r="I12" t="n">
+      <c r="S12" t="n">
+        <v>0.6431215278839518</v>
+      </c>
+      <c r="T12" t="n">
         <v>0.1893491124260355</v>
       </c>
-      <c r="J12" t="n">
+      <c r="U12" t="n">
+        <v>0.3094873878932521</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.4136052996277887</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.9612954956371355</v>
+      </c>
+      <c r="X12" t="n">
         <v>0.8319526627218935</v>
       </c>
-      <c r="K12" t="n">
+      <c r="Y12" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="Z12" t="n">
         <v>0.5137171648327384</v>
       </c>
-      <c r="L12" t="n">
+      <c r="AA12" t="n">
+        <v>0.6315384603567777</v>
+      </c>
+      <c r="AB12" t="n">
         <v>0.2047337278106509</v>
       </c>
-      <c r="M12" t="n">
+      <c r="AC12" t="n">
+        <v>0.2959656336218747</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0.3988408269098094</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0.9579655687445956</v>
+      </c>
+      <c r="AF12" t="n">
         <v>0.8189349112426035</v>
       </c>
-      <c r="N12" t="n">
+      <c r="AG12" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="AH12" t="n">
         <v>0.4877189995122264</v>
       </c>
-      <c r="O12" t="n">
+      <c r="AI12" t="n">
+        <v>0.6465303491816524</v>
+      </c>
+      <c r="AJ12" t="n">
         <v>0.1905325443786982</v>
       </c>
-      <c r="P12" t="n">
+      <c r="AK12" t="n">
+        <v>0.3232003508647483</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>0.4180014924129494</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>0.9625060922883422</v>
+      </c>
+      <c r="AN12" t="n">
         <v>0.8284023668639053</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="AO12" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="AP12" t="n">
         <v>0.4937478934117296</v>
       </c>
-      <c r="R12" t="n">
+      <c r="AQ12" t="n">
+        <v>0.6431215278839518</v>
+      </c>
+      <c r="AR12" t="n">
         <v>0.1893491124260355</v>
       </c>
-      <c r="S12" t="n">
+      <c r="AS12" t="n">
+        <v>0.3094873878932521</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0.4136052996277887</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.9612954956371355</v>
+      </c>
+      <c r="AV12" t="n">
         <v>0.8319526627218935</v>
       </c>
-      <c r="T12" t="n">
+      <c r="AW12" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="AX12" t="n">
         <v>0.5148677086363542</v>
       </c>
-      <c r="U12" t="n">
+      <c r="AY12" t="n">
+        <v>0.6406375715079251</v>
+      </c>
+      <c r="AZ12" t="n">
         <v>0.2035502958579882</v>
       </c>
-      <c r="V12" t="n">
+      <c r="BA12" t="n">
+        <v>0.3040630438700719</v>
+      </c>
+      <c r="BB12" t="n">
+        <v>0.4104164980275718</v>
+      </c>
+      <c r="BC12" t="n">
+        <v>0.9581165002751356</v>
+      </c>
+      <c r="BD12" t="n">
         <v>0.821301775147929</v>
       </c>
-      <c r="W12" t="n">
+      <c r="BE12" t="n">
+        <v>0.9798816568047337</v>
+      </c>
+      <c r="BF12" t="n">
         <v>0.4877189995122264</v>
       </c>
-      <c r="X12" t="n">
+      <c r="BG12" t="n">
+        <v>0.6465303491816524</v>
+      </c>
+      <c r="BH12" t="n">
         <v>0.1905325443786982</v>
       </c>
-      <c r="Y12" t="n">
+      <c r="BI12" t="n">
+        <v>0.3232003508647483</v>
+      </c>
+      <c r="BJ12" t="n">
+        <v>0.4180014924129494</v>
+      </c>
+      <c r="BK12" t="n">
+        <v>0.9625060922883422</v>
+      </c>
+      <c r="BL12" t="n">
         <v>0.8284023668639053</v>
+      </c>
+      <c r="BM12" t="n">
+        <v>0.9846153846153847</v>
       </c>
     </row>
     <row r="13">
@@ -1351,74 +2653,192 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4554190548258276</v>
+        <v>0.4623824243811015</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2745606345879602</v>
-      </c>
-      <c r="D13" t="inlineStr"/>
+        <v>0.6340636203826128</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.2835653659182524</v>
+      </c>
       <c r="E13" t="n">
-        <v>0.4791511231506904</v>
+        <v>0.3916669329988137</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1798816568047337</v>
+        <v>0.402036674692706</v>
       </c>
       <c r="G13" t="n">
-        <v>0.8390532544378698</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.6837072628704299</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.4035502958579882</v>
-      </c>
+        <v>0.9774891911013285</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="n">
-        <v>0.6177514792899408</v>
+        <v>0.506759048984634</v>
       </c>
       <c r="K13" t="n">
-        <v>0.5547001962252291</v>
+        <v>0.6832498933534507</v>
       </c>
       <c r="L13" t="n">
-        <v>0.2461538461538462</v>
+        <v>0.2047337278106509</v>
       </c>
       <c r="M13" t="n">
-        <v>0.778698224852071</v>
+        <v>0.3676863681113329</v>
       </c>
       <c r="N13" t="n">
-        <v>0.6839639214624242</v>
+        <v>0.4668304167675018</v>
       </c>
       <c r="O13" t="n">
-        <v>0.4059822971712957</v>
+        <v>0.9576448392421979</v>
       </c>
       <c r="P13" t="n">
-        <v>0.6177514792899408</v>
+        <v>0.8153846153846154</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.5373615137407071</v>
+        <v>0.9846153846153847</v>
       </c>
       <c r="R13" t="n">
-        <v>0.2414201183431953</v>
+        <v>0.6897388237372275</v>
       </c>
       <c r="S13" t="n">
-        <v>0.7751479289940828</v>
+        <v>0.8069421254921904</v>
       </c>
       <c r="T13" t="n">
-        <v>0.5032439148860347</v>
+        <v>0.4165680473372781</v>
       </c>
       <c r="U13" t="n">
-        <v>0.1988165680473373</v>
+        <v>0.498881278649509</v>
       </c>
       <c r="V13" t="n">
-        <v>0.8224852071005917</v>
+        <v>0.6511555938938538</v>
       </c>
       <c r="W13" t="n">
-        <v>0.5376880331662462</v>
+        <v>0.9405864318842858</v>
       </c>
       <c r="X13" t="n">
-        <v>0.2438521196565028</v>
+        <v>0.6047337278106509</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.7751479289940828</v>
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.5704768066996664</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>0.7045740871608913</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0.2662721893491125</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>0.3875769576655045</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>0.4964246442986033</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0.9460231113906139</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>0.757396449704142</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>0.9810650887573964</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>0.6901479538241796</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>0.8071588678204578</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>0.4196669759671213</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>0.5006239891110495</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>0.6515054379012032</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>0.9406147315462621</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>0.6047337278106509</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>0.9834319526627219</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>0.54934064834945</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>0.6865582680204986</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>0.2544378698224852</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>0.3755228840810114</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>0.4713622553873067</v>
+      </c>
+      <c r="AU13" t="n">
+        <v>0.951972329219401</v>
+      </c>
+      <c r="AV13" t="n">
+        <v>0.7633136094674556</v>
+      </c>
+      <c r="AW13" t="n">
+        <v>0.98698224852071</v>
+      </c>
+      <c r="AX13" t="n">
+        <v>0.5228506297835824</v>
+      </c>
+      <c r="AY13" t="n">
+        <v>0.7018357277289305</v>
+      </c>
+      <c r="AZ13" t="n">
+        <v>0.221301775147929</v>
+      </c>
+      <c r="BA13" t="n">
+        <v>0.393812658605438</v>
+      </c>
+      <c r="BB13" t="n">
+        <v>0.4925733887167976</v>
+      </c>
+      <c r="BC13" t="n">
+        <v>0.9541985692948668</v>
+      </c>
+      <c r="BD13" t="n">
+        <v>0.7988165680473372</v>
+      </c>
+      <c r="BE13" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="BF13" t="n">
+        <v>0.5498542544404671</v>
+      </c>
+      <c r="BG13" t="n">
+        <v>0.686813001765878</v>
+      </c>
+      <c r="BH13" t="n">
+        <v>0.2575367984523284</v>
+      </c>
+      <c r="BI13" t="n">
+        <v>0.377265594542552</v>
+      </c>
+      <c r="BJ13" t="n">
+        <v>0.471712099394656</v>
+      </c>
+      <c r="BK13" t="n">
+        <v>0.9520540837984435</v>
+      </c>
+      <c r="BL13" t="n">
+        <v>0.7633136094674556</v>
+      </c>
+      <c r="BM13" t="n">
+        <v>0.9857988165680474</v>
       </c>
     </row>
     <row r="14">
@@ -1431,71 +2851,189 @@
         <v>0.6499886207470034</v>
       </c>
       <c r="C14" t="n">
+        <v>0.6852985072099496</v>
+      </c>
+      <c r="D14" t="n">
         <v>0.3467455621301775</v>
       </c>
-      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
+        <v>0.3861356324277022</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.4696340439841853</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.9304614417105573</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="n">
         <v>0.6499886207470034</v>
       </c>
-      <c r="F14" t="n">
-        <v>0.3467455621301775</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.6887573964497041</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.6499886207470034</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.3467455621301775</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.6887573964497041</v>
-      </c>
       <c r="K14" t="n">
-        <v>0.6499886207470034</v>
+        <v>0.6852985072099496</v>
       </c>
       <c r="L14" t="n">
         <v>0.3467455621301775</v>
       </c>
       <c r="M14" t="n">
-        <v>0.6887573964497041</v>
+        <v>0.3861356324277022</v>
       </c>
       <c r="N14" t="n">
-        <v>0.6499886207470034</v>
+        <v>0.4696340439841853</v>
       </c>
       <c r="O14" t="n">
-        <v>0.3467455621301775</v>
+        <v>0.9304614417105573</v>
       </c>
       <c r="P14" t="n">
         <v>0.6887573964497041</v>
       </c>
       <c r="Q14" t="n">
+        <v>0.9668639053254438</v>
+      </c>
+      <c r="R14" t="n">
         <v>0.6499886207470034</v>
       </c>
-      <c r="R14" t="n">
+      <c r="S14" t="n">
+        <v>0.6852985072099496</v>
+      </c>
+      <c r="T14" t="n">
         <v>0.3467455621301775</v>
       </c>
-      <c r="S14" t="n">
+      <c r="U14" t="n">
+        <v>0.3861356324277022</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0.4696340439841853</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0.9304614417105573</v>
+      </c>
+      <c r="X14" t="n">
         <v>0.6887573964497041</v>
       </c>
-      <c r="T14" t="n">
+      <c r="Y14" t="n">
+        <v>0.9668639053254438</v>
+      </c>
+      <c r="Z14" t="n">
         <v>0.6499886207470034</v>
       </c>
-      <c r="U14" t="n">
+      <c r="AA14" t="n">
+        <v>0.6852985072099496</v>
+      </c>
+      <c r="AB14" t="n">
         <v>0.3467455621301775</v>
       </c>
-      <c r="V14" t="n">
+      <c r="AC14" t="n">
+        <v>0.3861356324277022</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>0.4696340439841853</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>0.9304614417105573</v>
+      </c>
+      <c r="AF14" t="n">
         <v>0.6887573964497041</v>
       </c>
-      <c r="W14" t="n">
+      <c r="AG14" t="n">
+        <v>0.9668639053254438</v>
+      </c>
+      <c r="AH14" t="n">
         <v>0.6499886207470034</v>
       </c>
-      <c r="X14" t="n">
+      <c r="AI14" t="n">
+        <v>0.6852985072099496</v>
+      </c>
+      <c r="AJ14" t="n">
         <v>0.3467455621301775</v>
       </c>
-      <c r="Y14" t="n">
+      <c r="AK14" t="n">
+        <v>0.3861356324277022</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>0.4696340439841853</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>0.9304614417105573</v>
+      </c>
+      <c r="AN14" t="n">
         <v>0.6887573964497041</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>0.9668639053254438</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>0.6499886207470034</v>
+      </c>
+      <c r="AQ14" t="n">
+        <v>0.6852985072099496</v>
+      </c>
+      <c r="AR14" t="n">
+        <v>0.3467455621301775</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>0.3861356324277022</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>0.4696340439841853</v>
+      </c>
+      <c r="AU14" t="n">
+        <v>0.9304614417105573</v>
+      </c>
+      <c r="AV14" t="n">
+        <v>0.6887573964497041</v>
+      </c>
+      <c r="AW14" t="n">
+        <v>0.9668639053254438</v>
+      </c>
+      <c r="AX14" t="n">
+        <v>0.6499886207470034</v>
+      </c>
+      <c r="AY14" t="n">
+        <v>0.6852985072099496</v>
+      </c>
+      <c r="AZ14" t="n">
+        <v>0.3467455621301775</v>
+      </c>
+      <c r="BA14" t="n">
+        <v>0.3861356324277022</v>
+      </c>
+      <c r="BB14" t="n">
+        <v>0.4696340439841853</v>
+      </c>
+      <c r="BC14" t="n">
+        <v>0.9304614417105573</v>
+      </c>
+      <c r="BD14" t="n">
+        <v>0.6887573964497041</v>
+      </c>
+      <c r="BE14" t="n">
+        <v>0.9668639053254438</v>
+      </c>
+      <c r="BF14" t="n">
+        <v>0.6499886207470034</v>
+      </c>
+      <c r="BG14" t="n">
+        <v>0.6852985072099496</v>
+      </c>
+      <c r="BH14" t="n">
+        <v>0.3467455621301775</v>
+      </c>
+      <c r="BI14" t="n">
+        <v>0.3861356324277022</v>
+      </c>
+      <c r="BJ14" t="n">
+        <v>0.4696340439841853</v>
+      </c>
+      <c r="BK14" t="n">
+        <v>0.9304614417105573</v>
+      </c>
+      <c r="BL14" t="n">
+        <v>0.6887573964497041</v>
+      </c>
+      <c r="BM14" t="n">
+        <v>0.9668639053254438</v>
       </c>
     </row>
     <row r="15">
@@ -1508,71 +3046,189 @@
         <v>0.6066690508655493</v>
       </c>
       <c r="C15" t="n">
+        <v>0.6576778610115588</v>
+      </c>
+      <c r="D15" t="n">
         <v>0.3112426035502959</v>
       </c>
-      <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
+        <v>0.3610679494145611</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.4325401688647393</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.9394764562534392</v>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="n">
         <v>0.6066690508655493</v>
       </c>
-      <c r="F15" t="n">
-        <v>0.3112426035502959</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.7159763313609467</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.6066690508655493</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0.3112426035502959</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0.7159763313609467</v>
-      </c>
       <c r="K15" t="n">
-        <v>0.6066690508655493</v>
+        <v>0.6576778610115588</v>
       </c>
       <c r="L15" t="n">
         <v>0.3112426035502959</v>
       </c>
       <c r="M15" t="n">
-        <v>0.7159763313609467</v>
+        <v>0.3610679494145611</v>
       </c>
       <c r="N15" t="n">
-        <v>0.6066690508655493</v>
+        <v>0.4325401688647393</v>
       </c>
       <c r="O15" t="n">
-        <v>0.3112426035502959</v>
+        <v>0.9394764562534392</v>
       </c>
       <c r="P15" t="n">
         <v>0.7159763313609467</v>
       </c>
       <c r="Q15" t="n">
+        <v>0.9739644970414201</v>
+      </c>
+      <c r="R15" t="n">
         <v>0.6066690508655493</v>
       </c>
-      <c r="R15" t="n">
+      <c r="S15" t="n">
+        <v>0.6576778610115588</v>
+      </c>
+      <c r="T15" t="n">
         <v>0.3112426035502959</v>
       </c>
-      <c r="S15" t="n">
+      <c r="U15" t="n">
+        <v>0.3610679494145611</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0.4325401688647393</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0.9394764562534392</v>
+      </c>
+      <c r="X15" t="n">
         <v>0.7159763313609467</v>
       </c>
-      <c r="T15" t="n">
+      <c r="Y15" t="n">
+        <v>0.9739644970414201</v>
+      </c>
+      <c r="Z15" t="n">
         <v>0.6066690508655493</v>
       </c>
-      <c r="U15" t="n">
+      <c r="AA15" t="n">
+        <v>0.6576778610115588</v>
+      </c>
+      <c r="AB15" t="n">
         <v>0.3112426035502959</v>
       </c>
-      <c r="V15" t="n">
+      <c r="AC15" t="n">
+        <v>0.3610679494145611</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>0.4325401688647393</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>0.9394764562534392</v>
+      </c>
+      <c r="AF15" t="n">
         <v>0.7159763313609467</v>
       </c>
-      <c r="W15" t="n">
+      <c r="AG15" t="n">
+        <v>0.9739644970414201</v>
+      </c>
+      <c r="AH15" t="n">
         <v>0.6066690508655493</v>
       </c>
-      <c r="X15" t="n">
+      <c r="AI15" t="n">
+        <v>0.6576778610115588</v>
+      </c>
+      <c r="AJ15" t="n">
         <v>0.3112426035502959</v>
       </c>
-      <c r="Y15" t="n">
+      <c r="AK15" t="n">
+        <v>0.3610679494145611</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>0.4325401688647393</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>0.9394764562534392</v>
+      </c>
+      <c r="AN15" t="n">
         <v>0.7159763313609467</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>0.9739644970414201</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>0.6066690508655493</v>
+      </c>
+      <c r="AQ15" t="n">
+        <v>0.6576778610115588</v>
+      </c>
+      <c r="AR15" t="n">
+        <v>0.3112426035502959</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>0.3610679494145611</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>0.4325401688647393</v>
+      </c>
+      <c r="AU15" t="n">
+        <v>0.9394764562534392</v>
+      </c>
+      <c r="AV15" t="n">
+        <v>0.7159763313609467</v>
+      </c>
+      <c r="AW15" t="n">
+        <v>0.9739644970414201</v>
+      </c>
+      <c r="AX15" t="n">
+        <v>0.6066690508655493</v>
+      </c>
+      <c r="AY15" t="n">
+        <v>0.6576778610115588</v>
+      </c>
+      <c r="AZ15" t="n">
+        <v>0.3112426035502959</v>
+      </c>
+      <c r="BA15" t="n">
+        <v>0.3610679494145611</v>
+      </c>
+      <c r="BB15" t="n">
+        <v>0.4325401688647393</v>
+      </c>
+      <c r="BC15" t="n">
+        <v>0.9394764562534392</v>
+      </c>
+      <c r="BD15" t="n">
+        <v>0.7159763313609467</v>
+      </c>
+      <c r="BE15" t="n">
+        <v>0.9739644970414201</v>
+      </c>
+      <c r="BF15" t="n">
+        <v>0.6066690508655493</v>
+      </c>
+      <c r="BG15" t="n">
+        <v>0.6576778610115588</v>
+      </c>
+      <c r="BH15" t="n">
+        <v>0.3112426035502959</v>
+      </c>
+      <c r="BI15" t="n">
+        <v>0.3610679494145611</v>
+      </c>
+      <c r="BJ15" t="n">
+        <v>0.4325401688647393</v>
+      </c>
+      <c r="BK15" t="n">
+        <v>0.9394764562534392</v>
+      </c>
+      <c r="BL15" t="n">
+        <v>0.7159763313609467</v>
+      </c>
+      <c r="BM15" t="n">
+        <v>0.9739644970414201</v>
       </c>
     </row>
     <row r="16">
@@ -1585,71 +3241,189 @@
         <v>0.6017725297110137</v>
       </c>
       <c r="C16" t="n">
+        <v>0.6883138174732198</v>
+      </c>
+      <c r="D16" t="n">
         <v>0.2035502958579882</v>
       </c>
-      <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
+        <v>0.3474697619873517</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.473775911324557</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.956943636506564</v>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="n">
         <v>0.6017725297110137</v>
       </c>
-      <c r="F16" t="n">
-        <v>0.2035502958579882</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.8319526627218935</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.6017725297110137</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0.2035502958579882</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0.8319526627218935</v>
-      </c>
       <c r="K16" t="n">
-        <v>0.6017725297110137</v>
+        <v>0.6883138174732198</v>
       </c>
       <c r="L16" t="n">
         <v>0.2035502958579882</v>
       </c>
       <c r="M16" t="n">
-        <v>0.8319526627218935</v>
+        <v>0.3474697619873517</v>
       </c>
       <c r="N16" t="n">
-        <v>0.6017725297110137</v>
+        <v>0.473775911324557</v>
       </c>
       <c r="O16" t="n">
-        <v>0.2035502958579882</v>
+        <v>0.956943636506564</v>
       </c>
       <c r="P16" t="n">
         <v>0.8319526627218935</v>
       </c>
       <c r="Q16" t="n">
+        <v>0.9751479289940829</v>
+      </c>
+      <c r="R16" t="n">
         <v>0.6017725297110137</v>
       </c>
-      <c r="R16" t="n">
+      <c r="S16" t="n">
+        <v>0.6883138174732198</v>
+      </c>
+      <c r="T16" t="n">
         <v>0.2035502958579882</v>
       </c>
-      <c r="S16" t="n">
+      <c r="U16" t="n">
+        <v>0.3474697619873517</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0.473775911324557</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0.956943636506564</v>
+      </c>
+      <c r="X16" t="n">
         <v>0.8319526627218935</v>
       </c>
-      <c r="T16" t="n">
+      <c r="Y16" t="n">
+        <v>0.9751479289940829</v>
+      </c>
+      <c r="Z16" t="n">
         <v>0.6017725297110137</v>
       </c>
-      <c r="U16" t="n">
+      <c r="AA16" t="n">
+        <v>0.6883138174732198</v>
+      </c>
+      <c r="AB16" t="n">
         <v>0.2035502958579882</v>
       </c>
-      <c r="V16" t="n">
+      <c r="AC16" t="n">
+        <v>0.3474697619873517</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>0.473775911324557</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>0.956943636506564</v>
+      </c>
+      <c r="AF16" t="n">
         <v>0.8319526627218935</v>
       </c>
-      <c r="W16" t="n">
+      <c r="AG16" t="n">
+        <v>0.9751479289940829</v>
+      </c>
+      <c r="AH16" t="n">
         <v>0.6017725297110137</v>
       </c>
-      <c r="X16" t="n">
+      <c r="AI16" t="n">
+        <v>0.6883138174732198</v>
+      </c>
+      <c r="AJ16" t="n">
         <v>0.2035502958579882</v>
       </c>
-      <c r="Y16" t="n">
+      <c r="AK16" t="n">
+        <v>0.3474697619873517</v>
+      </c>
+      <c r="AL16" t="n">
+        <v>0.473775911324557</v>
+      </c>
+      <c r="AM16" t="n">
+        <v>0.956943636506564</v>
+      </c>
+      <c r="AN16" t="n">
         <v>0.8319526627218935</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>0.9751479289940829</v>
+      </c>
+      <c r="AP16" t="n">
+        <v>0.6017725297110137</v>
+      </c>
+      <c r="AQ16" t="n">
+        <v>0.6883138174732198</v>
+      </c>
+      <c r="AR16" t="n">
+        <v>0.2035502958579882</v>
+      </c>
+      <c r="AS16" t="n">
+        <v>0.3474697619873517</v>
+      </c>
+      <c r="AT16" t="n">
+        <v>0.473775911324557</v>
+      </c>
+      <c r="AU16" t="n">
+        <v>0.956943636506564</v>
+      </c>
+      <c r="AV16" t="n">
+        <v>0.8319526627218935</v>
+      </c>
+      <c r="AW16" t="n">
+        <v>0.9751479289940829</v>
+      </c>
+      <c r="AX16" t="n">
+        <v>0.6017725297110137</v>
+      </c>
+      <c r="AY16" t="n">
+        <v>0.6883138174732198</v>
+      </c>
+      <c r="AZ16" t="n">
+        <v>0.2035502958579882</v>
+      </c>
+      <c r="BA16" t="n">
+        <v>0.3474697619873517</v>
+      </c>
+      <c r="BB16" t="n">
+        <v>0.473775911324557</v>
+      </c>
+      <c r="BC16" t="n">
+        <v>0.956943636506564</v>
+      </c>
+      <c r="BD16" t="n">
+        <v>0.8319526627218935</v>
+      </c>
+      <c r="BE16" t="n">
+        <v>0.9751479289940829</v>
+      </c>
+      <c r="BF16" t="n">
+        <v>0.6017725297110137</v>
+      </c>
+      <c r="BG16" t="n">
+        <v>0.6883138174732198</v>
+      </c>
+      <c r="BH16" t="n">
+        <v>0.2035502958579882</v>
+      </c>
+      <c r="BI16" t="n">
+        <v>0.3474697619873517</v>
+      </c>
+      <c r="BJ16" t="n">
+        <v>0.473775911324557</v>
+      </c>
+      <c r="BK16" t="n">
+        <v>0.956943636506564</v>
+      </c>
+      <c r="BL16" t="n">
+        <v>0.8319526627218935</v>
+      </c>
+      <c r="BM16" t="n">
+        <v>0.9751479289940829</v>
       </c>
     </row>
     <row r="17">
@@ -1662,71 +3436,189 @@
         <v>0.5938541250959626</v>
       </c>
       <c r="C17" t="n">
+        <v>0.661357302381815</v>
+      </c>
+      <c r="D17" t="n">
         <v>0.2958579881656805</v>
       </c>
-      <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
+        <v>0.3663589015892664</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.4373934814137515</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.9435893404606556</v>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="n">
         <v>0.5938541250959626</v>
       </c>
-      <c r="F17" t="n">
-        <v>0.2958579881656805</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.7301775147928994</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.5938541250959626</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.2958579881656805</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0.7301775147928994</v>
-      </c>
       <c r="K17" t="n">
-        <v>0.5938541250959626</v>
+        <v>0.661357302381815</v>
       </c>
       <c r="L17" t="n">
         <v>0.2958579881656805</v>
       </c>
       <c r="M17" t="n">
-        <v>0.7301775147928994</v>
+        <v>0.3663589015892664</v>
       </c>
       <c r="N17" t="n">
-        <v>0.5938541250959626</v>
+        <v>0.4373934814137515</v>
       </c>
       <c r="O17" t="n">
-        <v>0.2958579881656805</v>
+        <v>0.9435893404606556</v>
       </c>
       <c r="P17" t="n">
         <v>0.7301775147928994</v>
       </c>
       <c r="Q17" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="R17" t="n">
         <v>0.5938541250959626</v>
       </c>
-      <c r="R17" t="n">
+      <c r="S17" t="n">
+        <v>0.661357302381815</v>
+      </c>
+      <c r="T17" t="n">
         <v>0.2958579881656805</v>
       </c>
-      <c r="S17" t="n">
+      <c r="U17" t="n">
+        <v>0.3663589015892664</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.4373934814137515</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0.9435893404606556</v>
+      </c>
+      <c r="X17" t="n">
         <v>0.7301775147928994</v>
       </c>
-      <c r="T17" t="n">
+      <c r="Y17" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="Z17" t="n">
         <v>0.5938541250959626</v>
       </c>
-      <c r="U17" t="n">
+      <c r="AA17" t="n">
+        <v>0.661357302381815</v>
+      </c>
+      <c r="AB17" t="n">
         <v>0.2958579881656805</v>
       </c>
-      <c r="V17" t="n">
+      <c r="AC17" t="n">
+        <v>0.3663589015892664</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>0.4373934814137515</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>0.9435893404606556</v>
+      </c>
+      <c r="AF17" t="n">
         <v>0.7301775147928994</v>
       </c>
-      <c r="W17" t="n">
+      <c r="AG17" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="AH17" t="n">
         <v>0.5938541250959626</v>
       </c>
-      <c r="X17" t="n">
+      <c r="AI17" t="n">
+        <v>0.661357302381815</v>
+      </c>
+      <c r="AJ17" t="n">
         <v>0.2958579881656805</v>
       </c>
-      <c r="Y17" t="n">
+      <c r="AK17" t="n">
+        <v>0.3663589015892664</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>0.4373934814137515</v>
+      </c>
+      <c r="AM17" t="n">
+        <v>0.9435893404606556</v>
+      </c>
+      <c r="AN17" t="n">
         <v>0.7301775147928994</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="AP17" t="n">
+        <v>0.5938541250959626</v>
+      </c>
+      <c r="AQ17" t="n">
+        <v>0.661357302381815</v>
+      </c>
+      <c r="AR17" t="n">
+        <v>0.2958579881656805</v>
+      </c>
+      <c r="AS17" t="n">
+        <v>0.3663589015892664</v>
+      </c>
+      <c r="AT17" t="n">
+        <v>0.4373934814137515</v>
+      </c>
+      <c r="AU17" t="n">
+        <v>0.9435893404606556</v>
+      </c>
+      <c r="AV17" t="n">
+        <v>0.7301775147928994</v>
+      </c>
+      <c r="AW17" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="AX17" t="n">
+        <v>0.5938541250959626</v>
+      </c>
+      <c r="AY17" t="n">
+        <v>0.661357302381815</v>
+      </c>
+      <c r="AZ17" t="n">
+        <v>0.2958579881656805</v>
+      </c>
+      <c r="BA17" t="n">
+        <v>0.3663589015892664</v>
+      </c>
+      <c r="BB17" t="n">
+        <v>0.4373934814137515</v>
+      </c>
+      <c r="BC17" t="n">
+        <v>0.9435893404606556</v>
+      </c>
+      <c r="BD17" t="n">
+        <v>0.7301775147928994</v>
+      </c>
+      <c r="BE17" t="n">
+        <v>0.9763313609467456</v>
+      </c>
+      <c r="BF17" t="n">
+        <v>0.5938541250959626</v>
+      </c>
+      <c r="BG17" t="n">
+        <v>0.661357302381815</v>
+      </c>
+      <c r="BH17" t="n">
+        <v>0.2958579881656805</v>
+      </c>
+      <c r="BI17" t="n">
+        <v>0.3663589015892664</v>
+      </c>
+      <c r="BJ17" t="n">
+        <v>0.4373934814137515</v>
+      </c>
+      <c r="BK17" t="n">
+        <v>0.9435893404606556</v>
+      </c>
+      <c r="BL17" t="n">
+        <v>0.7301775147928994</v>
+      </c>
+      <c r="BM17" t="n">
+        <v>0.9763313609467456</v>
       </c>
     </row>
     <row r="18">
@@ -1739,71 +3631,189 @@
         <v>0.6095880848048908</v>
       </c>
       <c r="C18" t="n">
+        <v>0.6608846749711658</v>
+      </c>
+      <c r="D18" t="n">
         <v>0.3005917159763314</v>
       </c>
-      <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
+        <v>0.3648799752862116</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.4367685536117434</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.9400267274585331</v>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="n">
         <v>0.6095880848048908</v>
       </c>
-      <c r="F18" t="n">
-        <v>0.3005917159763314</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.7325443786982249</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.6095880848048908</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0.3005917159763314</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.7325443786982249</v>
-      </c>
       <c r="K18" t="n">
-        <v>0.6095880848048908</v>
+        <v>0.6608846749711658</v>
       </c>
       <c r="L18" t="n">
         <v>0.3005917159763314</v>
       </c>
       <c r="M18" t="n">
-        <v>0.7325443786982249</v>
+        <v>0.3648799752862116</v>
       </c>
       <c r="N18" t="n">
-        <v>0.6095880848048908</v>
+        <v>0.4367685536117434</v>
       </c>
       <c r="O18" t="n">
-        <v>0.3005917159763314</v>
+        <v>0.9400267274585331</v>
       </c>
       <c r="P18" t="n">
         <v>0.7325443786982249</v>
       </c>
       <c r="Q18" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="R18" t="n">
         <v>0.6095880848048908</v>
       </c>
-      <c r="R18" t="n">
+      <c r="S18" t="n">
+        <v>0.6608846749711658</v>
+      </c>
+      <c r="T18" t="n">
         <v>0.3005917159763314</v>
       </c>
-      <c r="S18" t="n">
+      <c r="U18" t="n">
+        <v>0.3648799752862116</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0.4367685536117434</v>
+      </c>
+      <c r="W18" t="n">
+        <v>0.9400267274585331</v>
+      </c>
+      <c r="X18" t="n">
         <v>0.7325443786982249</v>
       </c>
-      <c r="T18" t="n">
+      <c r="Y18" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="Z18" t="n">
         <v>0.6095880848048908</v>
       </c>
-      <c r="U18" t="n">
+      <c r="AA18" t="n">
+        <v>0.6608846749711658</v>
+      </c>
+      <c r="AB18" t="n">
         <v>0.3005917159763314</v>
       </c>
-      <c r="V18" t="n">
+      <c r="AC18" t="n">
+        <v>0.3648799752862116</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>0.4367685536117434</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>0.9400267274585331</v>
+      </c>
+      <c r="AF18" t="n">
         <v>0.7325443786982249</v>
       </c>
-      <c r="W18" t="n">
+      <c r="AG18" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="AH18" t="n">
         <v>0.6095880848048908</v>
       </c>
-      <c r="X18" t="n">
+      <c r="AI18" t="n">
+        <v>0.6608846749711658</v>
+      </c>
+      <c r="AJ18" t="n">
         <v>0.3005917159763314</v>
       </c>
-      <c r="Y18" t="n">
+      <c r="AK18" t="n">
+        <v>0.3648799752862116</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>0.4367685536117434</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>0.9400267274585331</v>
+      </c>
+      <c r="AN18" t="n">
         <v>0.7325443786982249</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="AP18" t="n">
+        <v>0.6095880848048908</v>
+      </c>
+      <c r="AQ18" t="n">
+        <v>0.6608846749711658</v>
+      </c>
+      <c r="AR18" t="n">
+        <v>0.3005917159763314</v>
+      </c>
+      <c r="AS18" t="n">
+        <v>0.3648799752862116</v>
+      </c>
+      <c r="AT18" t="n">
+        <v>0.4367685536117434</v>
+      </c>
+      <c r="AU18" t="n">
+        <v>0.9400267274585331</v>
+      </c>
+      <c r="AV18" t="n">
+        <v>0.7325443786982249</v>
+      </c>
+      <c r="AW18" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="AX18" t="n">
+        <v>0.6095880848048908</v>
+      </c>
+      <c r="AY18" t="n">
+        <v>0.6608846749711658</v>
+      </c>
+      <c r="AZ18" t="n">
+        <v>0.3005917159763314</v>
+      </c>
+      <c r="BA18" t="n">
+        <v>0.3648799752862116</v>
+      </c>
+      <c r="BB18" t="n">
+        <v>0.4367685536117434</v>
+      </c>
+      <c r="BC18" t="n">
+        <v>0.9400267274585331</v>
+      </c>
+      <c r="BD18" t="n">
+        <v>0.7325443786982249</v>
+      </c>
+      <c r="BE18" t="n">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="BF18" t="n">
+        <v>0.6095880848048908</v>
+      </c>
+      <c r="BG18" t="n">
+        <v>0.6608846749711658</v>
+      </c>
+      <c r="BH18" t="n">
+        <v>0.3005917159763314</v>
+      </c>
+      <c r="BI18" t="n">
+        <v>0.3648799752862116</v>
+      </c>
+      <c r="BJ18" t="n">
+        <v>0.4367685536117434</v>
+      </c>
+      <c r="BK18" t="n">
+        <v>0.9400267274585331</v>
+      </c>
+      <c r="BL18" t="n">
+        <v>0.7325443786982249</v>
+      </c>
+      <c r="BM18" t="n">
+        <v>0.9692307692307692</v>
       </c>
     </row>
     <row r="19">
@@ -1816,71 +3826,189 @@
         <v>0.6027550161279918</v>
       </c>
       <c r="C19" t="n">
+        <v>0.6919515956109662</v>
+      </c>
+      <c r="D19" t="n">
         <v>0.2</v>
       </c>
-      <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
+        <v>0.3505817859045826</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.4787970106685621</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.9571040012577627</v>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="n">
         <v>0.6027550161279918</v>
       </c>
-      <c r="F19" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.8378698224852071</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.6027550161279918</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0.8378698224852071</v>
-      </c>
       <c r="K19" t="n">
-        <v>0.6027550161279918</v>
+        <v>0.6919515956109662</v>
       </c>
       <c r="L19" t="n">
         <v>0.2</v>
       </c>
       <c r="M19" t="n">
-        <v>0.8378698224852071</v>
+        <v>0.3505817859045826</v>
       </c>
       <c r="N19" t="n">
-        <v>0.6027550161279918</v>
+        <v>0.4787970106685621</v>
       </c>
       <c r="O19" t="n">
-        <v>0.2</v>
+        <v>0.9571040012577627</v>
       </c>
       <c r="P19" t="n">
         <v>0.8378698224852071</v>
       </c>
       <c r="Q19" t="n">
+        <v>0.9727810650887574</v>
+      </c>
+      <c r="R19" t="n">
         <v>0.6027550161279918</v>
       </c>
-      <c r="R19" t="n">
+      <c r="S19" t="n">
+        <v>0.6919515956109662</v>
+      </c>
+      <c r="T19" t="n">
         <v>0.2</v>
       </c>
-      <c r="S19" t="n">
+      <c r="U19" t="n">
+        <v>0.3505817859045826</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0.4787970106685621</v>
+      </c>
+      <c r="W19" t="n">
+        <v>0.9571040012577627</v>
+      </c>
+      <c r="X19" t="n">
         <v>0.8378698224852071</v>
       </c>
-      <c r="T19" t="n">
+      <c r="Y19" t="n">
+        <v>0.9727810650887574</v>
+      </c>
+      <c r="Z19" t="n">
         <v>0.6027550161279918</v>
       </c>
-      <c r="U19" t="n">
+      <c r="AA19" t="n">
+        <v>0.6919515956109662</v>
+      </c>
+      <c r="AB19" t="n">
         <v>0.2</v>
       </c>
-      <c r="V19" t="n">
+      <c r="AC19" t="n">
+        <v>0.3505817859045826</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>0.4787970106685621</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>0.9571040012577627</v>
+      </c>
+      <c r="AF19" t="n">
         <v>0.8378698224852071</v>
       </c>
-      <c r="W19" t="n">
+      <c r="AG19" t="n">
+        <v>0.9727810650887574</v>
+      </c>
+      <c r="AH19" t="n">
         <v>0.6027550161279918</v>
       </c>
-      <c r="X19" t="n">
+      <c r="AI19" t="n">
+        <v>0.6919515956109662</v>
+      </c>
+      <c r="AJ19" t="n">
         <v>0.2</v>
       </c>
-      <c r="Y19" t="n">
+      <c r="AK19" t="n">
+        <v>0.3505817859045826</v>
+      </c>
+      <c r="AL19" t="n">
+        <v>0.4787970106685621</v>
+      </c>
+      <c r="AM19" t="n">
+        <v>0.9571040012577627</v>
+      </c>
+      <c r="AN19" t="n">
         <v>0.8378698224852071</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>0.9727810650887574</v>
+      </c>
+      <c r="AP19" t="n">
+        <v>0.6027550161279918</v>
+      </c>
+      <c r="AQ19" t="n">
+        <v>0.6919515956109662</v>
+      </c>
+      <c r="AR19" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AS19" t="n">
+        <v>0.3505817859045826</v>
+      </c>
+      <c r="AT19" t="n">
+        <v>0.4787970106685621</v>
+      </c>
+      <c r="AU19" t="n">
+        <v>0.9571040012577627</v>
+      </c>
+      <c r="AV19" t="n">
+        <v>0.8378698224852071</v>
+      </c>
+      <c r="AW19" t="n">
+        <v>0.9727810650887574</v>
+      </c>
+      <c r="AX19" t="n">
+        <v>0.6027550161279918</v>
+      </c>
+      <c r="AY19" t="n">
+        <v>0.6919515956109662</v>
+      </c>
+      <c r="AZ19" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BA19" t="n">
+        <v>0.3505817859045826</v>
+      </c>
+      <c r="BB19" t="n">
+        <v>0.4787970106685621</v>
+      </c>
+      <c r="BC19" t="n">
+        <v>0.9571040012577627</v>
+      </c>
+      <c r="BD19" t="n">
+        <v>0.8378698224852071</v>
+      </c>
+      <c r="BE19" t="n">
+        <v>0.9727810650887574</v>
+      </c>
+      <c r="BF19" t="n">
+        <v>0.6027550161279918</v>
+      </c>
+      <c r="BG19" t="n">
+        <v>0.6919515956109662</v>
+      </c>
+      <c r="BH19" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BI19" t="n">
+        <v>0.3505817859045826</v>
+      </c>
+      <c r="BJ19" t="n">
+        <v>0.4787970106685621</v>
+      </c>
+      <c r="BK19" t="n">
+        <v>0.9571040012577627</v>
+      </c>
+      <c r="BL19" t="n">
+        <v>0.8378698224852071</v>
+      </c>
+      <c r="BM19" t="n">
+        <v>0.9727810650887574</v>
       </c>
     </row>
     <row r="20">
@@ -1893,71 +4021,189 @@
         <v>0.5317553841367666</v>
       </c>
       <c r="C20" t="n">
+        <v>0.6138490378095712</v>
+      </c>
+      <c r="D20" t="n">
         <v>0.3882510321476291</v>
       </c>
-      <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
+        <v>0.4121357438145184</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.3768106412197364</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.9684710321515604</v>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="n">
         <v>0.565266863719195</v>
       </c>
-      <c r="F20" t="n">
+      <c r="K20" t="n">
+        <v>0.6786384329859394</v>
+      </c>
+      <c r="L20" t="n">
         <v>0.2840236686390533</v>
       </c>
-      <c r="G20" t="n">
+      <c r="M20" t="n">
+        <v>0.3737183070107226</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.4605501227256114</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.9476236144957157</v>
+      </c>
+      <c r="P20" t="n">
         <v>0.7325443786982249</v>
       </c>
-      <c r="H20" t="n">
+      <c r="Q20" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="R20" t="n">
         <v>0.565266863719195</v>
       </c>
-      <c r="I20" t="n">
+      <c r="S20" t="n">
+        <v>0.6786384329859394</v>
+      </c>
+      <c r="T20" t="n">
         <v>0.2840236686390533</v>
       </c>
-      <c r="J20" t="n">
+      <c r="U20" t="n">
+        <v>0.3737183070107226</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0.4605501227256114</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0.9476236144957157</v>
+      </c>
+      <c r="X20" t="n">
         <v>0.7325443786982249</v>
       </c>
-      <c r="K20" t="n">
+      <c r="Y20" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="Z20" t="n">
         <v>0.5704768066996664</v>
       </c>
-      <c r="L20" t="n">
+      <c r="AA20" t="n">
+        <v>0.685260114959152</v>
+      </c>
+      <c r="AB20" t="n">
         <v>0.285207100591716</v>
       </c>
-      <c r="M20" t="n">
+      <c r="AC20" t="n">
+        <v>0.380279334372393</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>0.4695814251538302</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>0.9411807247857873</v>
+      </c>
+      <c r="AF20" t="n">
         <v>0.7337278106508875</v>
       </c>
-      <c r="N20" t="n">
+      <c r="AG20" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="AH20" t="n">
         <v>0.5589508346026139</v>
       </c>
-      <c r="O20" t="n">
+      <c r="AI20" t="n">
+        <v>0.6835609480856952</v>
+      </c>
+      <c r="AJ20" t="n">
         <v>0.272189349112426</v>
       </c>
-      <c r="P20" t="n">
+      <c r="AK20" t="n">
+        <v>0.3784105788023592</v>
+      </c>
+      <c r="AL20" t="n">
+        <v>0.4672555697478145</v>
+      </c>
+      <c r="AM20" t="n">
+        <v>0.9435264523229306</v>
+      </c>
+      <c r="AN20" t="n">
         <v>0.7467455621301775</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="AO20" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="AP20" t="n">
         <v>0.565266863719195</v>
       </c>
-      <c r="R20" t="n">
+      <c r="AQ20" t="n">
+        <v>0.6786384329859394</v>
+      </c>
+      <c r="AR20" t="n">
         <v>0.2840236686390533</v>
       </c>
-      <c r="S20" t="n">
+      <c r="AS20" t="n">
+        <v>0.3737183070107226</v>
+      </c>
+      <c r="AT20" t="n">
+        <v>0.4605501227256114</v>
+      </c>
+      <c r="AU20" t="n">
+        <v>0.9476236144957157</v>
+      </c>
+      <c r="AV20" t="n">
         <v>0.7325443786982249</v>
       </c>
-      <c r="T20" t="n">
+      <c r="AW20" t="n">
+        <v>0.9846153846153847</v>
+      </c>
+      <c r="AX20" t="n">
         <v>0.5600084530215783</v>
       </c>
-      <c r="U20" t="n">
+      <c r="AY20" t="n">
+        <v>0.6712728627684483</v>
+      </c>
+      <c r="AZ20" t="n">
         <v>0.2733727810650888</v>
       </c>
-      <c r="V20" t="n">
+      <c r="BA20" t="n">
+        <v>0.3617622653438928</v>
+      </c>
+      <c r="BB20" t="n">
+        <v>0.4506072562893481</v>
+      </c>
+      <c r="BC20" t="n">
+        <v>0.9463752849618741</v>
+      </c>
+      <c r="BD20" t="n">
         <v>0.7455621301775148</v>
       </c>
-      <c r="W20" t="n">
+      <c r="BE20" t="n">
+        <v>0.9822485207100592</v>
+      </c>
+      <c r="BF20" t="n">
         <v>0.5642191021813</v>
       </c>
-      <c r="X20" t="n">
+      <c r="BG20" t="n">
+        <v>0.6839050472811407</v>
+      </c>
+      <c r="BH20" t="n">
         <v>0.2781065088757396</v>
       </c>
-      <c r="Y20" t="n">
+      <c r="BI20" t="n">
+        <v>0.378881122751164</v>
+      </c>
+      <c r="BJ20" t="n">
+        <v>0.4677261136966193</v>
+      </c>
+      <c r="BK20" t="n">
+        <v>0.9432088672274193</v>
+      </c>
+      <c r="BL20" t="n">
         <v>0.7408284023668639</v>
+      </c>
+      <c r="BM20" t="n">
+        <v>0.9822485207100592</v>
       </c>
     </row>
     <row r="21">
@@ -1967,74 +4213,192 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.5417482111279694</v>
+        <v>0.5621177201983111</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2414201183431953</v>
-      </c>
-      <c r="D21" t="inlineStr"/>
+        <v>0.6535159627964467</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.2662721893491125</v>
+      </c>
       <c r="E21" t="n">
-        <v>0.5417482111279694</v>
+        <v>0.3586532500000599</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2414201183431953</v>
+        <v>0.4270831136297668</v>
       </c>
       <c r="G21" t="n">
-        <v>0.7834319526627219</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.5417482111279694</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0.2414201183431953</v>
-      </c>
+        <v>0.9489379765741687</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="n">
-        <v>0.7834319526627219</v>
+        <v>0.5621177201983111</v>
       </c>
       <c r="K21" t="n">
-        <v>0.5417482111279694</v>
+        <v>0.6535159627964467</v>
       </c>
       <c r="L21" t="n">
-        <v>0.2414201183431953</v>
+        <v>0.2662721893491125</v>
       </c>
       <c r="M21" t="n">
-        <v>0.7834319526627219</v>
+        <v>0.3586532500000599</v>
       </c>
       <c r="N21" t="n">
-        <v>0.5417482111279694</v>
+        <v>0.4270831136297668</v>
       </c>
       <c r="O21" t="n">
-        <v>0.2414201183431953</v>
+        <v>0.9489379765741687</v>
       </c>
       <c r="P21" t="n">
-        <v>0.7834319526627219</v>
+        <v>0.757396449704142</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.5417482111279694</v>
+        <v>0.9775147928994082</v>
       </c>
       <c r="R21" t="n">
-        <v>0.2414201183431953</v>
+        <v>0.5621177201983111</v>
       </c>
       <c r="S21" t="n">
-        <v>0.7834319526627219</v>
+        <v>0.6535159627964467</v>
       </c>
       <c r="T21" t="n">
-        <v>0.5417482111279694</v>
+        <v>0.2662721893491125</v>
       </c>
       <c r="U21" t="n">
-        <v>0.2414201183431953</v>
+        <v>0.3586532500000599</v>
       </c>
       <c r="V21" t="n">
-        <v>0.7834319526627219</v>
+        <v>0.4270831136297668</v>
       </c>
       <c r="W21" t="n">
-        <v>0.5417482111279694</v>
+        <v>0.9489379765741687</v>
       </c>
       <c r="X21" t="n">
-        <v>0.2414201183431953</v>
+        <v>0.757396449704142</v>
       </c>
       <c r="Y21" t="n">
-        <v>0.7834319526627219</v>
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0.5621177201983111</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>0.6535159627964467</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>0.2662721893491125</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>0.3586532500000599</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>0.4270831136297668</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>0.9489379765741687</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>0.757396449704142</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>0.5621177201983111</v>
+      </c>
+      <c r="AI21" t="n">
+        <v>0.6535159627964467</v>
+      </c>
+      <c r="AJ21" t="n">
+        <v>0.2662721893491125</v>
+      </c>
+      <c r="AK21" t="n">
+        <v>0.3586532500000599</v>
+      </c>
+      <c r="AL21" t="n">
+        <v>0.4270831136297668</v>
+      </c>
+      <c r="AM21" t="n">
+        <v>0.9489379765741687</v>
+      </c>
+      <c r="AN21" t="n">
+        <v>0.757396449704142</v>
+      </c>
+      <c r="AO21" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="AP21" t="n">
+        <v>0.5621177201983111</v>
+      </c>
+      <c r="AQ21" t="n">
+        <v>0.6535159627964467</v>
+      </c>
+      <c r="AR21" t="n">
+        <v>0.2662721893491125</v>
+      </c>
+      <c r="AS21" t="n">
+        <v>0.3586532500000599</v>
+      </c>
+      <c r="AT21" t="n">
+        <v>0.4270831136297668</v>
+      </c>
+      <c r="AU21" t="n">
+        <v>0.9489379765741687</v>
+      </c>
+      <c r="AV21" t="n">
+        <v>0.757396449704142</v>
+      </c>
+      <c r="AW21" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="AX21" t="n">
+        <v>0.5621177201983111</v>
+      </c>
+      <c r="AY21" t="n">
+        <v>0.6535159627964467</v>
+      </c>
+      <c r="AZ21" t="n">
+        <v>0.2662721893491125</v>
+      </c>
+      <c r="BA21" t="n">
+        <v>0.3586532500000599</v>
+      </c>
+      <c r="BB21" t="n">
+        <v>0.4270831136297668</v>
+      </c>
+      <c r="BC21" t="n">
+        <v>0.9489379765741687</v>
+      </c>
+      <c r="BD21" t="n">
+        <v>0.757396449704142</v>
+      </c>
+      <c r="BE21" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="BF21" t="n">
+        <v>0.5621177201983111</v>
+      </c>
+      <c r="BG21" t="n">
+        <v>0.6535159627964467</v>
+      </c>
+      <c r="BH21" t="n">
+        <v>0.2662721893491125</v>
+      </c>
+      <c r="BI21" t="n">
+        <v>0.3586532500000599</v>
+      </c>
+      <c r="BJ21" t="n">
+        <v>0.4270831136297668</v>
+      </c>
+      <c r="BK21" t="n">
+        <v>0.9489379765741687</v>
+      </c>
+      <c r="BL21" t="n">
+        <v>0.757396449704142</v>
+      </c>
+      <c r="BM21" t="n">
+        <v>0.9775147928994082</v>
       </c>
     </row>
     <row r="22">
@@ -2044,86 +4408,204 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.5307134864818566</v>
+        <v>0.6305815855975138</v>
       </c>
       <c r="C22" t="n">
-        <v>0.2248520710059172</v>
-      </c>
-      <c r="D22" t="inlineStr"/>
+        <v>0.6276893301377549</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.3431952662721893</v>
+      </c>
       <c r="E22" t="n">
-        <v>0.5318272620751878</v>
+        <v>0.3576477345855125</v>
       </c>
       <c r="F22" t="n">
-        <v>0.2260355029585799</v>
+        <v>0.3939938951687834</v>
       </c>
       <c r="G22" t="n">
-        <v>0.7988165680473372</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0.5318272620751878</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0.2260355029585799</v>
-      </c>
+        <v>0.9381432277336688</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="n">
-        <v>0.7988165680473372</v>
+        <v>0.6305815855975138</v>
       </c>
       <c r="K22" t="n">
-        <v>0.5318272620751878</v>
+        <v>0.6276893301377549</v>
       </c>
       <c r="L22" t="n">
-        <v>0.2260355029585799</v>
+        <v>0.3431952662721893</v>
       </c>
       <c r="M22" t="n">
-        <v>0.7988165680473372</v>
+        <v>0.3576477345855125</v>
       </c>
       <c r="N22" t="n">
-        <v>0.5318272620751878</v>
+        <v>0.3939938951687834</v>
       </c>
       <c r="O22" t="n">
-        <v>0.2260355029585799</v>
+        <v>0.9381432277336688</v>
       </c>
       <c r="P22" t="n">
-        <v>0.7988165680473372</v>
+        <v>0.6816568047337278</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.5318272620751878</v>
+        <v>0.9775147928994082</v>
       </c>
       <c r="R22" t="n">
-        <v>0.2260355029585799</v>
+        <v>0.6305815855975138</v>
       </c>
       <c r="S22" t="n">
-        <v>0.7988165680473372</v>
+        <v>0.6276893301377549</v>
       </c>
       <c r="T22" t="n">
-        <v>0.5318272620751878</v>
+        <v>0.3431952662721893</v>
       </c>
       <c r="U22" t="n">
-        <v>0.2260355029585799</v>
+        <v>0.3576477345855125</v>
       </c>
       <c r="V22" t="n">
-        <v>0.7988165680473372</v>
+        <v>0.3939938951687834</v>
       </c>
       <c r="W22" t="n">
-        <v>0.5318272620751878</v>
+        <v>0.9381432277336688</v>
       </c>
       <c r="X22" t="n">
-        <v>0.2260355029585799</v>
+        <v>0.6816568047337278</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.7988165680473372</v>
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>0.6305815855975138</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>0.6276893301377549</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>0.3431952662721893</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>0.3576477345855125</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>0.3939938951687834</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>0.9381432277336688</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>0.6816568047337278</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>0.6305815855975138</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>0.6276893301377549</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>0.3431952662721893</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>0.3576477345855125</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>0.3939938951687834</v>
+      </c>
+      <c r="AM22" t="n">
+        <v>0.9381432277336688</v>
+      </c>
+      <c r="AN22" t="n">
+        <v>0.6816568047337278</v>
+      </c>
+      <c r="AO22" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="AP22" t="n">
+        <v>0.6305815855975138</v>
+      </c>
+      <c r="AQ22" t="n">
+        <v>0.6276893301377549</v>
+      </c>
+      <c r="AR22" t="n">
+        <v>0.3431952662721893</v>
+      </c>
+      <c r="AS22" t="n">
+        <v>0.3576477345855125</v>
+      </c>
+      <c r="AT22" t="n">
+        <v>0.3939938951687834</v>
+      </c>
+      <c r="AU22" t="n">
+        <v>0.9381432277336688</v>
+      </c>
+      <c r="AV22" t="n">
+        <v>0.6816568047337278</v>
+      </c>
+      <c r="AW22" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="AX22" t="n">
+        <v>0.6305815855975138</v>
+      </c>
+      <c r="AY22" t="n">
+        <v>0.6276893301377549</v>
+      </c>
+      <c r="AZ22" t="n">
+        <v>0.3431952662721893</v>
+      </c>
+      <c r="BA22" t="n">
+        <v>0.3576477345855125</v>
+      </c>
+      <c r="BB22" t="n">
+        <v>0.3939938951687834</v>
+      </c>
+      <c r="BC22" t="n">
+        <v>0.9381432277336688</v>
+      </c>
+      <c r="BD22" t="n">
+        <v>0.6816568047337278</v>
+      </c>
+      <c r="BE22" t="n">
+        <v>0.9775147928994082</v>
+      </c>
+      <c r="BF22" t="n">
+        <v>0.6305815855975138</v>
+      </c>
+      <c r="BG22" t="n">
+        <v>0.6276893301377549</v>
+      </c>
+      <c r="BH22" t="n">
+        <v>0.3431952662721893</v>
+      </c>
+      <c r="BI22" t="n">
+        <v>0.3576477345855125</v>
+      </c>
+      <c r="BJ22" t="n">
+        <v>0.3939938951687834</v>
+      </c>
+      <c r="BK22" t="n">
+        <v>0.9381432277336688</v>
+      </c>
+      <c r="BL22" t="n">
+        <v>0.6816568047337278</v>
+      </c>
+      <c r="BM22" t="n">
+        <v>0.9775147928994082</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="AP1:AW1"/>
+    <mergeCell ref="R1:Y1"/>
+    <mergeCell ref="Z1:AG1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="AX1:BE1"/>
+    <mergeCell ref="AH1:AO1"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="BF1:BM1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>